<commit_message>
changed to glorot normal initialiser in GRU
</commit_message>
<xml_diff>
--- a/Logging/Tools/Results_Summary.xlsx
+++ b/Logging/Tools/Results_Summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/github/Forecasting/Logging/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/github/Forecasting/Logging/Tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65618F00-2F06-924F-BF5F-41538F8CD2F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26B4F0B-D0D6-DB4D-8853-B688776854AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" activeTab="1" xr2:uid="{D6C4A1CF-C8B6-1A42-B202-9397802E1C24}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="23">
   <si>
     <t>2014/15</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>28 Day Lag</t>
+  </si>
+  <si>
+    <t>ADD STDDEV</t>
+  </si>
+  <si>
+    <t>3yrs weighted avg, patience around 20</t>
+  </si>
+  <si>
+    <t>Add normal distribition centred to 0 for weights</t>
   </si>
 </sst>
 </file>
@@ -402,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -464,51 +473,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -532,6 +496,52 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4038,32 +4048,32 @@
   <cols>
     <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="12" width="7.83203125" customWidth="1"/>
-    <col min="13" max="13" width="7.83203125" style="74" customWidth="1"/>
+    <col min="13" max="13" width="7.83203125" style="59" customWidth="1"/>
     <col min="14" max="18" width="7.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="55" t="s">
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="55" t="s">
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="57"/>
+      <c r="O1" s="75"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="76"/>
     </row>
     <row r="2" spans="2:19" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
@@ -4094,7 +4104,7 @@
       <c r="L2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="70" t="s">
+      <c r="M2" s="55" t="s">
         <v>11</v>
       </c>
       <c r="N2" s="13" t="s">
@@ -4114,7 +4124,7 @@
       </c>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="77" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -4148,7 +4158,7 @@
       <c r="L3" s="5">
         <v>3.43553758963114</v>
       </c>
-      <c r="M3" s="71">
+      <c r="M3" s="56">
         <f t="shared" ref="M3:M5" si="1">AVERAGE(I3:L3)</f>
         <v>2.38648426568732</v>
       </c>
@@ -4174,7 +4184,7 @@
       </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B4" s="59"/>
+      <c r="B4" s="78"/>
       <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
@@ -4206,7 +4216,7 @@
       <c r="L4" s="8">
         <v>5.0925985304313803</v>
       </c>
-      <c r="M4" s="72">
+      <c r="M4" s="57">
         <f t="shared" si="1"/>
         <v>3.4291134192345627</v>
       </c>
@@ -4232,7 +4242,7 @@
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B5" s="60"/>
+      <c r="B5" s="79"/>
       <c r="C5" s="9" t="s">
         <v>3</v>
       </c>
@@ -4262,7 +4272,7 @@
       <c r="L5" s="11">
         <v>0.95260904725644702</v>
       </c>
-      <c r="M5" s="73">
+      <c r="M5" s="58">
         <f t="shared" si="1"/>
         <v>0.91678180627835093</v>
       </c>
@@ -4288,7 +4298,7 @@
       </c>
     </row>
     <row r="6" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="77" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -4311,7 +4321,7 @@
       <c r="L6" s="4">
         <v>3.8764715799860401</v>
       </c>
-      <c r="M6" s="75">
+      <c r="M6" s="60">
         <f t="shared" ref="M6:M14" si="3">AVERAGE(I6:L6)</f>
         <v>2.9697513553968622</v>
       </c>
@@ -4323,7 +4333,7 @@
       <c r="S6" s="31"/>
     </row>
     <row r="7" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="59"/>
+      <c r="B7" s="78"/>
       <c r="C7" s="6" t="s">
         <v>2</v>
       </c>
@@ -4344,7 +4354,7 @@
       <c r="L7" s="7">
         <v>5.8113440561706202</v>
       </c>
-      <c r="M7" s="76">
+      <c r="M7" s="61">
         <f t="shared" si="3"/>
         <v>3.9127758170678426</v>
       </c>
@@ -4356,7 +4366,7 @@
       <c r="S7" s="31"/>
     </row>
     <row r="8" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="60"/>
+      <c r="B8" s="79"/>
       <c r="C8" s="9" t="s">
         <v>3</v>
       </c>
@@ -4377,7 +4387,7 @@
       <c r="L8" s="11">
         <v>0.93756979228410697</v>
       </c>
-      <c r="M8" s="77">
+      <c r="M8" s="62">
         <f t="shared" si="3"/>
         <v>0.90002519673884451</v>
       </c>
@@ -4389,7 +4399,7 @@
       <c r="S8" s="31"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="77" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -4423,7 +4433,7 @@
       <c r="L9" s="4">
         <v>5.0992717742919904</v>
       </c>
-      <c r="M9" s="75">
+      <c r="M9" s="60">
         <f t="shared" si="3"/>
         <v>3.0401082038879377</v>
       </c>
@@ -4449,7 +4459,7 @@
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B10" s="59"/>
+      <c r="B10" s="78"/>
       <c r="C10" s="6" t="s">
         <v>2</v>
       </c>
@@ -4481,7 +4491,7 @@
       <c r="L10" s="7">
         <v>10.1773061752319</v>
       </c>
-      <c r="M10" s="76">
+      <c r="M10" s="61">
         <f t="shared" si="3"/>
         <v>5.2025534510612381</v>
       </c>
@@ -4507,7 +4517,7 @@
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B11" s="60"/>
+      <c r="B11" s="79"/>
       <c r="C11" s="9" t="s">
         <v>3</v>
       </c>
@@ -4539,7 +4549,7 @@
       <c r="L11" s="11">
         <v>0.89986450953195596</v>
       </c>
-      <c r="M11" s="77">
+      <c r="M11" s="62">
         <f t="shared" si="3"/>
         <v>0.8782371039654342</v>
       </c>
@@ -4565,7 +4575,7 @@
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="77" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -4599,7 +4609,7 @@
       <c r="L12" s="4">
         <v>4.9369132120285499</v>
       </c>
-      <c r="M12" s="75">
+      <c r="M12" s="60">
         <f t="shared" si="3"/>
         <v>3.5515046456024724</v>
       </c>
@@ -4625,7 +4635,7 @@
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B13" s="59"/>
+      <c r="B13" s="78"/>
       <c r="C13" s="6" t="s">
         <v>2</v>
       </c>
@@ -4657,7 +4667,7 @@
       <c r="L13" s="7">
         <v>9.0892070968884102</v>
       </c>
-      <c r="M13" s="76">
+      <c r="M13" s="61">
         <f t="shared" si="3"/>
         <v>5.407339365431282</v>
       </c>
@@ -4683,7 +4693,7 @@
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B14" s="60"/>
+      <c r="B14" s="79"/>
       <c r="C14" s="9" t="s">
         <v>3</v>
       </c>
@@ -4715,7 +4725,7 @@
       <c r="L14" s="11">
         <v>0.96213563093856302</v>
       </c>
-      <c r="M14" s="77">
+      <c r="M14" s="62">
         <f t="shared" si="3"/>
         <v>0.90994596363098057</v>
       </c>
@@ -4761,13 +4771,13 @@
   <dimension ref="B1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="13" width="7.83203125" customWidth="1"/>
-    <col min="14" max="14" width="7.83203125" style="88" customWidth="1"/>
+    <col min="14" max="14" width="7.83203125" style="73" customWidth="1"/>
     <col min="15" max="20" width="7.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4784,32 +4794,32 @@
       <c r="K1" s="49"/>
       <c r="L1" s="49"/>
       <c r="M1" s="49"/>
-      <c r="N1" s="78"/>
+      <c r="N1" s="63"/>
     </row>
     <row r="2" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="48"/>
-      <c r="E2" s="66" t="s">
+      <c r="E2" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="66" t="s">
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="66" t="s">
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="67"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="61" t="s">
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="86"/>
+      <c r="T2" s="87" t="s">
         <v>11</v>
       </c>
     </row>
@@ -4842,7 +4852,7 @@
       <c r="M3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="79" t="s">
+      <c r="N3" s="64" t="s">
         <v>11</v>
       </c>
       <c r="O3" s="13" t="s">
@@ -4860,13 +4870,13 @@
       <c r="S3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="T3" s="61"/>
+      <c r="T3" s="87"/>
     </row>
     <row r="4" spans="2:20" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="88" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="32" t="s">
@@ -4900,7 +4910,7 @@
       <c r="M4" s="5">
         <v>3.8174018183023102</v>
       </c>
-      <c r="N4" s="80">
+      <c r="N4" s="65">
         <f>AVERAGE(J4:M4)</f>
         <v>2.344711916674965</v>
       </c>
@@ -4926,8 +4936,8 @@
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B5" s="69"/>
-      <c r="C5" s="63"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="80"/>
       <c r="D5" s="33" t="s">
         <v>2</v>
       </c>
@@ -4959,8 +4969,8 @@
       <c r="M5" s="8">
         <v>6.6739345871975901</v>
       </c>
-      <c r="N5" s="81">
-        <f t="shared" ref="N5:N12" si="2">AVERAGE(J5:M5)</f>
+      <c r="N5" s="66">
+        <f t="shared" ref="N5:N16" si="2">AVERAGE(J5:M5)</f>
         <v>3.784683046079885</v>
       </c>
       <c r="O5" s="17">
@@ -4985,8 +4995,8 @@
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B6" s="69"/>
-      <c r="C6" s="64"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="83"/>
       <c r="D6" s="35" t="s">
         <v>3</v>
       </c>
@@ -5018,7 +5028,7 @@
       <c r="M6" s="11">
         <v>0.89387289085965904</v>
       </c>
-      <c r="N6" s="82">
+      <c r="N6" s="67">
         <f t="shared" si="2"/>
         <v>0.90070431948485419</v>
       </c>
@@ -5044,8 +5054,8 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B7" s="69"/>
-      <c r="C7" s="63" t="s">
+      <c r="B7" s="82"/>
+      <c r="C7" s="80" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="33" t="s">
@@ -5079,7 +5089,7 @@
       <c r="M7" s="4">
         <v>3.9885256813269501</v>
       </c>
-      <c r="N7" s="83">
+      <c r="N7" s="68">
         <f t="shared" si="2"/>
         <v>2.3850224629946677</v>
       </c>
@@ -5105,8 +5115,8 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B8" s="69"/>
-      <c r="C8" s="63"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="80"/>
       <c r="D8" s="33" t="s">
         <v>2</v>
       </c>
@@ -5138,7 +5148,7 @@
       <c r="M8" s="7">
         <v>7.1204901400938203</v>
       </c>
-      <c r="N8" s="84">
+      <c r="N8" s="69">
         <f t="shared" si="2"/>
         <v>3.7068315760122053</v>
       </c>
@@ -5164,8 +5174,8 @@
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B9" s="69"/>
-      <c r="C9" s="64"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="83"/>
       <c r="D9" s="35" t="s">
         <v>3</v>
       </c>
@@ -5197,7 +5207,7 @@
       <c r="M9" s="10">
         <v>0.96553763117116298</v>
       </c>
-      <c r="N9" s="85">
+      <c r="N9" s="70">
         <f t="shared" si="2"/>
         <v>0.92301232047725934</v>
       </c>
@@ -5223,8 +5233,8 @@
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B10" s="69"/>
-      <c r="C10" s="63" t="s">
+      <c r="B10" s="82"/>
+      <c r="C10" s="80" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="33" t="s">
@@ -5258,7 +5268,7 @@
       <c r="M10" s="4">
         <v>4.9135642051696804</v>
       </c>
-      <c r="N10" s="83">
+      <c r="N10" s="68">
         <f t="shared" si="2"/>
         <v>2.9949735999107374</v>
       </c>
@@ -5284,8 +5294,8 @@
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B11" s="69"/>
-      <c r="C11" s="63"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="33" t="s">
         <v>2</v>
       </c>
@@ -5317,7 +5327,7 @@
       <c r="M11" s="7">
         <v>10.0702199935913</v>
       </c>
-      <c r="N11" s="84">
+      <c r="N11" s="69">
         <f t="shared" si="2"/>
         <v>5.4313469529151872</v>
       </c>
@@ -5343,8 +5353,8 @@
       </c>
     </row>
     <row r="12" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="69"/>
-      <c r="C12" s="65"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="81"/>
       <c r="D12" s="34" t="s">
         <v>3</v>
       </c>
@@ -5376,7 +5386,7 @@
       <c r="M12" s="43">
         <v>0.89094506505740301</v>
       </c>
-      <c r="N12" s="86">
+      <c r="N12" s="71">
         <f t="shared" si="2"/>
         <v>0.86014506516166545</v>
       </c>
@@ -5411,7 +5421,7 @@
       <c r="K13" s="54"/>
       <c r="L13" s="54"/>
       <c r="M13" s="54"/>
-      <c r="N13" s="87"/>
+      <c r="N13" s="72"/>
       <c r="O13" s="54"/>
       <c r="P13" s="54"/>
       <c r="Q13" s="54"/>
@@ -5425,11 +5435,22 @@
       <c r="G14" s="54"/>
       <c r="H14" s="54"/>
       <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="54"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="87"/>
+      <c r="J14" s="21">
+        <v>1.68553034493036</v>
+      </c>
+      <c r="K14" s="5">
+        <v>1.5020625826862199</v>
+      </c>
+      <c r="L14" s="5">
+        <v>1.85347392895776</v>
+      </c>
+      <c r="M14" s="5">
+        <v>3.53088879060993</v>
+      </c>
+      <c r="N14" s="65">
+        <f t="shared" si="2"/>
+        <v>2.1429889117960674</v>
+      </c>
       <c r="O14" s="54"/>
       <c r="P14" s="54"/>
       <c r="Q14" s="54"/>
@@ -5443,11 +5464,22 @@
       <c r="G15" s="54"/>
       <c r="H15" s="54"/>
       <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="54"/>
-      <c r="M15" s="54"/>
-      <c r="N15" s="87"/>
+      <c r="J15" s="17">
+        <v>2.89145108940507</v>
+      </c>
+      <c r="K15" s="8">
+        <v>2.41428861776037</v>
+      </c>
+      <c r="L15" s="7">
+        <v>2.8916910345628999</v>
+      </c>
+      <c r="M15" s="7">
+        <v>7.0112605606291396</v>
+      </c>
+      <c r="N15" s="69">
+        <f t="shared" si="2"/>
+        <v>3.8021728255893699</v>
+      </c>
       <c r="O15" s="54"/>
       <c r="P15" s="54"/>
       <c r="Q15" s="54"/>
@@ -5455,17 +5487,28 @@
       <c r="S15" s="54"/>
       <c r="T15" s="54"/>
     </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E16" s="54"/>
       <c r="F16" s="54"/>
       <c r="G16" s="54"/>
       <c r="H16" s="54"/>
       <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="54"/>
-      <c r="N16" s="87"/>
+      <c r="J16" s="27">
+        <v>0.91113849598193597</v>
+      </c>
+      <c r="K16" s="10">
+        <v>0.94647925984624404</v>
+      </c>
+      <c r="L16" s="10">
+        <v>0.92030712483090504</v>
+      </c>
+      <c r="M16" s="10">
+        <v>0.96357185661028399</v>
+      </c>
+      <c r="N16" s="89">
+        <f t="shared" si="2"/>
+        <v>0.93537418431734221</v>
+      </c>
       <c r="O16" s="54"/>
       <c r="P16" s="54"/>
       <c r="Q16" s="54"/>
@@ -5483,7 +5526,7 @@
       <c r="K17" s="54"/>
       <c r="L17" s="54"/>
       <c r="M17" s="54"/>
-      <c r="N17" s="87"/>
+      <c r="N17" s="72"/>
       <c r="O17" s="54"/>
       <c r="P17" s="54"/>
       <c r="Q17" s="54"/>
@@ -5499,9 +5542,11 @@
       <c r="I18" s="54"/>
       <c r="J18" s="54"/>
       <c r="K18" s="54"/>
-      <c r="L18" s="54"/>
+      <c r="L18" s="54" t="s">
+        <v>21</v>
+      </c>
       <c r="M18" s="54"/>
-      <c r="N18" s="87"/>
+      <c r="N18" s="72"/>
       <c r="O18" s="54"/>
       <c r="P18" s="54"/>
       <c r="Q18" s="54"/>
@@ -5519,7 +5564,7 @@
       <c r="K19" s="54"/>
       <c r="L19" s="54"/>
       <c r="M19" s="54"/>
-      <c r="N19" s="87"/>
+      <c r="N19" s="72"/>
       <c r="O19" s="54"/>
       <c r="P19" s="54"/>
       <c r="Q19" s="54"/>
@@ -5535,9 +5580,11 @@
       <c r="I20" s="54"/>
       <c r="J20" s="54"/>
       <c r="K20" s="54"/>
-      <c r="L20" s="54"/>
+      <c r="L20" s="54" t="s">
+        <v>20</v>
+      </c>
       <c r="M20" s="54"/>
-      <c r="N20" s="87"/>
+      <c r="N20" s="72"/>
       <c r="O20" s="54"/>
       <c r="P20" s="54"/>
       <c r="Q20" s="54"/>
@@ -5552,10 +5599,11 @@
       <c r="H21" s="54"/>
       <c r="I21" s="54"/>
       <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54"/>
+      <c r="L21" s="54" t="s">
+        <v>22</v>
+      </c>
       <c r="M21" s="54"/>
-      <c r="N21" s="87"/>
+      <c r="N21" s="72"/>
       <c r="O21" s="54"/>
       <c r="P21" s="54"/>
       <c r="Q21" s="54"/>
@@ -5573,7 +5621,7 @@
       <c r="K22" s="54"/>
       <c r="L22" s="54"/>
       <c r="M22" s="54"/>
-      <c r="N22" s="87"/>
+      <c r="N22" s="72"/>
       <c r="O22" s="54"/>
       <c r="P22" s="54"/>
       <c r="Q22" s="54"/>
@@ -5583,14 +5631,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="O2:S2"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="C4:C6"/>
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="B4:B12"/>
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:N2"/>
-    <mergeCell ref="O2:S2"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="C4:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5612,28 +5660,28 @@
   <sheetData>
     <row r="1" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="66" t="s">
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="66" t="s">
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="67"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="61" t="s">
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="86"/>
+      <c r="S2" s="87" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5683,10 +5731,10 @@
       <c r="R3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="S3" s="61"/>
+      <c r="S3" s="87"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="88" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="32" t="s">
@@ -5746,7 +5794,7 @@
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B5" s="63"/>
+      <c r="B5" s="80"/>
       <c r="C5" s="33" t="s">
         <v>2</v>
       </c>
@@ -5804,7 +5852,7 @@
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B6" s="64"/>
+      <c r="B6" s="83"/>
       <c r="C6" s="35" t="s">
         <v>3</v>
       </c>
@@ -5860,7 +5908,7 @@
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="80" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="33" t="s">
@@ -5920,7 +5968,7 @@
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B8" s="63"/>
+      <c r="B8" s="80"/>
       <c r="C8" s="33" t="s">
         <v>2</v>
       </c>
@@ -5978,7 +6026,7 @@
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B9" s="64"/>
+      <c r="B9" s="83"/>
       <c r="C9" s="35" t="s">
         <v>3</v>
       </c>
@@ -6034,7 +6082,7 @@
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="80" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="33" t="s">
@@ -6094,7 +6142,7 @@
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B11" s="63"/>
+      <c r="B11" s="80"/>
       <c r="C11" s="33" t="s">
         <v>2</v>
       </c>
@@ -6152,7 +6200,7 @@
       </c>
     </row>
     <row r="12" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="65"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="34" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Added model uncertainty models
</commit_message>
<xml_diff>
--- a/Logging/Tools/Results_Summary.xlsx
+++ b/Logging/Tools/Results_Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/github/Forecasting/Logging/Tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E4912A-ABBC-0748-8D84-FF8C773EC0BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2BAB60-33F0-9D44-9210-6589301FAC88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15880" activeTab="1" xr2:uid="{D6C4A1CF-C8B6-1A42-B202-9397802E1C24}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" activeTab="1" xr2:uid="{D6C4A1CF-C8B6-1A42-B202-9397802E1C24}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="237">
   <si>
     <t>2014/15</t>
   </si>
@@ -775,6 +775,9 @@
   </si>
   <si>
     <t>Parameter</t>
+  </si>
+  <si>
+    <t>Linear Model with Confidence Intervals and Squared Inputs</t>
   </si>
 </sst>
 </file>
@@ -1194,7 +1197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1396,93 +1399,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1493,28 +1409,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1562,19 +1460,120 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6927,8 +6926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F65057-F8D9-5340-9C4E-E5CBE3EA5B75}">
   <dimension ref="B1:BW103"/>
   <sheetViews>
-    <sheetView topLeftCell="S21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V26" sqref="V26:AE44"/>
+    <sheetView topLeftCell="R3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X56" sqref="X56:AA59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6955,28 +6954,28 @@
     </row>
     <row r="2" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="13"/>
-      <c r="E2" s="128" t="s">
+      <c r="E2" s="171" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="129"/>
-      <c r="G2" s="129"/>
-      <c r="H2" s="129"/>
-      <c r="I2" s="130"/>
-      <c r="J2" s="128" t="s">
+      <c r="F2" s="172"/>
+      <c r="G2" s="172"/>
+      <c r="H2" s="172"/>
+      <c r="I2" s="173"/>
+      <c r="J2" s="171" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="129"/>
-      <c r="L2" s="129"/>
-      <c r="M2" s="129"/>
-      <c r="N2" s="130"/>
-      <c r="O2" s="128" t="s">
+      <c r="K2" s="172"/>
+      <c r="L2" s="172"/>
+      <c r="M2" s="172"/>
+      <c r="N2" s="173"/>
+      <c r="O2" s="171" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="129"/>
-      <c r="Q2" s="129"/>
-      <c r="R2" s="129"/>
-      <c r="S2" s="130"/>
-      <c r="T2" s="141" t="s">
+      <c r="P2" s="172"/>
+      <c r="Q2" s="172"/>
+      <c r="R2" s="172"/>
+      <c r="S2" s="173"/>
+      <c r="T2" s="174" t="s">
         <v>9</v>
       </c>
     </row>
@@ -7027,13 +7026,13 @@
       <c r="S3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="T3" s="141"/>
+      <c r="T3" s="174"/>
     </row>
     <row r="4" spans="2:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="140" t="s">
+      <c r="B4" s="170" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="142" t="s">
+      <c r="C4" s="175" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="8" t="s">
@@ -7093,8 +7092,8 @@
       </c>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B5" s="140"/>
-      <c r="C5" s="138"/>
+      <c r="B5" s="170"/>
+      <c r="C5" s="165"/>
       <c r="D5" s="9" t="s">
         <v>2</v>
       </c>
@@ -7152,8 +7151,8 @@
       </c>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B6" s="140"/>
-      <c r="C6" s="143"/>
+      <c r="B6" s="170"/>
+      <c r="C6" s="176"/>
       <c r="D6" s="11" t="s">
         <v>3</v>
       </c>
@@ -7211,8 +7210,8 @@
       </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B7" s="140"/>
-      <c r="C7" s="138" t="s">
+      <c r="B7" s="170"/>
+      <c r="C7" s="165" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="9" t="s">
@@ -7272,8 +7271,8 @@
       </c>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B8" s="140"/>
-      <c r="C8" s="138"/>
+      <c r="B8" s="170"/>
+      <c r="C8" s="165"/>
       <c r="D8" s="9" t="s">
         <v>2</v>
       </c>
@@ -7331,8 +7330,8 @@
       </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B9" s="140"/>
-      <c r="C9" s="143"/>
+      <c r="B9" s="170"/>
+      <c r="C9" s="176"/>
       <c r="D9" s="11" t="s">
         <v>3</v>
       </c>
@@ -7390,8 +7389,8 @@
       </c>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B10" s="140"/>
-      <c r="C10" s="138" t="s">
+      <c r="B10" s="170"/>
+      <c r="C10" s="165" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="9" t="s">
@@ -7451,8 +7450,8 @@
       </c>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B11" s="140"/>
-      <c r="C11" s="138"/>
+      <c r="B11" s="170"/>
+      <c r="C11" s="165"/>
       <c r="D11" s="9" t="s">
         <v>2</v>
       </c>
@@ -7510,8 +7509,8 @@
       </c>
     </row>
     <row r="12" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="140"/>
-      <c r="C12" s="139"/>
+      <c r="B12" s="170"/>
+      <c r="C12" s="166"/>
       <c r="D12" s="10" t="s">
         <v>3</v>
       </c>
@@ -7569,8 +7568,8 @@
       </c>
     </row>
     <row r="13" spans="2:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="140"/>
-      <c r="C13" s="138" t="s">
+      <c r="B13" s="170"/>
+      <c r="C13" s="165" t="s">
         <v>208</v>
       </c>
       <c r="D13" s="9" t="s">
@@ -7630,8 +7629,8 @@
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B14" s="140"/>
-      <c r="C14" s="138"/>
+      <c r="B14" s="170"/>
+      <c r="C14" s="165"/>
       <c r="D14" s="9" t="s">
         <v>2</v>
       </c>
@@ -7693,8 +7692,8 @@
       </c>
     </row>
     <row r="15" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="140"/>
-      <c r="C15" s="139"/>
+      <c r="B15" s="170"/>
+      <c r="C15" s="166"/>
       <c r="D15" s="10" t="s">
         <v>3</v>
       </c>
@@ -7752,7 +7751,7 @@
       </c>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="C16" s="138" t="s">
+      <c r="C16" s="165" t="s">
         <v>207</v>
       </c>
       <c r="D16" s="9" t="s">
@@ -7812,7 +7811,7 @@
       </c>
     </row>
     <row r="17" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="C17" s="138"/>
+      <c r="C17" s="165"/>
       <c r="D17" s="9" t="s">
         <v>2</v>
       </c>
@@ -7870,7 +7869,7 @@
       </c>
     </row>
     <row r="18" spans="2:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="139"/>
+      <c r="C18" s="166"/>
       <c r="D18" s="10" t="s">
         <v>3</v>
       </c>
@@ -7928,7 +7927,7 @@
       </c>
     </row>
     <row r="19" spans="2:39" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C19" s="138" t="s">
+      <c r="C19" s="165" t="s">
         <v>182</v>
       </c>
       <c r="D19" s="9" t="s">
@@ -7963,7 +7962,7 @@
       <c r="T19" s="48"/>
     </row>
     <row r="20" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="C20" s="138"/>
+      <c r="C20" s="165"/>
       <c r="D20" s="9" t="s">
         <v>2</v>
       </c>
@@ -7996,7 +7995,7 @@
       <c r="T20" s="48"/>
     </row>
     <row r="21" spans="2:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="139"/>
+      <c r="C21" s="166"/>
       <c r="D21" s="10" t="s">
         <v>3</v>
       </c>
@@ -8029,7 +8028,7 @@
       <c r="T21" s="52"/>
     </row>
     <row r="22" spans="2:39" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="138" t="s">
+      <c r="C22" s="165" t="s">
         <v>183</v>
       </c>
       <c r="D22" s="9" t="s">
@@ -8064,7 +8063,7 @@
       <c r="T22" s="25"/>
     </row>
     <row r="23" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="C23" s="138"/>
+      <c r="C23" s="165"/>
       <c r="D23" s="9" t="s">
         <v>2</v>
       </c>
@@ -8097,7 +8096,7 @@
       <c r="T23" s="32"/>
     </row>
     <row r="24" spans="2:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="139"/>
+      <c r="C24" s="166"/>
       <c r="D24" s="10" t="s">
         <v>3</v>
       </c>
@@ -8131,48 +8130,48 @@
     </row>
     <row r="25" spans="2:39" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E26" s="128" t="s">
+      <c r="E26" s="171" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="129"/>
-      <c r="G26" s="129"/>
-      <c r="H26" s="129"/>
-      <c r="I26" s="130"/>
-      <c r="J26" s="128" t="s">
+      <c r="F26" s="172"/>
+      <c r="G26" s="172"/>
+      <c r="H26" s="172"/>
+      <c r="I26" s="173"/>
+      <c r="J26" s="171" t="s">
         <v>11</v>
       </c>
-      <c r="K26" s="129"/>
-      <c r="L26" s="129"/>
-      <c r="M26" s="129"/>
-      <c r="N26" s="130"/>
-      <c r="O26" s="128" t="s">
+      <c r="K26" s="172"/>
+      <c r="L26" s="172"/>
+      <c r="M26" s="172"/>
+      <c r="N26" s="173"/>
+      <c r="O26" s="171" t="s">
         <v>12</v>
       </c>
-      <c r="P26" s="129"/>
-      <c r="Q26" s="129"/>
-      <c r="R26" s="129"/>
-      <c r="S26" s="130"/>
+      <c r="P26" s="172"/>
+      <c r="Q26" s="172"/>
+      <c r="R26" s="172"/>
+      <c r="S26" s="173"/>
       <c r="T26" s="68"/>
-      <c r="X26" s="127" t="s">
+      <c r="X26" s="180" t="s">
         <v>209</v>
       </c>
-      <c r="Y26" s="127"/>
-      <c r="Z26" s="127"/>
-      <c r="AA26" s="127"/>
-      <c r="AB26" s="127"/>
-      <c r="AC26" s="127"/>
-      <c r="AD26" s="127"/>
-      <c r="AE26" s="127"/>
-      <c r="AF26" s="127" t="s">
+      <c r="Y26" s="180"/>
+      <c r="Z26" s="180"/>
+      <c r="AA26" s="180"/>
+      <c r="AB26" s="180"/>
+      <c r="AC26" s="180"/>
+      <c r="AD26" s="180"/>
+      <c r="AE26" s="180"/>
+      <c r="AF26" s="180" t="s">
         <v>206</v>
       </c>
-      <c r="AG26" s="127"/>
-      <c r="AH26" s="127"/>
-      <c r="AI26" s="127"/>
-      <c r="AJ26" s="127"/>
-      <c r="AK26" s="127"/>
-      <c r="AL26" s="127"/>
-      <c r="AM26" s="127"/>
+      <c r="AG26" s="180"/>
+      <c r="AH26" s="180"/>
+      <c r="AI26" s="180"/>
+      <c r="AJ26" s="180"/>
+      <c r="AK26" s="180"/>
+      <c r="AL26" s="180"/>
+      <c r="AM26" s="180"/>
     </row>
     <row r="27" spans="2:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E27" s="69" t="s">
@@ -8223,36 +8222,36 @@
       <c r="T27" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="X27" s="127" t="s">
+      <c r="X27" s="180" t="s">
         <v>210</v>
       </c>
-      <c r="Y27" s="127"/>
-      <c r="Z27" s="127"/>
-      <c r="AA27" s="127"/>
-      <c r="AB27" s="127" t="s">
+      <c r="Y27" s="180"/>
+      <c r="Z27" s="180"/>
+      <c r="AA27" s="180"/>
+      <c r="AB27" s="180" t="s">
         <v>5</v>
       </c>
-      <c r="AC27" s="127"/>
-      <c r="AD27" s="127"/>
-      <c r="AE27" s="127"/>
-      <c r="AF27" s="127" t="s">
+      <c r="AC27" s="180"/>
+      <c r="AD27" s="180"/>
+      <c r="AE27" s="180"/>
+      <c r="AF27" s="180" t="s">
         <v>210</v>
       </c>
-      <c r="AG27" s="127"/>
-      <c r="AH27" s="127"/>
-      <c r="AI27" s="127"/>
-      <c r="AJ27" s="127" t="s">
+      <c r="AG27" s="180"/>
+      <c r="AH27" s="180"/>
+      <c r="AI27" s="180"/>
+      <c r="AJ27" s="180" t="s">
         <v>5</v>
       </c>
-      <c r="AK27" s="127"/>
-      <c r="AL27" s="127"/>
-      <c r="AM27" s="127"/>
+      <c r="AK27" s="180"/>
+      <c r="AL27" s="180"/>
+      <c r="AM27" s="180"/>
     </row>
     <row r="28" spans="2:39" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="134" t="s">
+      <c r="B28" s="177" t="s">
         <v>209</v>
       </c>
-      <c r="C28" s="131" t="s">
+      <c r="C28" s="160" t="s">
         <v>210</v>
       </c>
       <c r="D28" s="53" t="s">
@@ -8366,8 +8365,8 @@
       </c>
     </row>
     <row r="29" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B29" s="135"/>
-      <c r="C29" s="132"/>
+      <c r="B29" s="163"/>
+      <c r="C29" s="161"/>
       <c r="D29" s="2" t="s">
         <v>2</v>
       </c>
@@ -8423,7 +8422,7 @@
         <f t="shared" ref="T29:T39" si="12">AVERAGE(I29,N29,S29)</f>
         <v>3.5639650679250701</v>
       </c>
-      <c r="V29" s="151">
+      <c r="V29" s="152">
         <v>7</v>
       </c>
       <c r="W29" s="101" t="s">
@@ -8479,8 +8478,8 @@
       </c>
     </row>
     <row r="30" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B30" s="135"/>
-      <c r="C30" s="132"/>
+      <c r="B30" s="163"/>
+      <c r="C30" s="161"/>
       <c r="D30" s="2" t="s">
         <v>3</v>
       </c>
@@ -8536,7 +8535,7 @@
         <f t="shared" si="12"/>
         <v>0.93524402885015689</v>
       </c>
-      <c r="V30" s="152"/>
+      <c r="V30" s="153"/>
       <c r="W30" s="105" t="s">
         <v>6</v>
       </c>
@@ -8590,8 +8589,8 @@
       </c>
     </row>
     <row r="31" spans="2:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="135"/>
-      <c r="C31" s="133"/>
+      <c r="B31" s="163"/>
+      <c r="C31" s="162"/>
       <c r="D31" s="54" t="s">
         <v>211</v>
       </c>
@@ -8647,7 +8646,7 @@
         <f t="shared" si="12"/>
         <v>15.833333333333334</v>
       </c>
-      <c r="V31" s="152"/>
+      <c r="V31" s="153"/>
       <c r="W31" s="105" t="s">
         <v>7</v>
       </c>
@@ -8701,8 +8700,8 @@
       </c>
     </row>
     <row r="32" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B32" s="135"/>
-      <c r="C32" s="131" t="s">
+      <c r="B32" s="163"/>
+      <c r="C32" s="160" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="53" t="s">
@@ -8760,7 +8759,7 @@
         <f t="shared" si="12"/>
         <v>2.2776308536949266</v>
       </c>
-      <c r="V32" s="152"/>
+      <c r="V32" s="153"/>
       <c r="W32" s="105" t="s">
         <v>8</v>
       </c>
@@ -8813,9 +8812,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="2:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="135"/>
-      <c r="C33" s="132"/>
+    <row r="33" spans="2:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="163"/>
+      <c r="C33" s="161"/>
       <c r="D33" s="2" t="s">
         <v>2</v>
       </c>
@@ -8871,7 +8870,7 @@
         <f t="shared" si="12"/>
         <v>3.7603605058238752</v>
       </c>
-      <c r="V33" s="153"/>
+      <c r="V33" s="154"/>
       <c r="W33" s="72" t="s">
         <v>9</v>
       </c>
@@ -8940,9 +8939,9 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="34" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B34" s="135"/>
-      <c r="C34" s="132"/>
+    <row r="34" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="B34" s="163"/>
+      <c r="C34" s="161"/>
       <c r="D34" s="2" t="s">
         <v>3</v>
       </c>
@@ -8998,7 +8997,7 @@
         <f t="shared" si="12"/>
         <v>0.91488429714260311</v>
       </c>
-      <c r="V34" s="151">
+      <c r="V34" s="152">
         <v>14</v>
       </c>
       <c r="W34" s="101" t="s">
@@ -9053,9 +9052,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="2:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="135"/>
-      <c r="C35" s="133"/>
+    <row r="35" spans="2:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="163"/>
+      <c r="C35" s="162"/>
       <c r="D35" s="95" t="s">
         <v>211</v>
       </c>
@@ -9111,7 +9110,7 @@
         <f t="shared" si="12"/>
         <v>10.583333333333334</v>
       </c>
-      <c r="V35" s="152"/>
+      <c r="V35" s="153"/>
       <c r="W35" s="105" t="s">
         <v>6</v>
       </c>
@@ -9164,9 +9163,9 @@
         <v>-55</v>
       </c>
     </row>
-    <row r="36" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B36" s="135"/>
-      <c r="C36" s="132" t="s">
+    <row r="36" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="B36" s="163"/>
+      <c r="C36" s="161" t="s">
         <v>4</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -9224,7 +9223,7 @@
         <f t="shared" si="12"/>
         <v>3.0008085841689058</v>
       </c>
-      <c r="V36" s="152"/>
+      <c r="V36" s="153"/>
       <c r="W36" s="105" t="s">
         <v>7</v>
       </c>
@@ -9277,9 +9276,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B37" s="135"/>
-      <c r="C37" s="132"/>
+    <row r="37" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="B37" s="163"/>
+      <c r="C37" s="161"/>
       <c r="D37" s="2" t="s">
         <v>2</v>
       </c>
@@ -9335,7 +9334,7 @@
         <f t="shared" si="12"/>
         <v>5.158547971052232</v>
       </c>
-      <c r="V37" s="152"/>
+      <c r="V37" s="153"/>
       <c r="W37" s="105" t="s">
         <v>8</v>
       </c>
@@ -9388,9 +9387,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="2:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="135"/>
-      <c r="C38" s="132"/>
+    <row r="38" spans="2:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="163"/>
+      <c r="C38" s="161"/>
       <c r="D38" s="2" t="s">
         <v>3</v>
       </c>
@@ -9446,7 +9445,7 @@
         <f t="shared" si="12"/>
         <v>0.87064370203199515</v>
       </c>
-      <c r="V38" s="153"/>
+      <c r="V38" s="154"/>
       <c r="W38" s="72" t="s">
         <v>9</v>
       </c>
@@ -9515,9 +9514,9 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="39" spans="2:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="136"/>
-      <c r="C39" s="137"/>
+    <row r="39" spans="2:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="178"/>
+      <c r="C39" s="179"/>
       <c r="D39" s="92" t="s">
         <v>212</v>
       </c>
@@ -9573,7 +9572,7 @@
         <f t="shared" si="12"/>
         <v>23.25</v>
       </c>
-      <c r="V39" s="151">
+      <c r="V39" s="152">
         <v>21</v>
       </c>
       <c r="W39" s="101" t="s">
@@ -9628,11 +9627,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="2:39" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="135" t="s">
+    <row r="40" spans="2:40" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="163" t="s">
         <v>206</v>
       </c>
-      <c r="C40" s="132" t="s">
+      <c r="C40" s="161" t="s">
         <v>210</v>
       </c>
       <c r="D40" s="13" t="s">
@@ -9690,7 +9689,7 @@
         <f>AVERAGE(I40,N40,S40)</f>
         <v>0.48197307962486019</v>
       </c>
-      <c r="V40" s="152"/>
+      <c r="V40" s="153"/>
       <c r="W40" s="105" t="s">
         <v>6</v>
       </c>
@@ -9743,9 +9742,9 @@
         <v>-48</v>
       </c>
     </row>
-    <row r="41" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B41" s="135"/>
-      <c r="C41" s="132"/>
+    <row r="41" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="B41" s="163"/>
+      <c r="C41" s="161"/>
       <c r="D41" s="13" t="s">
         <v>2</v>
       </c>
@@ -9801,7 +9800,7 @@
         <f>AVERAGE(I41,N41,S41)</f>
         <v>0.71483607643238045</v>
       </c>
-      <c r="V41" s="152"/>
+      <c r="V41" s="153"/>
       <c r="W41" s="105" t="s">
         <v>7</v>
       </c>
@@ -9854,9 +9853,9 @@
         <v>-19</v>
       </c>
     </row>
-    <row r="42" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B42" s="135"/>
-      <c r="C42" s="132"/>
+    <row r="42" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="B42" s="163"/>
+      <c r="C42" s="161"/>
       <c r="D42" s="13" t="s">
         <v>3</v>
       </c>
@@ -9912,7 +9911,7 @@
         <f>AVERAGE(I42,N42,S42)</f>
         <v>0.89514895097951153</v>
       </c>
-      <c r="V42" s="152"/>
+      <c r="V42" s="153"/>
       <c r="W42" s="105" t="s">
         <v>8</v>
       </c>
@@ -9965,9 +9964,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="2:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="135"/>
-      <c r="C43" s="133"/>
+    <row r="43" spans="2:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="163"/>
+      <c r="C43" s="162"/>
       <c r="D43" s="54" t="s">
         <v>211</v>
       </c>
@@ -10023,7 +10022,7 @@
         <f>AVERAGE(I43,N43,S43)</f>
         <v>12.666666666666666</v>
       </c>
-      <c r="V43" s="153"/>
+      <c r="V43" s="154"/>
       <c r="W43" s="72" t="s">
         <v>9</v>
       </c>
@@ -10092,9 +10091,9 @@
         <v>29.25</v>
       </c>
     </row>
-    <row r="44" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B44" s="135"/>
-      <c r="C44" s="131" t="s">
+    <row r="44" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="B44" s="163"/>
+      <c r="C44" s="160" t="s">
         <v>5</v>
       </c>
       <c r="D44" s="13" t="s">
@@ -10152,10 +10151,10 @@
         <f t="shared" ref="T44:T51" si="21">AVERAGE(I44,N44,S44)</f>
         <v>0.38309457795371937</v>
       </c>
-      <c r="V44" s="154" t="s">
+      <c r="V44" s="155" t="s">
         <v>9</v>
       </c>
-      <c r="W44" s="155"/>
+      <c r="W44" s="156"/>
       <c r="X44" s="113">
         <f t="shared" ref="X44:AM44" si="22">AVERAGE(X33,X38,X43)</f>
         <v>2.1519019847241818</v>
@@ -10221,9 +10220,9 @@
         <v>22.666666666666668</v>
       </c>
     </row>
-    <row r="45" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B45" s="135"/>
-      <c r="C45" s="132"/>
+    <row r="45" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="B45" s="163"/>
+      <c r="C45" s="161"/>
       <c r="D45" s="13" t="s">
         <v>2</v>
       </c>
@@ -10280,9 +10279,9 @@
         <v>0.64001520720967164</v>
       </c>
     </row>
-    <row r="46" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B46" s="135"/>
-      <c r="C46" s="132"/>
+    <row r="46" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="B46" s="163"/>
+      <c r="C46" s="161"/>
       <c r="D46" s="13" t="s">
         <v>3</v>
       </c>
@@ -10339,9 +10338,9 @@
         <v>0.89019675793226261</v>
       </c>
     </row>
-    <row r="47" spans="2:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="135"/>
-      <c r="C47" s="133"/>
+    <row r="47" spans="2:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="163"/>
+      <c r="C47" s="162"/>
       <c r="D47" s="54" t="s">
         <v>212</v>
       </c>
@@ -10398,9 +10397,9 @@
         <v>22.666666666666668</v>
       </c>
     </row>
-    <row r="48" spans="2:39" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="135"/>
-      <c r="C48" s="131" t="s">
+    <row r="48" spans="2:40" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="163"/>
+      <c r="C48" s="160" t="s">
         <v>4</v>
       </c>
       <c r="D48" s="13" t="s">
@@ -10458,10 +10457,34 @@
         <f t="shared" si="21"/>
         <v>0.39189308315984867</v>
       </c>
+      <c r="AF48" s="14">
+        <v>0.35796936955289599</v>
+      </c>
+      <c r="AG48" s="14">
+        <v>0.66473447345483505</v>
+      </c>
+      <c r="AH48" s="14">
+        <v>0.92222008954877499</v>
+      </c>
+      <c r="AI48" s="14">
+        <v>14</v>
+      </c>
+      <c r="AK48" s="14">
+        <v>0.35796936955289599</v>
+      </c>
+      <c r="AL48" s="14">
+        <v>0.66473447345483505</v>
+      </c>
+      <c r="AM48" s="14">
+        <v>0.92222008954877499</v>
+      </c>
+      <c r="AN48" s="14">
+        <v>14</v>
+      </c>
     </row>
     <row r="49" spans="2:75" x14ac:dyDescent="0.2">
-      <c r="B49" s="135"/>
-      <c r="C49" s="132"/>
+      <c r="B49" s="163"/>
+      <c r="C49" s="161"/>
       <c r="D49" s="13" t="s">
         <v>2</v>
       </c>
@@ -10517,10 +10540,34 @@
         <f t="shared" si="21"/>
         <v>0.65457595636860355</v>
       </c>
+      <c r="AF49" s="14">
+        <v>0.70783747752433801</v>
+      </c>
+      <c r="AG49" s="14">
+        <v>0.91714326933989698</v>
+      </c>
+      <c r="AH49" s="14">
+        <v>0.68507741763765395</v>
+      </c>
+      <c r="AI49" s="14">
+        <v>-76</v>
+      </c>
+      <c r="AK49" s="14">
+        <v>0.70783747752433801</v>
+      </c>
+      <c r="AL49" s="14">
+        <v>0.91714326933989698</v>
+      </c>
+      <c r="AM49" s="14">
+        <v>0.68507741763765395</v>
+      </c>
+      <c r="AN49" s="14">
+        <v>-76</v>
+      </c>
     </row>
     <row r="50" spans="2:75" x14ac:dyDescent="0.2">
-      <c r="B50" s="135"/>
-      <c r="C50" s="132"/>
+      <c r="B50" s="163"/>
+      <c r="C50" s="161"/>
       <c r="D50" s="13" t="s">
         <v>3</v>
       </c>
@@ -10576,10 +10623,46 @@
         <f t="shared" si="21"/>
         <v>0.9228938832775202</v>
       </c>
+      <c r="X50" s="14">
+        <v>2.18889478259779</v>
+      </c>
+      <c r="Y50" s="14">
+        <v>3.1818987539986998</v>
+      </c>
+      <c r="Z50" s="14">
+        <v>0.916741705190941</v>
+      </c>
+      <c r="AA50" s="14">
+        <v>-1</v>
+      </c>
+      <c r="AF50" s="14">
+        <v>0.31514394509268701</v>
+      </c>
+      <c r="AG50" s="14">
+        <v>0.60444995035413995</v>
+      </c>
+      <c r="AH50" s="14">
+        <v>0.91300985657772304</v>
+      </c>
+      <c r="AI50" s="14">
+        <v>27</v>
+      </c>
+      <c r="AK50" s="14">
+        <v>0.31514394509268701</v>
+      </c>
+      <c r="AL50" s="14">
+        <v>0.60444995035413995</v>
+      </c>
+      <c r="AM50" s="14">
+        <v>0.91300985657772304</v>
+      </c>
+      <c r="AN50" s="14">
+        <v>27</v>
+      </c>
     </row>
     <row r="51" spans="2:75" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="147"/>
-      <c r="C51" s="133"/>
+      <c r="B51" s="164"/>
+      <c r="C51" s="162"/>
       <c r="D51" s="54" t="s">
         <v>212</v>
       </c>
@@ -10635,14 +10718,90 @@
         <f t="shared" si="21"/>
         <v>15.333333333333334</v>
       </c>
-    </row>
-    <row r="52" spans="2:75" x14ac:dyDescent="0.2">
+      <c r="X51" s="14">
+        <v>2.4345324171165399</v>
+      </c>
+      <c r="Y51" s="14">
+        <v>3.87634162808421</v>
+      </c>
+      <c r="Z51" s="14">
+        <v>0.90012737645273899</v>
+      </c>
+      <c r="AA51" s="14">
+        <v>24</v>
+      </c>
+      <c r="AF51" s="14">
+        <v>0.47714903688258298</v>
+      </c>
+      <c r="AG51" s="14">
+        <v>0.85981918366161003</v>
+      </c>
+      <c r="AH51" s="14">
+        <v>0.97298149372320797</v>
+      </c>
+      <c r="AI51" s="14">
+        <v>-25</v>
+      </c>
+      <c r="AK51" s="14">
+        <v>0.47714903688258298</v>
+      </c>
+      <c r="AL51" s="14">
+        <v>0.85981918366161003</v>
+      </c>
+      <c r="AM51" s="14">
+        <v>0.97298149372320797</v>
+      </c>
+      <c r="AN51" s="14">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="52" spans="2:75" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="N52"/>
+      <c r="X52" s="14">
+        <v>1.4884645490472499</v>
+      </c>
+      <c r="Y52" s="14">
+        <v>1.8761973152521301</v>
+      </c>
+      <c r="Z52" s="14">
+        <v>0.93133083264287697</v>
+      </c>
+      <c r="AA52" s="14">
+        <v>-10</v>
+      </c>
+      <c r="AF52" s="112">
+        <f>AVERAGE(AF48:AF51)</f>
+        <v>0.46452495726312598</v>
+      </c>
+      <c r="AG52" s="109">
+        <f>AVERAGE(AG48:AG51)</f>
+        <v>0.76153671920262056</v>
+      </c>
+      <c r="AH52" s="110">
+        <f>AVERAGE(AH48:AH51)</f>
+        <v>0.87332221437183999</v>
+      </c>
+      <c r="AI52" s="111" cm="1">
+        <f t="array" ref="AI52">AVERAGE(ABS(AI48:AI51))</f>
+        <v>35.5</v>
+      </c>
     </row>
     <row r="53" spans="2:75" x14ac:dyDescent="0.2">
       <c r="N53"/>
-    </row>
-    <row r="54" spans="2:75" x14ac:dyDescent="0.2">
+      <c r="X53" s="14">
+        <v>2.34718667513649</v>
+      </c>
+      <c r="Y53" s="14">
+        <v>5.1280902147820804</v>
+      </c>
+      <c r="Z53" s="14">
+        <v>0.94798486909373503</v>
+      </c>
+      <c r="AA53" s="14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="2:75" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>214</v>
       </c>
@@ -10650,6 +10809,34 @@
         <v>213</v>
       </c>
       <c r="N54"/>
+      <c r="X54" s="112">
+        <f>AVERAGE(X50:X53)</f>
+        <v>2.1147696059745176</v>
+      </c>
+      <c r="Y54" s="109">
+        <f>AVERAGE(Y50:Y53)</f>
+        <v>3.5156319780292802</v>
+      </c>
+      <c r="Z54" s="110">
+        <f>AVERAGE(Z50:Z53)</f>
+        <v>0.92404619584507297</v>
+      </c>
+      <c r="AA54" s="111" cm="1">
+        <f t="array" ref="AA54">AVERAGE(ABS(AA50:AA53))</f>
+        <v>12.5</v>
+      </c>
+      <c r="AC54" s="14">
+        <v>2.4567639652206101</v>
+      </c>
+      <c r="AD54" s="14">
+        <v>2.5687105568278001</v>
+      </c>
+      <c r="AE54" s="14">
+        <v>1.4237578110570199</v>
+      </c>
+      <c r="AF54" s="14">
+        <v>4.1331423251827397</v>
+      </c>
     </row>
     <row r="55" spans="2:75" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
@@ -10681,6 +10868,18 @@
       <c r="U55" s="13"/>
       <c r="V55" s="13"/>
       <c r="W55" s="13"/>
+      <c r="AC55" s="14">
+        <v>3.60906396395155</v>
+      </c>
+      <c r="AD55" s="14">
+        <v>4.1564176321666499</v>
+      </c>
+      <c r="AE55" s="14">
+        <v>1.84851632832792</v>
+      </c>
+      <c r="AF55" s="14">
+        <v>7.7586509468645399</v>
+      </c>
       <c r="AQ55" s="13"/>
       <c r="AR55" s="13"/>
       <c r="AS55" s="13"/>
@@ -10716,10 +10915,10 @@
       <c r="BW55" s="13"/>
     </row>
     <row r="56" spans="2:75" x14ac:dyDescent="0.2">
-      <c r="B56" s="148">
+      <c r="B56" s="167">
         <v>0</v>
       </c>
-      <c r="C56" s="144">
+      <c r="C56" s="157">
         <v>0</v>
       </c>
       <c r="D56" s="53" t="s">
@@ -10748,6 +10947,30 @@
       <c r="U56" s="55"/>
       <c r="V56" s="55"/>
       <c r="W56" s="55"/>
+      <c r="X56" s="14">
+        <v>2.4567639652206101</v>
+      </c>
+      <c r="Y56" s="14">
+        <v>3.60906396395155</v>
+      </c>
+      <c r="Z56" s="14">
+        <v>0.90480715838214798</v>
+      </c>
+      <c r="AA56" s="14">
+        <v>-1</v>
+      </c>
+      <c r="AC56" s="14">
+        <v>0.90480715838214798</v>
+      </c>
+      <c r="AD56" s="14">
+        <v>0.89542968062926698</v>
+      </c>
+      <c r="AE56" s="14">
+        <v>0.94037969334473304</v>
+      </c>
+      <c r="AF56" s="14">
+        <v>0.93867726209864499</v>
+      </c>
       <c r="AQ56" s="55"/>
       <c r="AR56" s="55"/>
       <c r="AS56" s="55"/>
@@ -10783,8 +11006,8 @@
       <c r="BW56" s="55"/>
     </row>
     <row r="57" spans="2:75" x14ac:dyDescent="0.2">
-      <c r="B57" s="149"/>
-      <c r="C57" s="145"/>
+      <c r="B57" s="168"/>
+      <c r="C57" s="158"/>
       <c r="D57" s="2" t="s">
         <v>2</v>
       </c>
@@ -10815,6 +11038,30 @@
       <c r="U57" s="55"/>
       <c r="V57" s="55"/>
       <c r="W57" s="55"/>
+      <c r="X57" s="14">
+        <v>2.5687105568278001</v>
+      </c>
+      <c r="Y57" s="14">
+        <v>4.1564176321666499</v>
+      </c>
+      <c r="Z57" s="14">
+        <v>0.89542968062926698</v>
+      </c>
+      <c r="AA57" s="14">
+        <v>12</v>
+      </c>
+      <c r="AC57" s="14">
+        <v>-1</v>
+      </c>
+      <c r="AD57" s="14">
+        <v>12</v>
+      </c>
+      <c r="AE57" s="14">
+        <v>-10</v>
+      </c>
+      <c r="AF57" s="14">
+        <v>15</v>
+      </c>
       <c r="AQ57" s="55"/>
       <c r="AR57" s="55"/>
       <c r="AS57" s="55"/>
@@ -10850,8 +11097,8 @@
       <c r="BW57" s="55"/>
     </row>
     <row r="58" spans="2:75" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="150"/>
-      <c r="C58" s="146"/>
+      <c r="B58" s="169"/>
+      <c r="C58" s="159"/>
       <c r="D58" s="54" t="s">
         <v>3</v>
       </c>
@@ -10882,6 +11129,22 @@
       <c r="U58" s="55"/>
       <c r="V58" s="55"/>
       <c r="W58" s="55"/>
+      <c r="X58" s="14">
+        <v>1.4237578110570199</v>
+      </c>
+      <c r="Y58" s="14">
+        <v>1.84851632832792</v>
+      </c>
+      <c r="Z58" s="14">
+        <v>0.94037969334473304</v>
+      </c>
+      <c r="AA58" s="14">
+        <v>-10</v>
+      </c>
+      <c r="AC58" s="14"/>
+      <c r="AD58" s="14"/>
+      <c r="AE58" s="14"/>
+      <c r="AF58" s="14"/>
       <c r="AQ58" s="55"/>
       <c r="AR58" s="55"/>
       <c r="AS58" s="55"/>
@@ -10917,10 +11180,10 @@
       <c r="BW58" s="55"/>
     </row>
     <row r="59" spans="2:75" x14ac:dyDescent="0.2">
-      <c r="B59" s="148">
+      <c r="B59" s="167">
         <v>0</v>
       </c>
-      <c r="C59" s="144">
+      <c r="C59" s="157">
         <v>1E-3</v>
       </c>
       <c r="D59" s="53" t="s">
@@ -10952,10 +11215,34 @@
       <c r="N59" s="55"/>
       <c r="O59" s="55"/>
       <c r="P59" s="55"/>
-    </row>
-    <row r="60" spans="2:75" x14ac:dyDescent="0.2">
-      <c r="B60" s="149"/>
-      <c r="C60" s="145"/>
+      <c r="X59" s="14">
+        <v>4.1331423251827397</v>
+      </c>
+      <c r="Y59" s="14">
+        <v>7.7586509468645399</v>
+      </c>
+      <c r="Z59" s="14">
+        <v>0.93867726209864499</v>
+      </c>
+      <c r="AA59" s="14">
+        <v>15</v>
+      </c>
+      <c r="AC59" s="14">
+        <v>2.4567639652206101</v>
+      </c>
+      <c r="AD59" s="14">
+        <v>3.60906396395155</v>
+      </c>
+      <c r="AE59" s="14">
+        <v>0.90480715838214798</v>
+      </c>
+      <c r="AF59" s="14">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:75" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="168"/>
+      <c r="C60" s="158"/>
       <c r="D60" s="2" t="s">
         <v>2</v>
       </c>
@@ -10983,10 +11270,38 @@
       <c r="N60" s="55"/>
       <c r="O60" s="55"/>
       <c r="P60" s="55"/>
+      <c r="X60" s="112">
+        <f>AVERAGE(X56:X59)</f>
+        <v>2.6455936645720426</v>
+      </c>
+      <c r="Y60" s="109">
+        <f>AVERAGE(Y56:Y59)</f>
+        <v>4.3431622178276648</v>
+      </c>
+      <c r="Z60" s="110">
+        <f>AVERAGE(Z56:Z59)</f>
+        <v>0.91982344861369825</v>
+      </c>
+      <c r="AA60" s="111" cm="1">
+        <f t="array" ref="AA60">AVERAGE(ABS(AA56:AA59))</f>
+        <v>9.5</v>
+      </c>
+      <c r="AC60" s="14">
+        <v>2.5687105568278001</v>
+      </c>
+      <c r="AD60" s="14">
+        <v>4.1564176321666499</v>
+      </c>
+      <c r="AE60" s="14">
+        <v>0.89542968062926698</v>
+      </c>
+      <c r="AF60" s="14">
+        <v>12</v>
+      </c>
     </row>
     <row r="61" spans="2:75" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="150"/>
-      <c r="C61" s="146"/>
+      <c r="B61" s="169"/>
+      <c r="C61" s="159"/>
       <c r="D61" s="54" t="s">
         <v>3</v>
       </c>
@@ -11010,12 +11325,24 @@
         <v>195</v>
       </c>
       <c r="N61"/>
+      <c r="AC61" s="14">
+        <v>1.4237578110570199</v>
+      </c>
+      <c r="AD61" s="14">
+        <v>1.84851632832792</v>
+      </c>
+      <c r="AE61" s="14">
+        <v>0.94037969334473304</v>
+      </c>
+      <c r="AF61" s="14">
+        <v>-10</v>
+      </c>
     </row>
     <row r="62" spans="2:75" x14ac:dyDescent="0.2">
-      <c r="B62" s="144">
+      <c r="B62" s="157">
         <v>0</v>
       </c>
-      <c r="C62" s="144">
+      <c r="C62" s="157">
         <v>0.01</v>
       </c>
       <c r="D62" s="53" t="s">
@@ -11041,10 +11368,22 @@
         <v>196</v>
       </c>
       <c r="N62"/>
+      <c r="AC62" s="14">
+        <v>4.1331423251827397</v>
+      </c>
+      <c r="AD62" s="14">
+        <v>7.7586509468645399</v>
+      </c>
+      <c r="AE62" s="14">
+        <v>0.93867726209864499</v>
+      </c>
+      <c r="AF62" s="14">
+        <v>15</v>
+      </c>
     </row>
     <row r="63" spans="2:75" x14ac:dyDescent="0.2">
-      <c r="B63" s="145"/>
-      <c r="C63" s="145"/>
+      <c r="B63" s="158"/>
+      <c r="C63" s="158"/>
       <c r="D63" s="2" t="s">
         <v>2</v>
       </c>
@@ -11071,10 +11410,14 @@
         <v>190</v>
       </c>
       <c r="N63"/>
+      <c r="AC63" s="14"/>
+      <c r="AD63" s="14"/>
+      <c r="AE63" s="14"/>
+      <c r="AF63" s="14"/>
     </row>
     <row r="64" spans="2:75" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="146"/>
-      <c r="C64" s="146"/>
+      <c r="B64" s="159"/>
+      <c r="C64" s="159"/>
       <c r="D64" s="54" t="s">
         <v>3</v>
       </c>
@@ -11098,12 +11441,16 @@
         <v>197</v>
       </c>
       <c r="N64"/>
+      <c r="AC64" s="14"/>
+      <c r="AD64" s="14"/>
+      <c r="AE64" s="14"/>
+      <c r="AF64" s="14"/>
     </row>
     <row r="65" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B65" s="144">
+      <c r="B65" s="157">
         <v>0</v>
       </c>
-      <c r="C65" s="144">
+      <c r="C65" s="157">
         <v>0.1</v>
       </c>
       <c r="D65" s="53" t="s">
@@ -11131,8 +11478,8 @@
       <c r="N65"/>
     </row>
     <row r="66" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B66" s="145"/>
-      <c r="C66" s="145"/>
+      <c r="B66" s="158"/>
+      <c r="C66" s="158"/>
       <c r="D66" s="2" t="s">
         <v>2</v>
       </c>
@@ -11158,8 +11505,8 @@
       <c r="N66"/>
     </row>
     <row r="67" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="146"/>
-      <c r="C67" s="146"/>
+      <c r="B67" s="159"/>
+      <c r="C67" s="159"/>
       <c r="D67" s="54" t="s">
         <v>3</v>
       </c>
@@ -11188,10 +11535,10 @@
       <c r="N67"/>
     </row>
     <row r="68" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B68" s="144">
+      <c r="B68" s="157">
         <v>1E-3</v>
       </c>
-      <c r="C68" s="144">
+      <c r="C68" s="157">
         <v>0</v>
       </c>
       <c r="D68" s="53" t="s">
@@ -11219,8 +11566,8 @@
       <c r="N68"/>
     </row>
     <row r="69" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B69" s="145"/>
-      <c r="C69" s="145"/>
+      <c r="B69" s="158"/>
+      <c r="C69" s="158"/>
       <c r="D69" s="2" t="s">
         <v>2</v>
       </c>
@@ -11246,8 +11593,8 @@
       <c r="N69"/>
     </row>
     <row r="70" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="146"/>
-      <c r="C70" s="146"/>
+      <c r="B70" s="159"/>
+      <c r="C70" s="159"/>
       <c r="D70" s="54" t="s">
         <v>3</v>
       </c>
@@ -11274,10 +11621,10 @@
       <c r="O70" s="1"/>
     </row>
     <row r="71" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B71" s="144">
+      <c r="B71" s="157">
         <v>1E-3</v>
       </c>
-      <c r="C71" s="144">
+      <c r="C71" s="157">
         <v>1E-3</v>
       </c>
       <c r="D71" s="53" t="s">
@@ -11309,8 +11656,8 @@
       <c r="O71" s="1"/>
     </row>
     <row r="72" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B72" s="145"/>
-      <c r="C72" s="145"/>
+      <c r="B72" s="158"/>
+      <c r="C72" s="158"/>
       <c r="D72" s="2" t="s">
         <v>2</v>
       </c>
@@ -11337,8 +11684,8 @@
       <c r="O72" s="1"/>
     </row>
     <row r="73" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="146"/>
-      <c r="C73" s="146"/>
+      <c r="B73" s="159"/>
+      <c r="C73" s="159"/>
       <c r="D73" s="54" t="s">
         <v>3</v>
       </c>
@@ -11366,10 +11713,10 @@
       <c r="S73" s="1"/>
     </row>
     <row r="74" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B74" s="144">
+      <c r="B74" s="157">
         <v>1E-3</v>
       </c>
-      <c r="C74" s="144">
+      <c r="C74" s="157">
         <v>0.01</v>
       </c>
       <c r="D74" s="53" t="s">
@@ -11398,8 +11745,8 @@
       <c r="O74" s="1"/>
     </row>
     <row r="75" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B75" s="145"/>
-      <c r="C75" s="145"/>
+      <c r="B75" s="158"/>
+      <c r="C75" s="158"/>
       <c r="D75" s="2" t="s">
         <v>2</v>
       </c>
@@ -11422,8 +11769,8 @@
       <c r="N75"/>
     </row>
     <row r="76" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="146"/>
-      <c r="C76" s="146"/>
+      <c r="B76" s="159"/>
+      <c r="C76" s="159"/>
       <c r="D76" s="54" t="s">
         <v>3</v>
       </c>
@@ -11446,10 +11793,10 @@
       <c r="N76"/>
     </row>
     <row r="77" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B77" s="144">
+      <c r="B77" s="157">
         <v>1E-3</v>
       </c>
-      <c r="C77" s="144">
+      <c r="C77" s="157">
         <v>0.1</v>
       </c>
       <c r="D77" s="53" t="s">
@@ -11474,8 +11821,8 @@
       <c r="N77"/>
     </row>
     <row r="78" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B78" s="145"/>
-      <c r="C78" s="145"/>
+      <c r="B78" s="158"/>
+      <c r="C78" s="158"/>
       <c r="D78" s="2" t="s">
         <v>2</v>
       </c>
@@ -11498,8 +11845,8 @@
       <c r="N78"/>
     </row>
     <row r="79" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="146"/>
-      <c r="C79" s="146"/>
+      <c r="B79" s="159"/>
+      <c r="C79" s="159"/>
       <c r="D79" s="54" t="s">
         <v>3</v>
       </c>
@@ -11522,10 +11869,10 @@
       <c r="N79"/>
     </row>
     <row r="80" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B80" s="144">
+      <c r="B80" s="157">
         <v>0.01</v>
       </c>
-      <c r="C80" s="144">
+      <c r="C80" s="157">
         <v>0</v>
       </c>
       <c r="D80" s="53" t="s">
@@ -11550,8 +11897,8 @@
       <c r="N80"/>
     </row>
     <row r="81" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B81" s="145"/>
-      <c r="C81" s="145"/>
+      <c r="B81" s="158"/>
+      <c r="C81" s="158"/>
       <c r="D81" s="2" t="s">
         <v>2</v>
       </c>
@@ -11574,8 +11921,8 @@
       <c r="N81"/>
     </row>
     <row r="82" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="146"/>
-      <c r="C82" s="146"/>
+      <c r="B82" s="159"/>
+      <c r="C82" s="159"/>
       <c r="D82" s="54" t="s">
         <v>3</v>
       </c>
@@ -11598,10 +11945,10 @@
       <c r="N82"/>
     </row>
     <row r="83" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B83" s="144">
+      <c r="B83" s="157">
         <v>0.01</v>
       </c>
-      <c r="C83" s="144">
+      <c r="C83" s="157">
         <v>1E-3</v>
       </c>
       <c r="D83" s="53" t="s">
@@ -11626,8 +11973,8 @@
       <c r="N83"/>
     </row>
     <row r="84" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B84" s="145"/>
-      <c r="C84" s="145"/>
+      <c r="B84" s="158"/>
+      <c r="C84" s="158"/>
       <c r="D84" s="2" t="s">
         <v>2</v>
       </c>
@@ -11650,8 +11997,8 @@
       <c r="N84"/>
     </row>
     <row r="85" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="146"/>
-      <c r="C85" s="146"/>
+      <c r="B85" s="159"/>
+      <c r="C85" s="159"/>
       <c r="D85" s="54" t="s">
         <v>3</v>
       </c>
@@ -11674,10 +12021,10 @@
       <c r="N85"/>
     </row>
     <row r="86" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B86" s="144">
+      <c r="B86" s="157">
         <v>0.01</v>
       </c>
-      <c r="C86" s="144">
+      <c r="C86" s="157">
         <v>0.01</v>
       </c>
       <c r="D86" s="53" t="s">
@@ -11702,8 +12049,8 @@
       <c r="N86"/>
     </row>
     <row r="87" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B87" s="145"/>
-      <c r="C87" s="145"/>
+      <c r="B87" s="158"/>
+      <c r="C87" s="158"/>
       <c r="D87" s="2" t="s">
         <v>2</v>
       </c>
@@ -11726,8 +12073,8 @@
       <c r="N87"/>
     </row>
     <row r="88" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="146"/>
-      <c r="C88" s="146"/>
+      <c r="B88" s="159"/>
+      <c r="C88" s="159"/>
       <c r="D88" s="54" t="s">
         <v>3</v>
       </c>
@@ -11750,10 +12097,10 @@
       <c r="N88"/>
     </row>
     <row r="89" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B89" s="144">
+      <c r="B89" s="157">
         <v>0.01</v>
       </c>
-      <c r="C89" s="144">
+      <c r="C89" s="157">
         <v>0.1</v>
       </c>
       <c r="D89" s="53" t="s">
@@ -11778,8 +12125,8 @@
       <c r="N89"/>
     </row>
     <row r="90" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B90" s="145"/>
-      <c r="C90" s="145"/>
+      <c r="B90" s="158"/>
+      <c r="C90" s="158"/>
       <c r="D90" s="2" t="s">
         <v>2</v>
       </c>
@@ -11802,8 +12149,8 @@
       <c r="N90"/>
     </row>
     <row r="91" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="146"/>
-      <c r="C91" s="146"/>
+      <c r="B91" s="159"/>
+      <c r="C91" s="159"/>
       <c r="D91" s="54" t="s">
         <v>3</v>
       </c>
@@ -11826,10 +12173,10 @@
       <c r="N91"/>
     </row>
     <row r="92" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B92" s="144">
+      <c r="B92" s="157">
         <v>0.1</v>
       </c>
-      <c r="C92" s="144">
+      <c r="C92" s="157">
         <v>0</v>
       </c>
       <c r="D92" s="53" t="s">
@@ -11854,8 +12201,8 @@
       <c r="N92"/>
     </row>
     <row r="93" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B93" s="145"/>
-      <c r="C93" s="145"/>
+      <c r="B93" s="158"/>
+      <c r="C93" s="158"/>
       <c r="D93" s="2" t="s">
         <v>2</v>
       </c>
@@ -11877,8 +12224,8 @@
       </c>
     </row>
     <row r="94" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="146"/>
-      <c r="C94" s="146"/>
+      <c r="B94" s="159"/>
+      <c r="C94" s="159"/>
       <c r="D94" s="54" t="s">
         <v>3</v>
       </c>
@@ -11900,10 +12247,10 @@
       </c>
     </row>
     <row r="95" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B95" s="144">
+      <c r="B95" s="157">
         <v>0.1</v>
       </c>
-      <c r="C95" s="144">
+      <c r="C95" s="157">
         <v>1E-3</v>
       </c>
       <c r="D95" s="53" t="s">
@@ -11927,8 +12274,8 @@
       </c>
     </row>
     <row r="96" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B96" s="145"/>
-      <c r="C96" s="145"/>
+      <c r="B96" s="158"/>
+      <c r="C96" s="158"/>
       <c r="D96" s="2" t="s">
         <v>2</v>
       </c>
@@ -11950,8 +12297,8 @@
       </c>
     </row>
     <row r="97" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="146"/>
-      <c r="C97" s="146"/>
+      <c r="B97" s="159"/>
+      <c r="C97" s="159"/>
       <c r="D97" s="54" t="s">
         <v>3</v>
       </c>
@@ -11973,10 +12320,10 @@
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B98" s="144">
+      <c r="B98" s="157">
         <v>0.1</v>
       </c>
-      <c r="C98" s="144">
+      <c r="C98" s="157">
         <v>0.01</v>
       </c>
       <c r="D98" s="53" t="s">
@@ -12000,8 +12347,8 @@
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B99" s="145"/>
-      <c r="C99" s="145"/>
+      <c r="B99" s="158"/>
+      <c r="C99" s="158"/>
       <c r="D99" s="2" t="s">
         <v>2</v>
       </c>
@@ -12023,8 +12370,8 @@
       </c>
     </row>
     <row r="100" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="146"/>
-      <c r="C100" s="146"/>
+      <c r="B100" s="159"/>
+      <c r="C100" s="159"/>
       <c r="D100" s="54" t="s">
         <v>3</v>
       </c>
@@ -12046,10 +12393,10 @@
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B101" s="144">
+      <c r="B101" s="157">
         <v>0.1</v>
       </c>
-      <c r="C101" s="144">
+      <c r="C101" s="157">
         <v>0.1</v>
       </c>
       <c r="D101" s="53" t="s">
@@ -12073,8 +12420,8 @@
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B102" s="145"/>
-      <c r="C102" s="145"/>
+      <c r="B102" s="158"/>
+      <c r="C102" s="158"/>
       <c r="D102" s="2" t="s">
         <v>2</v>
       </c>
@@ -12096,8 +12443,8 @@
       </c>
     </row>
     <row r="103" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="146"/>
-      <c r="C103" s="146"/>
+      <c r="B103" s="159"/>
+      <c r="C103" s="159"/>
       <c r="D103" s="54" t="s">
         <v>3</v>
       </c>
@@ -12120,24 +12467,37 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="V29:V33"/>
-    <mergeCell ref="V34:V38"/>
-    <mergeCell ref="V39:V43"/>
-    <mergeCell ref="V44:W44"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="B40:B51"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="C62:C64"/>
+    <mergeCell ref="AF26:AM26"/>
+    <mergeCell ref="X27:AA27"/>
+    <mergeCell ref="AB27:AE27"/>
+    <mergeCell ref="AF27:AI27"/>
+    <mergeCell ref="AJ27:AM27"/>
+    <mergeCell ref="X26:AE26"/>
+    <mergeCell ref="J26:N26"/>
+    <mergeCell ref="O26:S26"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="B28:B39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="B4:B15"/>
+    <mergeCell ref="O2:S2"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="C89:C91"/>
+    <mergeCell ref="C92:C94"/>
+    <mergeCell ref="C95:C97"/>
+    <mergeCell ref="C98:C100"/>
+    <mergeCell ref="C71:C73"/>
+    <mergeCell ref="C74:C76"/>
+    <mergeCell ref="C77:C79"/>
+    <mergeCell ref="C80:C82"/>
+    <mergeCell ref="C83:C85"/>
     <mergeCell ref="C101:C103"/>
     <mergeCell ref="B62:B64"/>
     <mergeCell ref="B65:B67"/>
@@ -12154,49 +12514,37 @@
     <mergeCell ref="B98:B100"/>
     <mergeCell ref="B101:B103"/>
     <mergeCell ref="C86:C88"/>
-    <mergeCell ref="C89:C91"/>
-    <mergeCell ref="C92:C94"/>
-    <mergeCell ref="C95:C97"/>
-    <mergeCell ref="C98:C100"/>
-    <mergeCell ref="C71:C73"/>
-    <mergeCell ref="C74:C76"/>
-    <mergeCell ref="C77:C79"/>
-    <mergeCell ref="C80:C82"/>
-    <mergeCell ref="C83:C85"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="B4:B15"/>
-    <mergeCell ref="O2:S2"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:N2"/>
-    <mergeCell ref="J26:N26"/>
-    <mergeCell ref="O26:S26"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="B28:B39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="AF26:AM26"/>
-    <mergeCell ref="X27:AA27"/>
-    <mergeCell ref="AB27:AE27"/>
-    <mergeCell ref="AF27:AI27"/>
-    <mergeCell ref="AJ27:AM27"/>
-    <mergeCell ref="X26:AE26"/>
+    <mergeCell ref="C68:C70"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="B40:B51"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="C56:C58"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="C62:C64"/>
+    <mergeCell ref="V29:V33"/>
+    <mergeCell ref="V34:V38"/>
+    <mergeCell ref="V39:V43"/>
+    <mergeCell ref="V44:W44"/>
+    <mergeCell ref="C65:C67"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AFB687B-AE8A-9E4C-93B1-A2032A687EEF}">
-  <dimension ref="C4:Y58"/>
+  <dimension ref="C4:Y55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21:M25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12208,37 +12556,37 @@
   <sheetData>
     <row r="4" spans="3:25" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="3:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="X5" s="172" t="s">
+      <c r="X5" s="137" t="s">
         <v>235</v>
       </c>
-      <c r="Y5" s="173" t="s">
+      <c r="Y5" s="138" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="6" spans="3:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C6" s="13"/>
-      <c r="F6" s="128" t="s">
+      <c r="F6" s="171" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="129"/>
-      <c r="H6" s="129"/>
-      <c r="I6" s="129"/>
-      <c r="J6" s="130"/>
-      <c r="K6" s="128" t="s">
+      <c r="G6" s="172"/>
+      <c r="H6" s="172"/>
+      <c r="I6" s="172"/>
+      <c r="J6" s="173"/>
+      <c r="K6" s="171" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="129"/>
-      <c r="M6" s="129"/>
-      <c r="N6" s="129"/>
-      <c r="O6" s="130"/>
-      <c r="P6" s="128" t="s">
+      <c r="L6" s="172"/>
+      <c r="M6" s="172"/>
+      <c r="N6" s="172"/>
+      <c r="O6" s="173"/>
+      <c r="P6" s="171" t="s">
         <v>12</v>
       </c>
-      <c r="Q6" s="129"/>
-      <c r="R6" s="129"/>
-      <c r="S6" s="129"/>
-      <c r="T6" s="130"/>
-      <c r="U6" s="141" t="s">
+      <c r="Q6" s="172"/>
+      <c r="R6" s="172"/>
+      <c r="S6" s="172"/>
+      <c r="T6" s="173"/>
+      <c r="U6" s="174" t="s">
         <v>9</v>
       </c>
       <c r="X6" s="121" t="s">
@@ -12295,7 +12643,7 @@
       <c r="T7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="U7" s="141"/>
+      <c r="U7" s="174"/>
       <c r="X7" s="122" t="s">
         <v>212</v>
       </c>
@@ -12304,10 +12652,10 @@
       </c>
     </row>
     <row r="8" spans="3:25" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="140" t="s">
+      <c r="C8" s="170" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="131" t="s">
+      <c r="D8" s="160" t="s">
         <v>210</v>
       </c>
       <c r="E8" s="53" t="s">
@@ -12373,8 +12721,8 @@
       </c>
     </row>
     <row r="9" spans="3:25" x14ac:dyDescent="0.2">
-      <c r="C9" s="140"/>
-      <c r="D9" s="132"/>
+      <c r="C9" s="170"/>
+      <c r="D9" s="161"/>
       <c r="E9" s="2" t="s">
         <v>2</v>
       </c>
@@ -12438,8 +12786,8 @@
       </c>
     </row>
     <row r="10" spans="3:25" x14ac:dyDescent="0.2">
-      <c r="C10" s="140"/>
-      <c r="D10" s="132"/>
+      <c r="C10" s="170"/>
+      <c r="D10" s="161"/>
       <c r="E10" s="2" t="s">
         <v>3</v>
       </c>
@@ -12498,13 +12846,13 @@
       <c r="X10" s="122" t="s">
         <v>234</v>
       </c>
-      <c r="Y10" s="174" t="b">
+      <c r="Y10" s="139" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="3:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="140"/>
-      <c r="D11" s="133"/>
+      <c r="C11" s="170"/>
+      <c r="D11" s="162"/>
       <c r="E11" s="54" t="s">
         <v>211</v>
       </c>
@@ -12568,8 +12916,8 @@
       </c>
     </row>
     <row r="12" spans="3:25" x14ac:dyDescent="0.2">
-      <c r="C12" s="140"/>
-      <c r="D12" s="131" t="s">
+      <c r="C12" s="170"/>
+      <c r="D12" s="160" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="53" t="s">
@@ -12635,8 +12983,8 @@
       </c>
     </row>
     <row r="13" spans="3:25" x14ac:dyDescent="0.2">
-      <c r="C13" s="140"/>
-      <c r="D13" s="132"/>
+      <c r="C13" s="170"/>
+      <c r="D13" s="161"/>
       <c r="E13" s="2" t="s">
         <v>2</v>
       </c>
@@ -12700,7 +13048,7 @@
       </c>
     </row>
     <row r="14" spans="3:25" x14ac:dyDescent="0.2">
-      <c r="D14" s="132"/>
+      <c r="D14" s="161"/>
       <c r="E14" s="2" t="s">
         <v>3</v>
       </c>
@@ -12764,7 +13112,7 @@
       </c>
     </row>
     <row r="15" spans="3:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="133"/>
+      <c r="D15" s="162"/>
       <c r="E15" s="50" t="s">
         <v>211</v>
       </c>
@@ -12836,21 +13184,31 @@
       </c>
     </row>
     <row r="18" spans="4:22" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="4:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D19" s="158"/>
-      <c r="E19" s="158"/>
-      <c r="F19" s="131" t="s">
+    <row r="19" spans="4:22" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="129"/>
+      <c r="E19" s="129"/>
+      <c r="F19" s="160" t="s">
         <v>218</v>
       </c>
-      <c r="G19" s="160"/>
-      <c r="H19" s="160"/>
-      <c r="I19" s="164"/>
-      <c r="J19" s="160" t="s">
+      <c r="G19" s="185"/>
+      <c r="H19" s="185"/>
+      <c r="I19" s="186"/>
+      <c r="J19" s="185" t="s">
         <v>217</v>
       </c>
-      <c r="K19" s="160"/>
-      <c r="L19" s="160"/>
-      <c r="M19" s="161"/>
+      <c r="K19" s="185"/>
+      <c r="L19" s="185"/>
+      <c r="M19" s="187"/>
+      <c r="N19" s="160" t="s">
+        <v>236</v>
+      </c>
+      <c r="O19" s="185"/>
+      <c r="P19" s="185"/>
+      <c r="Q19" s="186"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="14"/>
+      <c r="U19" s="14"/>
     </row>
     <row r="20" spans="4:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D20" s="97" t="s">
@@ -12868,7 +13226,7 @@
       <c r="H20" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="I20" s="186" t="s">
+      <c r="I20" s="150" t="s">
         <v>211</v>
       </c>
       <c r="J20" s="98" t="s">
@@ -12883,25 +13241,41 @@
       <c r="M20" s="100" t="s">
         <v>211</v>
       </c>
+      <c r="N20" s="97" t="s">
+        <v>1</v>
+      </c>
+      <c r="O20" s="98" t="s">
+        <v>2</v>
+      </c>
+      <c r="P20" s="98" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="150" t="s">
+        <v>211</v>
+      </c>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
+      <c r="U20" s="14"/>
     </row>
     <row r="21" spans="4:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D21" s="151">
+      <c r="D21" s="152">
         <v>7</v>
       </c>
-      <c r="E21" s="159" t="s">
+      <c r="E21" s="130" t="s">
         <v>0</v>
       </c>
       <c r="F21" s="107">
-        <v>1.88859227383446</v>
-      </c>
-      <c r="G21" s="165">
-        <v>2.59165720584447</v>
-      </c>
-      <c r="H21" s="165">
-        <v>0.92528922808715897</v>
-      </c>
-      <c r="I21" s="175">
-        <v>-2</v>
+        <v>1.9564223092324899</v>
+      </c>
+      <c r="G21" s="131">
+        <v>2.7898785700676898</v>
+      </c>
+      <c r="H21" s="131">
+        <v>0.93519973480315999</v>
+      </c>
+      <c r="I21" s="140">
+        <v>-3</v>
       </c>
       <c r="J21" s="114">
         <v>1.3953039029454499</v>
@@ -12915,201 +13289,184 @@
       <c r="M21" s="115">
         <v>-8</v>
       </c>
-      <c r="O21" s="14">
-        <v>1.3953039029454499</v>
-      </c>
-      <c r="P21" s="14">
-        <v>1.43611328003703</v>
-      </c>
-      <c r="Q21" s="14">
-        <v>1.43662992745592</v>
-      </c>
-      <c r="R21" s="14">
-        <v>2.64327513122756</v>
-      </c>
+      <c r="N21" s="133">
+        <v>2.9512770024242001</v>
+      </c>
+      <c r="O21" s="133">
+        <v>4.3127364592540296</v>
+      </c>
+      <c r="P21" s="133">
+        <v>0.86352584150675904</v>
+      </c>
+      <c r="Q21" s="115">
+        <v>-8</v>
+      </c>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
+      <c r="T21" s="14"/>
+      <c r="U21" s="14"/>
     </row>
     <row r="22" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D22" s="152"/>
+      <c r="D22" s="153"/>
       <c r="E22" s="6" t="s">
         <v>6</v>
       </c>
       <c r="F22" s="107">
-        <v>2.4394765425882001</v>
-      </c>
-      <c r="G22" s="165">
-        <v>3.6985519699639902</v>
-      </c>
-      <c r="H22" s="165">
-        <v>0.91731307019144204</v>
-      </c>
-      <c r="I22" s="176">
+        <v>2.4302778542036299</v>
+      </c>
+      <c r="G22" s="131">
+        <v>3.7246070271155398</v>
+      </c>
+      <c r="H22" s="131">
+        <v>0.92083933133732099</v>
+      </c>
+      <c r="I22" s="141">
         <v>17</v>
       </c>
-      <c r="J22" s="166">
+      <c r="J22" s="132">
         <v>1.43611328003703</v>
       </c>
-      <c r="K22" s="166">
+      <c r="K22" s="132">
         <v>2.1674456180120298</v>
       </c>
-      <c r="L22" s="166">
+      <c r="L22" s="132">
         <v>0.94566824672413197</v>
       </c>
       <c r="M22" s="108">
         <v>5</v>
       </c>
-      <c r="O22" s="14">
-        <v>2.2410296522764201</v>
-      </c>
-      <c r="P22" s="14">
-        <v>2.1674456180120298</v>
-      </c>
-      <c r="Q22" s="14">
-        <v>2.3696005644861899</v>
-      </c>
-      <c r="R22" s="14">
-        <v>4.6866517625012403</v>
-      </c>
-      <c r="S22" s="14">
-        <v>1.3953039029454499</v>
-      </c>
-      <c r="T22" s="14">
-        <v>2.2410296522764201</v>
-      </c>
-      <c r="U22" s="14">
-        <v>0.95539454820134895</v>
-      </c>
-      <c r="V22" s="14">
-        <v>-8</v>
-      </c>
+      <c r="N22" s="131">
+        <v>2.6259942309225002</v>
+      </c>
+      <c r="O22" s="131">
+        <v>4.0622906378416799</v>
+      </c>
+      <c r="P22" s="131">
+        <v>0.91021773196631095</v>
+      </c>
+      <c r="Q22" s="103">
+        <v>17</v>
+      </c>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
+      <c r="T22" s="14"/>
+      <c r="U22" s="14"/>
+      <c r="V22" s="14"/>
     </row>
     <row r="23" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D23" s="152"/>
+      <c r="D23" s="153"/>
       <c r="E23" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F23" s="104">
-        <v>1.2464504398454599</v>
-      </c>
-      <c r="G23" s="166">
-        <v>1.52064727305979</v>
-      </c>
-      <c r="H23" s="166">
-        <v>0.96607855073938698</v>
-      </c>
-      <c r="I23" s="175">
-        <v>-17</v>
-      </c>
-      <c r="J23" s="165">
+        <v>1.18227722221772</v>
+      </c>
+      <c r="G23" s="132">
+        <v>1.4563743635887201</v>
+      </c>
+      <c r="H23" s="132">
+        <v>0.96987730378416304</v>
+      </c>
+      <c r="I23" s="140">
+        <v>-18</v>
+      </c>
+      <c r="J23" s="131">
         <v>1.43662992745592</v>
       </c>
-      <c r="K23" s="165">
+      <c r="K23" s="131">
         <v>2.3696005644861899</v>
       </c>
-      <c r="L23" s="165">
+      <c r="L23" s="131">
         <v>0.925151573702932</v>
       </c>
       <c r="M23" s="103">
         <v>-21</v>
       </c>
-      <c r="O23" s="14">
-        <v>0.95539454820134895</v>
-      </c>
-      <c r="P23" s="14">
-        <v>0.94566824672413197</v>
-      </c>
-      <c r="Q23" s="14">
-        <v>0.925151573702932</v>
-      </c>
-      <c r="R23" s="14">
-        <v>0.97624377007180496</v>
-      </c>
-      <c r="S23" s="14">
-        <v>1.43611328003703</v>
-      </c>
-      <c r="T23" s="14">
-        <v>2.1674456180120298</v>
-      </c>
-      <c r="U23" s="14">
-        <v>0.94566824672413197</v>
-      </c>
-      <c r="V23" s="14">
-        <v>5</v>
-      </c>
+      <c r="N23" s="131">
+        <v>1.50589329905638</v>
+      </c>
+      <c r="O23" s="131">
+        <v>2.0698032495027499</v>
+      </c>
+      <c r="P23" s="131">
+        <v>0.96135869199740298</v>
+      </c>
+      <c r="Q23" s="103">
+        <v>-17</v>
+      </c>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
+      <c r="T23" s="14"/>
+      <c r="U23" s="14"/>
+      <c r="V23" s="14"/>
     </row>
     <row r="24" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D24" s="152"/>
+      <c r="D24" s="153"/>
       <c r="E24" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F24" s="107">
-        <v>3.1531473150135501</v>
-      </c>
-      <c r="G24" s="165">
-        <v>5.4298722955533503</v>
-      </c>
-      <c r="H24" s="166">
-        <v>0.97967690834607302</v>
-      </c>
-      <c r="I24" s="176">
+        <v>3.3324126233429401</v>
+      </c>
+      <c r="G24" s="131">
+        <v>5.9976397930397898</v>
+      </c>
+      <c r="H24" s="132">
+        <v>0.98191973538189703</v>
+      </c>
+      <c r="I24" s="141">
         <v>9</v>
       </c>
-      <c r="J24" s="166">
+      <c r="J24" s="132">
         <v>2.64327513122756</v>
       </c>
-      <c r="K24" s="166">
+      <c r="K24" s="132">
         <v>4.6866517625012403</v>
       </c>
-      <c r="L24" s="165">
+      <c r="L24" s="131">
         <v>0.97624377007180496</v>
       </c>
       <c r="M24" s="108">
         <v>1</v>
       </c>
-      <c r="O24" s="14">
-        <v>-8</v>
-      </c>
-      <c r="P24" s="14">
-        <v>5</v>
-      </c>
-      <c r="Q24" s="14">
-        <v>-21</v>
-      </c>
-      <c r="R24" s="14">
-        <v>1</v>
-      </c>
-      <c r="S24" s="14">
-        <v>1.43662992745592</v>
-      </c>
-      <c r="T24" s="14">
-        <v>2.3696005644861899</v>
-      </c>
-      <c r="U24" s="14">
-        <v>0.925151573702932</v>
-      </c>
-      <c r="V24" s="14">
-        <v>-21</v>
-      </c>
+      <c r="N24" s="131">
+        <v>3.5480996358027301</v>
+      </c>
+      <c r="O24" s="131">
+        <v>5.8785085877251104</v>
+      </c>
+      <c r="P24" s="131">
+        <v>0.973848575563387</v>
+      </c>
+      <c r="Q24" s="103">
+        <v>10</v>
+      </c>
+      <c r="R24" s="14"/>
+      <c r="S24" s="14"/>
+      <c r="T24" s="14"/>
+      <c r="U24" s="14"/>
+      <c r="V24" s="14"/>
     </row>
     <row r="25" spans="4:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D25" s="153"/>
-      <c r="E25" s="156" t="s">
+      <c r="D25" s="154"/>
+      <c r="E25" s="127" t="s">
         <v>9</v>
       </c>
       <c r="F25" s="112">
         <f>AVERAGE(F21:F24)</f>
-        <v>2.1819166428204175</v>
+        <v>2.2253475022491949</v>
       </c>
       <c r="G25" s="109">
         <f>AVERAGE(G21:G24)</f>
-        <v>3.3101821861054002</v>
-      </c>
-      <c r="H25" s="109">
+        <v>3.4921249384529349</v>
+      </c>
+      <c r="H25" s="110">
         <f>AVERAGE(H21:H24)</f>
-        <v>0.9470894393410153</v>
-      </c>
-      <c r="I25" s="188" cm="1">
+        <v>0.95195902632663532</v>
+      </c>
+      <c r="I25" s="151" cm="1">
         <f t="array" ref="I25">AVERAGE(ABS(I21:I24))</f>
-        <v>11.25</v>
+        <v>11.75</v>
       </c>
       <c r="J25" s="110">
         <f>AVERAGE(J21:J24)</f>
@@ -13123,40 +13480,49 @@
         <f>AVERAGE(L21:L24)</f>
         <v>0.95061453467505452</v>
       </c>
-      <c r="M25" s="181" cm="1">
+      <c r="M25" s="146" cm="1">
         <f t="array" ref="M25">AVERAGE(ABS(M21:M24))</f>
         <v>8.75</v>
       </c>
-      <c r="S25" s="14">
-        <v>2.64327513122756</v>
-      </c>
-      <c r="T25" s="14">
-        <v>4.6866517625012403</v>
-      </c>
-      <c r="U25" s="14">
-        <v>0.97624377007180496</v>
-      </c>
-      <c r="V25" s="14">
-        <v>1</v>
-      </c>
+      <c r="N25" s="109">
+        <f>AVERAGE(N21:N24)</f>
+        <v>2.6578160420514525</v>
+      </c>
+      <c r="O25" s="109">
+        <f>AVERAGE(O21:O24)</f>
+        <v>4.0808347335808923</v>
+      </c>
+      <c r="P25" s="109">
+        <f>AVERAGE(P21:P24)</f>
+        <v>0.92723771025846502</v>
+      </c>
+      <c r="Q25" s="111" cm="1">
+        <f t="array" ref="Q25">AVERAGE(ABS(Q21:Q24))</f>
+        <v>13</v>
+      </c>
+      <c r="R25" s="14"/>
+      <c r="S25" s="14"/>
+      <c r="T25" s="14"/>
+      <c r="U25" s="14"/>
+      <c r="V25" s="14"/>
     </row>
     <row r="26" spans="4:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D26" s="151">
+      <c r="D26" s="152">
         <v>14</v>
       </c>
-      <c r="E26" s="159" t="s">
+      <c r="E26" s="130" t="s">
         <v>0</v>
       </c>
-      <c r="F26" s="167">
-        <v>2.20488301676775</v>
-      </c>
-      <c r="G26" s="168">
-        <v>3.2013188394651602</v>
-      </c>
-      <c r="H26" s="168">
-        <v>0.86211416571558996</v>
-      </c>
-      <c r="I26" s="178">
+      <c r="F26" s="107">
+        <v>2.2015640480718801</v>
+      </c>
+      <c r="G26" s="131">
+        <v>3.21185429999632</v>
+      </c>
+      <c r="H26" s="131">
+        <v>0.87748009004939498</v>
+      </c>
+      <c r="I26" s="140">
         <v>-1</v>
       </c>
       <c r="J26" s="114">
@@ -13168,120 +13534,220 @@
       <c r="L26" s="114">
         <v>0.94835615230597603</v>
       </c>
-      <c r="M26" s="180">
+      <c r="M26" s="145">
         <v>-1</v>
       </c>
+      <c r="N26" s="133">
+        <v>2.08940999846627</v>
+      </c>
+      <c r="O26" s="133">
+        <v>3.03673428906832</v>
+      </c>
+      <c r="P26" s="133">
+        <v>0.86824773134951405</v>
+      </c>
+      <c r="Q26" s="115">
+        <v>-1</v>
+      </c>
+      <c r="R26" s="14"/>
+      <c r="S26" s="14">
+        <v>2.9577961416509502</v>
+      </c>
+      <c r="T26" s="14">
+        <v>3.6086103265852998</v>
+      </c>
+      <c r="U26" s="14">
+        <v>2.29420340487271</v>
+      </c>
+      <c r="V26" s="14">
+        <v>5.0369887593202503</v>
+      </c>
     </row>
     <row r="27" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D27" s="152"/>
+      <c r="D27" s="153"/>
       <c r="E27" s="6" t="s">
         <v>6</v>
       </c>
       <c r="F27" s="107">
-        <v>2.5948577687192298</v>
-      </c>
-      <c r="G27" s="165">
-        <v>3.9865014193878601</v>
-      </c>
-      <c r="H27" s="165">
-        <v>0.85984276104255097</v>
-      </c>
-      <c r="I27" s="175">
+        <v>2.6121105803018101</v>
+      </c>
+      <c r="G27" s="131">
+        <v>4.1363807396934504</v>
+      </c>
+      <c r="H27" s="131">
+        <v>0.87245432969783698</v>
+      </c>
+      <c r="I27" s="140">
         <v>12</v>
       </c>
-      <c r="J27" s="166">
+      <c r="J27" s="132">
         <v>1.80342525350414</v>
       </c>
-      <c r="K27" s="166">
+      <c r="K27" s="132">
         <v>3.0195471174164301</v>
       </c>
-      <c r="L27" s="166">
+      <c r="L27" s="132">
         <v>0.90035813444998203</v>
       </c>
       <c r="M27" s="103">
         <v>-50</v>
       </c>
+      <c r="N27" s="131">
+        <v>2.59341289774882</v>
+      </c>
+      <c r="O27" s="131">
+        <v>3.9283370715763701</v>
+      </c>
+      <c r="P27" s="131">
+        <v>0.82727861848427597</v>
+      </c>
+      <c r="Q27" s="103">
+        <v>24</v>
+      </c>
+      <c r="R27" s="14"/>
+      <c r="S27" s="14">
+        <v>4.3657949130589202</v>
+      </c>
+      <c r="T27" s="14">
+        <v>5.4770218720708899</v>
+      </c>
+      <c r="U27" s="14">
+        <v>2.8968259156070699</v>
+      </c>
+      <c r="V27" s="14">
+        <v>9.1738224310701302</v>
+      </c>
     </row>
     <row r="28" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D28" s="152"/>
+      <c r="D28" s="153"/>
       <c r="E28" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F28" s="107">
-        <v>1.6361221877885901</v>
-      </c>
-      <c r="G28" s="166">
-        <v>1.9751604258767701</v>
-      </c>
-      <c r="H28" s="165">
-        <v>0.93683635929012099</v>
-      </c>
-      <c r="I28" s="175">
-        <v>-13</v>
-      </c>
-      <c r="J28" s="166">
+        <v>1.4230237455358901</v>
+      </c>
+      <c r="G28" s="132">
+        <v>1.79986332618016</v>
+      </c>
+      <c r="H28" s="132">
+        <v>0.94216001326646603</v>
+      </c>
+      <c r="I28" s="140">
+        <v>-11</v>
+      </c>
+      <c r="J28" s="132">
         <v>1.3021965625966001</v>
       </c>
-      <c r="K28" s="165">
+      <c r="K28" s="131">
         <v>2.0263847559545098</v>
       </c>
-      <c r="L28" s="166">
+      <c r="L28" s="131">
         <v>0.94134036018612899</v>
       </c>
       <c r="M28" s="103">
         <v>-19</v>
       </c>
+      <c r="N28" s="131">
+        <v>2.16553174994056</v>
+      </c>
+      <c r="O28" s="131">
+        <v>2.68736298828924</v>
+      </c>
+      <c r="P28" s="131">
+        <v>0.93198970183851204</v>
+      </c>
+      <c r="Q28" s="103">
+        <v>-12</v>
+      </c>
+      <c r="R28" s="14"/>
+      <c r="S28" s="14">
+        <v>0.71245087138951502</v>
+      </c>
+      <c r="T28" s="14">
+        <v>0.62210520724011198</v>
+      </c>
+      <c r="U28" s="14">
+        <v>0.86830984627044105</v>
+      </c>
+      <c r="V28" s="14">
+        <v>0.81204631699589402</v>
+      </c>
     </row>
     <row r="29" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D29" s="152"/>
+      <c r="D29" s="153"/>
       <c r="E29" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F29" s="107">
-        <v>3.7660561565634199</v>
-      </c>
-      <c r="G29" s="165">
-        <v>6.88452412655153</v>
-      </c>
-      <c r="H29" s="165">
-        <v>0.92598361339384805</v>
-      </c>
-      <c r="I29" s="176">
-        <v>16</v>
-      </c>
-      <c r="J29" s="166">
+        <v>3.8615626660905198</v>
+      </c>
+      <c r="G29" s="131">
+        <v>7.1237079074965699</v>
+      </c>
+      <c r="H29" s="132">
+        <v>0.93352159047577898</v>
+      </c>
+      <c r="I29" s="141">
+        <v>15</v>
+      </c>
+      <c r="J29" s="132">
         <v>3.42516909127299</v>
       </c>
-      <c r="K29" s="166">
+      <c r="K29" s="132">
         <v>6.3432324244527498</v>
       </c>
-      <c r="L29" s="166">
+      <c r="L29" s="132">
         <v>0.96568338875711102</v>
       </c>
       <c r="M29" s="108">
         <v>12</v>
       </c>
+      <c r="N29" s="131">
+        <v>3.0913191031952398</v>
+      </c>
+      <c r="O29" s="131">
+        <v>5.4776606910288299</v>
+      </c>
+      <c r="P29" s="131">
+        <v>0.93035650943687997</v>
+      </c>
+      <c r="Q29" s="103">
+        <v>15</v>
+      </c>
+      <c r="R29" s="14"/>
+      <c r="S29" s="14">
+        <v>-57</v>
+      </c>
+      <c r="T29" s="14">
+        <v>-128</v>
+      </c>
+      <c r="U29" s="14">
+        <v>-6</v>
+      </c>
+      <c r="V29" s="14">
+        <v>23</v>
+      </c>
     </row>
     <row r="30" spans="4:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="153"/>
-      <c r="E30" s="157" t="s">
+      <c r="D30" s="154"/>
+      <c r="E30" s="128" t="s">
         <v>9</v>
       </c>
       <c r="F30" s="112">
         <f>AVERAGE(F26:F29)</f>
-        <v>2.5504797824597478</v>
+        <v>2.524565260000025</v>
       </c>
       <c r="G30" s="109">
         <f>AVERAGE(G26:G29)</f>
-        <v>4.0118762028203303</v>
+        <v>4.0679515683416252</v>
       </c>
       <c r="H30" s="109">
         <f>AVERAGE(H26:H29)</f>
-        <v>0.89619422486052747</v>
-      </c>
-      <c r="I30" s="177" cm="1">
+        <v>0.90640400587236925</v>
+      </c>
+      <c r="I30" s="142" cm="1">
         <f t="array" ref="I30">AVERAGE(ABS(I26:I29))</f>
-        <v>10.5</v>
+        <v>9.75</v>
       </c>
       <c r="J30" s="110">
         <f>AVERAGE(J26:J29)</f>
@@ -13299,24 +13765,41 @@
         <f t="array" ref="M30">AVERAGE(ABS(M26:M29))</f>
         <v>20.5</v>
       </c>
+      <c r="N30" s="109">
+        <f>AVERAGE(N26:N29)</f>
+        <v>2.4849184373377224</v>
+      </c>
+      <c r="O30" s="109">
+        <f>AVERAGE(O26:O29)</f>
+        <v>3.7825237599906902</v>
+      </c>
+      <c r="P30" s="109">
+        <f>AVERAGE(P26:P29)</f>
+        <v>0.88946814027729548</v>
+      </c>
+      <c r="Q30" s="111" cm="1">
+        <f t="array" ref="Q30">AVERAGE(ABS(Q26:Q29))</f>
+        <v>13</v>
+      </c>
+      <c r="R30" s="14"/>
     </row>
     <row r="31" spans="4:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D31" s="151">
+      <c r="D31" s="152">
         <v>21</v>
       </c>
-      <c r="E31" s="159" t="s">
+      <c r="E31" s="130" t="s">
         <v>0</v>
       </c>
-      <c r="F31" s="167">
-        <v>2.63980864909824</v>
-      </c>
-      <c r="G31" s="168">
-        <v>3.88970385511591</v>
-      </c>
-      <c r="H31" s="168">
-        <v>0.77413283081775097</v>
-      </c>
-      <c r="I31" s="178">
+      <c r="F31" s="107">
+        <v>2.6003421049615798</v>
+      </c>
+      <c r="G31" s="131">
+        <v>3.8533046101259498</v>
+      </c>
+      <c r="H31" s="131">
+        <v>0.78209572947344197</v>
+      </c>
+      <c r="I31" s="140">
         <v>6</v>
       </c>
       <c r="J31" s="114">
@@ -13331,118 +13814,169 @@
       <c r="M31" s="115">
         <v>30</v>
       </c>
+      <c r="N31" s="133">
+        <v>2.9577961416509502</v>
+      </c>
+      <c r="O31" s="133">
+        <v>4.3657949130589202</v>
+      </c>
+      <c r="P31" s="133">
+        <v>0.71245087138951502</v>
+      </c>
+      <c r="Q31" s="115">
+        <v>-57</v>
+      </c>
+      <c r="R31" s="14"/>
     </row>
     <row r="32" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D32" s="152"/>
+      <c r="D32" s="153"/>
       <c r="E32" s="6" t="s">
         <v>6</v>
       </c>
       <c r="F32" s="107">
-        <v>3.11141102059951</v>
-      </c>
-      <c r="G32" s="165">
-        <v>4.5032490436190296</v>
-      </c>
-      <c r="H32" s="165">
-        <v>0.76103474519610004</v>
-      </c>
-      <c r="I32" s="176">
+        <v>3.072833434658</v>
+      </c>
+      <c r="G32" s="131">
+        <v>4.6761081714629498</v>
+      </c>
+      <c r="H32" s="131">
+        <v>0.75827596468298997</v>
+      </c>
+      <c r="I32" s="141">
         <v>-128</v>
       </c>
-      <c r="J32" s="166">
+      <c r="J32" s="132">
         <v>2.0795192420620499</v>
       </c>
-      <c r="K32" s="166">
+      <c r="K32" s="132">
         <v>3.2358569159613801</v>
       </c>
-      <c r="L32" s="166">
+      <c r="L32" s="132">
         <v>0.91291858690101302</v>
       </c>
       <c r="M32" s="108">
         <v>-5</v>
       </c>
-      <c r="P32" s="189"/>
-    </row>
-    <row r="33" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D33" s="152"/>
+      <c r="N32" s="131">
+        <v>3.6086103265852998</v>
+      </c>
+      <c r="O32" s="131">
+        <v>5.4770218720708899</v>
+      </c>
+      <c r="P32" s="131">
+        <v>0.62210520724011198</v>
+      </c>
+      <c r="Q32" s="103">
+        <v>-128</v>
+      </c>
+      <c r="R32" s="14"/>
+    </row>
+    <row r="33" spans="4:22" x14ac:dyDescent="0.2">
+      <c r="D33" s="153"/>
       <c r="E33" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F33" s="104">
-        <v>2.1549645407998299</v>
-      </c>
-      <c r="G33" s="166">
-        <v>2.69456632543171</v>
-      </c>
-      <c r="H33" s="166">
-        <v>0.89432312515617896</v>
-      </c>
-      <c r="I33" s="176">
-        <v>-6</v>
-      </c>
-      <c r="J33" s="165">
+        <v>1.97738331803615</v>
+      </c>
+      <c r="G33" s="132">
+        <v>2.47347283854304</v>
+      </c>
+      <c r="H33" s="132">
+        <v>0.90040220118840397</v>
+      </c>
+      <c r="I33" s="140">
+        <v>-4</v>
+      </c>
+      <c r="J33" s="131">
         <v>2.30948274738962</v>
       </c>
-      <c r="K33" s="165">
+      <c r="K33" s="131">
         <v>3.28202655837354</v>
       </c>
-      <c r="L33" s="165">
+      <c r="L33" s="131">
         <v>0.858369696353942</v>
       </c>
       <c r="M33" s="108">
         <v>-4</v>
       </c>
-    </row>
-    <row r="34" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D34" s="152"/>
+      <c r="N33" s="131">
+        <v>2.29420340487271</v>
+      </c>
+      <c r="O33" s="131">
+        <v>2.8968259156070699</v>
+      </c>
+      <c r="P33" s="131">
+        <v>0.86830984627044105</v>
+      </c>
+      <c r="Q33" s="103">
+        <v>-6</v>
+      </c>
+      <c r="R33" s="14"/>
+    </row>
+    <row r="34" spans="4:22" x14ac:dyDescent="0.2">
+      <c r="D34" s="153"/>
       <c r="E34" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F34" s="107">
-        <v>4.8042653181545898</v>
-      </c>
-      <c r="G34" s="165">
-        <v>8.7122527323115797</v>
-      </c>
-      <c r="H34" s="165">
-        <v>0.83218065673479502</v>
-      </c>
-      <c r="I34" s="176">
-        <v>23</v>
-      </c>
-      <c r="J34" s="166">
+        <v>4.8334136982145104</v>
+      </c>
+      <c r="G34" s="131">
+        <v>8.9407553087070006</v>
+      </c>
+      <c r="H34" s="131">
+        <v>0.84338822854782203</v>
+      </c>
+      <c r="I34" s="141">
+        <v>22</v>
+      </c>
+      <c r="J34" s="132">
         <v>3.1658921553716599</v>
       </c>
-      <c r="K34" s="166">
+      <c r="K34" s="132">
         <v>6.0402931230179897</v>
       </c>
-      <c r="L34" s="166">
+      <c r="L34" s="132">
         <v>0.91592370939289502</v>
       </c>
       <c r="M34" s="108">
         <v>15</v>
       </c>
-    </row>
-    <row r="35" spans="4:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D35" s="153"/>
+      <c r="N34" s="131">
+        <v>5.0369887593202503</v>
+      </c>
+      <c r="O34" s="131">
+        <v>9.1738224310701302</v>
+      </c>
+      <c r="P34" s="131">
+        <v>0.81204631699589402</v>
+      </c>
+      <c r="Q34" s="103">
+        <v>23</v>
+      </c>
+      <c r="R34" s="14"/>
+    </row>
+    <row r="35" spans="4:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D35" s="154"/>
       <c r="E35" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F35" s="107">
         <f>AVERAGE(F31:F34)</f>
-        <v>3.1776123821630424</v>
-      </c>
-      <c r="G35" s="165">
+        <v>3.12099313896756</v>
+      </c>
+      <c r="G35" s="131">
         <f>AVERAGE(G31:G34)</f>
-        <v>4.9499429891195579</v>
-      </c>
-      <c r="H35" s="165">
+        <v>4.9859102322097346</v>
+      </c>
+      <c r="H35" s="131">
         <f>AVERAGE(H31:H34)</f>
-        <v>0.81541783947620627</v>
-      </c>
-      <c r="I35" s="176" cm="1">
+        <v>0.82104053097316443</v>
+      </c>
+      <c r="I35" s="141" cm="1">
         <f t="array" ref="I35">AVERAGE(ABS(I31:I34))</f>
-        <v>40.75</v>
+        <v>40</v>
       </c>
       <c r="J35" s="110">
         <f>AVERAGE(J31:J34)</f>
@@ -13456,637 +13990,725 @@
         <f>AVERAGE(L31:L34)</f>
         <v>0.88744957625151377</v>
       </c>
-      <c r="M35" s="181" cm="1">
+      <c r="M35" s="146" cm="1">
         <f t="array" ref="M35">AVERAGE(ABS(M31:M34))</f>
         <v>13.5</v>
       </c>
-    </row>
-    <row r="36" spans="4:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D36" s="162" t="s">
+      <c r="N35" s="109">
+        <f>AVERAGE(N31:N34)</f>
+        <v>3.4743996581073024</v>
+      </c>
+      <c r="O35" s="109">
+        <f>AVERAGE(O31:O34)</f>
+        <v>5.4783662829517521</v>
+      </c>
+      <c r="P35" s="109">
+        <f>AVERAGE(P31:P34)</f>
+        <v>0.75372806047399044</v>
+      </c>
+      <c r="Q35" s="111" cm="1">
+        <f t="array" ref="Q35">AVERAGE(ABS(Q31:Q34))</f>
+        <v>53.5</v>
+      </c>
+      <c r="R35" s="14"/>
+      <c r="S35" s="14">
+        <v>2.9512770024242001</v>
+      </c>
+      <c r="T35" s="14">
+        <v>2.6259942309225002</v>
+      </c>
+      <c r="U35" s="14">
+        <v>1.50589329905638</v>
+      </c>
+      <c r="V35" s="14">
+        <v>3.5480996358027301</v>
+      </c>
+    </row>
+    <row r="36" spans="4:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D36" s="181" t="s">
         <v>9</v>
       </c>
-      <c r="E36" s="163"/>
-      <c r="F36" s="169">
-        <f>AVERAGE(F25,F30,F35)</f>
-        <v>2.6366696024810694</v>
-      </c>
-      <c r="G36" s="170">
-        <f>AVERAGE(G25,G30,G35)</f>
-        <v>4.090667126015096</v>
-      </c>
-      <c r="H36" s="170">
-        <f>AVERAGE(H25,H30,H35)</f>
-        <v>0.88623383455924964</v>
-      </c>
-      <c r="I36" s="179">
-        <f>AVERAGE(I25,I30,I35)</f>
-        <v>20.833333333333332</v>
-      </c>
-      <c r="J36" s="171">
-        <f>AVERAGE(J25,J30,J35)</f>
+      <c r="E36" s="182"/>
+      <c r="F36" s="134">
+        <f t="shared" ref="F36:M36" si="5">AVERAGE(F25,F30,F35)</f>
+        <v>2.6236353004055935</v>
+      </c>
+      <c r="G36" s="135">
+        <f t="shared" si="5"/>
+        <v>4.1819955796680981</v>
+      </c>
+      <c r="H36" s="135">
+        <f t="shared" si="5"/>
+        <v>0.89313452105738966</v>
+      </c>
+      <c r="I36" s="144">
+        <f t="shared" si="5"/>
+        <v>20.5</v>
+      </c>
+      <c r="J36" s="136">
+        <f t="shared" si="5"/>
         <v>2.0536008935787242</v>
       </c>
-      <c r="K36" s="171">
-        <f>AVERAGE(K25,K30,K35)</f>
+      <c r="K36" s="136">
+        <f t="shared" si="5"/>
         <v>3.4404324399992867</v>
       </c>
-      <c r="L36" s="171">
-        <f>AVERAGE(L25,L30,L35)</f>
+      <c r="L36" s="136">
+        <f t="shared" si="5"/>
         <v>0.92566620661712262</v>
       </c>
-      <c r="M36" s="182">
-        <f>AVERAGE(M25,M30,M35)</f>
+      <c r="M36" s="147">
+        <f t="shared" si="5"/>
         <v>14.25</v>
       </c>
-    </row>
-    <row r="40" spans="4:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="4:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F41" s="127" t="s">
+      <c r="N36" s="134">
+        <f t="shared" ref="N36:Q36" si="6">AVERAGE(N25,N30,N35)</f>
+        <v>2.8723780458321588</v>
+      </c>
+      <c r="O36" s="135">
+        <f t="shared" si="6"/>
+        <v>4.4472415921744455</v>
+      </c>
+      <c r="P36" s="135">
+        <f t="shared" si="6"/>
+        <v>0.85681130366991687</v>
+      </c>
+      <c r="Q36" s="144">
+        <f t="shared" si="6"/>
+        <v>26.5</v>
+      </c>
+      <c r="R36" s="14"/>
+      <c r="S36" s="14">
+        <v>4.3127364592540296</v>
+      </c>
+      <c r="T36" s="14">
+        <v>4.0622906378416799</v>
+      </c>
+      <c r="U36" s="14">
+        <v>2.0698032495027499</v>
+      </c>
+      <c r="V36" s="14">
+        <v>5.8785085877251104</v>
+      </c>
+    </row>
+    <row r="37" spans="4:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14">
+        <v>0.86352584150675904</v>
+      </c>
+      <c r="T37" s="14">
+        <v>0.91021773196631095</v>
+      </c>
+      <c r="U37" s="14">
+        <v>0.96135869199740298</v>
+      </c>
+      <c r="V37" s="14">
+        <v>0.973848575563387</v>
+      </c>
+    </row>
+    <row r="38" spans="4:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F38" s="180" t="s">
         <v>210</v>
       </c>
-      <c r="G41" s="127"/>
-      <c r="H41" s="127"/>
-      <c r="I41" s="187"/>
-      <c r="J41" s="185" t="s">
+      <c r="G38" s="180"/>
+      <c r="H38" s="180"/>
+      <c r="I38" s="183"/>
+      <c r="J38" s="184" t="s">
         <v>5</v>
       </c>
-      <c r="K41" s="127"/>
-      <c r="L41" s="127"/>
-      <c r="M41" s="127"/>
-    </row>
-    <row r="42" spans="4:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D42" s="97" t="s">
+      <c r="K38" s="180"/>
+      <c r="L38" s="180"/>
+      <c r="M38" s="180"/>
+      <c r="S38" s="14">
+        <v>-8</v>
+      </c>
+      <c r="T38" s="14">
+        <v>17</v>
+      </c>
+      <c r="U38" s="14">
+        <v>-17</v>
+      </c>
+      <c r="V38" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="4:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D39" s="97" t="s">
         <v>215</v>
       </c>
-      <c r="E42" s="98" t="s">
+      <c r="E39" s="98" t="s">
         <v>216</v>
       </c>
-      <c r="F42" s="97" t="s">
+      <c r="F39" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="G42" s="98" t="s">
+      <c r="G39" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="H42" s="98" t="s">
+      <c r="H39" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="I42" s="186" t="s">
+      <c r="I39" s="150" t="s">
         <v>211</v>
       </c>
-      <c r="J42" s="98" t="s">
+      <c r="J39" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="K42" s="98" t="s">
+      <c r="K39" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="L42" s="98" t="s">
+      <c r="L39" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="M42" s="100" t="s">
+      <c r="M39" s="100" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="43" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D43" s="151">
+    <row r="40" spans="4:22" x14ac:dyDescent="0.2">
+      <c r="D40" s="152">
         <v>7</v>
       </c>
-      <c r="E43" s="118" t="s">
+      <c r="E40" s="118" t="s">
         <v>0</v>
       </c>
-      <c r="F43" s="104">
+      <c r="F40" s="104">
         <v>1.1070353752755</v>
       </c>
-      <c r="G43" s="166">
+      <c r="G40" s="132">
         <v>1.71065271503125</v>
       </c>
-      <c r="H43" s="166">
+      <c r="H40" s="132">
         <v>0.97102104724119298</v>
       </c>
-      <c r="I43" s="176">
+      <c r="I40" s="141">
         <v>-8</v>
       </c>
-      <c r="J43" s="165">
+      <c r="J40" s="131">
         <v>1.10039806108107</v>
       </c>
-      <c r="K43" s="106">
+      <c r="K40" s="106">
         <v>1.8662734667024501</v>
       </c>
+      <c r="L40" s="106">
+        <v>0.95325832223974005</v>
+      </c>
+      <c r="M40" s="108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="4:22" x14ac:dyDescent="0.2">
+      <c r="D41" s="153"/>
+      <c r="E41" s="119" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" s="107">
+        <v>1.7518155433089799</v>
+      </c>
+      <c r="G41" s="131">
+        <v>2.67512928879747</v>
+      </c>
+      <c r="H41" s="131">
+        <v>0.94075340656478901</v>
+      </c>
+      <c r="I41" s="141">
+        <v>17</v>
+      </c>
+      <c r="J41" s="132">
+        <v>1.2890154038693</v>
+      </c>
+      <c r="K41" s="102">
+        <v>1.99847807058555</v>
+      </c>
+      <c r="L41" s="102">
+        <v>0.96949236584153597</v>
+      </c>
+      <c r="M41" s="108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="4:22" x14ac:dyDescent="0.2">
+      <c r="D42" s="153"/>
+      <c r="E42" s="119" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="104">
+        <v>1.04479746213702</v>
+      </c>
+      <c r="G42" s="132">
+        <v>1.35308256131581</v>
+      </c>
+      <c r="H42" s="132">
+        <v>0.96879591456060898</v>
+      </c>
+      <c r="I42" s="141">
+        <v>-25</v>
+      </c>
+      <c r="J42" s="131">
+        <v>1.87001411846128</v>
+      </c>
+      <c r="K42" s="106">
+        <v>2.7141148662689401</v>
+      </c>
+      <c r="L42" s="106">
+        <v>0.92859027188879795</v>
+      </c>
+      <c r="M42" s="108">
+        <v>-22</v>
+      </c>
+    </row>
+    <row r="43" spans="4:22" x14ac:dyDescent="0.2">
+      <c r="D43" s="153"/>
+      <c r="E43" s="119" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" s="107">
+        <v>2.6761359061132599</v>
+      </c>
+      <c r="G43" s="131">
+        <v>4.9397442690724001</v>
+      </c>
+      <c r="H43" s="132">
+        <v>0.98515001616769504</v>
+      </c>
+      <c r="I43" s="140">
+        <v>8</v>
+      </c>
+      <c r="J43" s="132">
+        <v>2.30257578140928</v>
+      </c>
+      <c r="K43" s="102">
+        <v>4.0813406210604999</v>
+      </c>
       <c r="L43" s="106">
-        <v>0.95325832223974005</v>
-      </c>
-      <c r="M43" s="108">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D44" s="152"/>
-      <c r="E44" s="119" t="s">
+        <v>0.97775233796657401</v>
+      </c>
+      <c r="M43" s="103">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="4:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D44" s="154"/>
+      <c r="E44" s="120" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="112">
+        <f>AVERAGE(F40:F43)</f>
+        <v>1.6449460717086901</v>
+      </c>
+      <c r="G44" s="109">
+        <f>AVERAGE(G40:G43)</f>
+        <v>2.6696522085542327</v>
+      </c>
+      <c r="H44" s="110">
+        <f>AVERAGE(H40:H43)</f>
+        <v>0.96643009613357156</v>
+      </c>
+      <c r="I44" s="151" cm="1">
+        <f t="array" ref="I44">AVERAGE(ABS(I40:I43))</f>
+        <v>14.5</v>
+      </c>
+      <c r="J44" s="110">
+        <f>AVERAGE(J40:J43)</f>
+        <v>1.6405008412052324</v>
+      </c>
+      <c r="K44" s="110">
+        <f>AVERAGE(K40:K43)</f>
+        <v>2.6650517561543601</v>
+      </c>
+      <c r="L44" s="109">
+        <f>AVERAGE(L40:L43)</f>
+        <v>0.95727332448416202</v>
+      </c>
+      <c r="M44" s="146" cm="1">
+        <f t="array" ref="M44">AVERAGE(ABS(M40:M43))</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="45" spans="4:22" x14ac:dyDescent="0.2">
+      <c r="D45" s="152">
+        <v>14</v>
+      </c>
+      <c r="E45" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="F45" s="113">
+        <v>1.66751317768397</v>
+      </c>
+      <c r="G45" s="114">
+        <v>2.58097335892377</v>
+      </c>
+      <c r="H45" s="114">
+        <v>0.954445957009327</v>
+      </c>
+      <c r="I45" s="143">
+        <v>-1</v>
+      </c>
+      <c r="J45" s="133">
+        <v>1.6694034748597599</v>
+      </c>
+      <c r="K45" s="133">
+        <v>2.8631346027687301</v>
+      </c>
+      <c r="L45" s="133">
+        <v>0.91627292446532504</v>
+      </c>
+      <c r="M45" s="115">
         <v>6</v>
       </c>
-      <c r="F44" s="107">
-        <v>1.7518155433089799</v>
-      </c>
-      <c r="G44" s="165">
-        <v>2.67512928879747</v>
-      </c>
-      <c r="H44" s="165">
-        <v>0.94075340656478901</v>
-      </c>
-      <c r="I44" s="176">
-        <v>17</v>
-      </c>
-      <c r="J44" s="166">
-        <v>1.2890154038693</v>
-      </c>
-      <c r="K44" s="102">
-        <v>1.99847807058555</v>
-      </c>
-      <c r="L44" s="102">
-        <v>0.96949236584153597</v>
-      </c>
-      <c r="M44" s="108">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D45" s="152"/>
-      <c r="E45" s="119" t="s">
+    </row>
+    <row r="46" spans="4:22" x14ac:dyDescent="0.2">
+      <c r="D46" s="153"/>
+      <c r="E46" s="119" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46" s="107">
+        <v>2.3132246887406902</v>
+      </c>
+      <c r="G46" s="131">
+        <v>3.4058351124445201</v>
+      </c>
+      <c r="H46" s="131">
+        <v>0.89100951575892395</v>
+      </c>
+      <c r="I46" s="141">
+        <v>24</v>
+      </c>
+      <c r="J46" s="132">
+        <v>1.68814282715754</v>
+      </c>
+      <c r="K46" s="102">
+        <v>2.6370715572724599</v>
+      </c>
+      <c r="L46" s="102">
+        <v>0.92553063381835099</v>
+      </c>
+      <c r="M46" s="108">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="4:22" x14ac:dyDescent="0.2">
+      <c r="D47" s="153"/>
+      <c r="E47" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="F45" s="104">
-        <v>1.04479746213702</v>
-      </c>
-      <c r="G45" s="166">
-        <v>1.35308256131581</v>
-      </c>
-      <c r="H45" s="166">
-        <v>0.96879591456060898</v>
-      </c>
-      <c r="I45" s="176">
-        <v>-25</v>
-      </c>
-      <c r="J45" s="165">
-        <v>1.87001411846128</v>
-      </c>
-      <c r="K45" s="106">
-        <v>2.7141148662689401</v>
-      </c>
-      <c r="L45" s="106">
-        <v>0.92859027188879795</v>
-      </c>
-      <c r="M45" s="108">
-        <v>-22</v>
-      </c>
-    </row>
-    <row r="46" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D46" s="152"/>
-      <c r="E46" s="119" t="s">
+      <c r="F47" s="104">
+        <v>1.18240441860918</v>
+      </c>
+      <c r="G47" s="132">
+        <v>1.54027935246862</v>
+      </c>
+      <c r="H47" s="132">
+        <v>0.95365281351530395</v>
+      </c>
+      <c r="I47" s="141">
+        <v>-20</v>
+      </c>
+      <c r="J47" s="131">
+        <v>2.3955166648425901</v>
+      </c>
+      <c r="K47" s="106">
+        <v>3.9394499960077098</v>
+      </c>
+      <c r="L47" s="106">
+        <v>0.81399577288686298</v>
+      </c>
+      <c r="M47" s="108">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="4:22" x14ac:dyDescent="0.2">
+      <c r="D48" s="153"/>
+      <c r="E48" s="119" t="s">
         <v>8</v>
       </c>
-      <c r="F46" s="107">
-        <v>2.6761359061132599</v>
-      </c>
-      <c r="G46" s="165">
-        <v>4.9397442690724001</v>
-      </c>
-      <c r="H46" s="166">
-        <v>0.98515001616769504</v>
-      </c>
-      <c r="I46" s="175">
+      <c r="F48" s="104">
+        <v>3.38073406616734</v>
+      </c>
+      <c r="G48" s="131">
+        <v>6.5032005417382903</v>
+      </c>
+      <c r="H48" s="132">
+        <v>0.95746143633606295</v>
+      </c>
+      <c r="I48" s="140">
+        <v>15</v>
+      </c>
+      <c r="J48" s="131">
+        <v>3.49637808647475</v>
+      </c>
+      <c r="K48" s="102">
+        <v>5.5705857717349998</v>
+      </c>
+      <c r="L48" s="106">
+        <v>0.95114531328013696</v>
+      </c>
+      <c r="M48" s="103">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="4:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D49" s="154"/>
+      <c r="E49" s="120" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="148">
+        <f>AVERAGE(F45:F48)</f>
+        <v>2.1359690878002953</v>
+      </c>
+      <c r="G49" s="110">
+        <f>AVERAGE(G45:G48)</f>
+        <v>3.5075720913937998</v>
+      </c>
+      <c r="H49" s="110">
+        <f>AVERAGE(H45:H48)</f>
+        <v>0.93914243065490455</v>
+      </c>
+      <c r="I49" s="151" cm="1">
+        <f t="array" ref="I49">AVERAGE(ABS(I45:I48))</f>
+        <v>15</v>
+      </c>
+      <c r="J49" s="109">
+        <f>AVERAGE(J45:J48)</f>
+        <v>2.3123602633336597</v>
+      </c>
+      <c r="K49" s="109">
+        <f>AVERAGE(K45:K48)</f>
+        <v>3.7525604819459746</v>
+      </c>
+      <c r="L49" s="109">
+        <f>AVERAGE(L45:L48)</f>
+        <v>0.90173616111266897</v>
+      </c>
+      <c r="M49" s="146" cm="1">
+        <f t="array" ref="M49">AVERAGE(ABS(M45:M48))</f>
         <v>8</v>
       </c>
-      <c r="J46" s="166">
-        <v>2.30257578140928</v>
-      </c>
-      <c r="K46" s="102">
-        <v>4.0813406210604999</v>
-      </c>
-      <c r="L46" s="106">
-        <v>0.97775233796657401</v>
-      </c>
-      <c r="M46" s="103">
+    </row>
+    <row r="50" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D50" s="152">
+        <v>21</v>
+      </c>
+      <c r="E50" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="F50" s="113">
+        <v>2.1129973554038899</v>
+      </c>
+      <c r="G50" s="114">
+        <v>3.2221003644184001</v>
+      </c>
+      <c r="H50" s="114">
+        <v>0.92579779817735197</v>
+      </c>
+      <c r="I50" s="143">
+        <v>6</v>
+      </c>
+      <c r="J50" s="133">
+        <v>2.14389271031561</v>
+      </c>
+      <c r="K50" s="133">
+        <v>3.8133579830603002</v>
+      </c>
+      <c r="L50" s="133">
+        <v>0.86590238254708896</v>
+      </c>
+      <c r="M50" s="115">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D51" s="153"/>
+      <c r="E51" s="119" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51" s="107">
+        <v>2.7022792382965002</v>
+      </c>
+      <c r="G51" s="131">
+        <v>4.3644126052041301</v>
+      </c>
+      <c r="H51" s="131">
+        <v>0.84116428262109</v>
+      </c>
+      <c r="I51" s="141">
+        <v>31</v>
+      </c>
+      <c r="J51" s="132">
+        <v>2.3045171885303999</v>
+      </c>
+      <c r="K51" s="102">
+        <v>3.4848589581447</v>
+      </c>
+      <c r="L51" s="102">
+        <v>0.88070730043297996</v>
+      </c>
+      <c r="M51" s="108">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D52" s="153"/>
+      <c r="E52" s="119" t="s">
+        <v>7</v>
+      </c>
+      <c r="F52" s="104">
+        <v>1.5929165836094401</v>
+      </c>
+      <c r="G52" s="132">
+        <v>1.9831003708369099</v>
+      </c>
+      <c r="H52" s="132">
+        <v>0.92825204303803599</v>
+      </c>
+      <c r="I52" s="140">
+        <v>-13</v>
+      </c>
+      <c r="J52" s="131">
+        <v>1.77413054896351</v>
+      </c>
+      <c r="K52" s="106">
+        <v>2.6534778524276499</v>
+      </c>
+      <c r="L52" s="106">
+        <v>0.86806701328723801</v>
+      </c>
+      <c r="M52" s="103">
+        <v>-19</v>
+      </c>
+    </row>
+    <row r="53" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D53" s="153"/>
+      <c r="E53" s="119" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="47" spans="4:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D47" s="153"/>
-      <c r="E47" s="120" t="s">
+      <c r="F53" s="104">
+        <v>4.2909700013444096</v>
+      </c>
+      <c r="G53" s="132">
+        <v>8.4890702748492703</v>
+      </c>
+      <c r="H53" s="131">
+        <v>0.90542411521149901</v>
+      </c>
+      <c r="I53" s="141">
+        <v>22</v>
+      </c>
+      <c r="J53" s="131">
+        <v>5.2975853783740297</v>
+      </c>
+      <c r="K53" s="106">
+        <v>9.5021823238525105</v>
+      </c>
+      <c r="L53" s="102">
+        <v>0.92789692705660498</v>
+      </c>
+      <c r="M53" s="108">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="4:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D54" s="154"/>
+      <c r="E54" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="F47" s="112">
-        <f>AVERAGE(F43:F46)</f>
-        <v>1.6449460717086901</v>
-      </c>
-      <c r="G47" s="109">
-        <f>AVERAGE(G43:G46)</f>
-        <v>2.6696522085542327</v>
-      </c>
-      <c r="H47" s="110">
-        <f>AVERAGE(H43:H46)</f>
-        <v>0.96643009613357156</v>
-      </c>
-      <c r="I47" s="188" cm="1">
-        <f t="array" ref="I47">AVERAGE(ABS(I43:I46))</f>
-        <v>14.5</v>
-      </c>
-      <c r="J47" s="110">
-        <f>AVERAGE(J43:J46)</f>
-        <v>1.6405008412052324</v>
-      </c>
-      <c r="K47" s="110">
-        <f>AVERAGE(K43:K46)</f>
-        <v>2.6650517561543601</v>
-      </c>
-      <c r="L47" s="109">
-        <f>AVERAGE(L43:L46)</f>
-        <v>0.95727332448416202</v>
-      </c>
-      <c r="M47" s="181" cm="1">
-        <f t="array" ref="M47">AVERAGE(ABS(M43:M46))</f>
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="48" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D48" s="151">
-        <v>14</v>
-      </c>
-      <c r="E48" s="118" t="s">
-        <v>0</v>
-      </c>
-      <c r="F48" s="113">
-        <v>1.66751317768397</v>
-      </c>
-      <c r="G48" s="114">
-        <v>2.58097335892377</v>
-      </c>
-      <c r="H48" s="114">
-        <v>0.954445957009327</v>
-      </c>
-      <c r="I48" s="178">
-        <v>-1</v>
-      </c>
-      <c r="J48" s="168">
-        <v>1.6694034748597599</v>
-      </c>
-      <c r="K48" s="168">
-        <v>2.8631346027687301</v>
-      </c>
-      <c r="L48" s="168">
-        <v>0.91627292446532504</v>
-      </c>
-      <c r="M48" s="115">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D49" s="152"/>
-      <c r="E49" s="119" t="s">
-        <v>6</v>
-      </c>
-      <c r="F49" s="107">
-        <v>2.3132246887406902</v>
-      </c>
-      <c r="G49" s="165">
-        <v>3.4058351124445201</v>
-      </c>
-      <c r="H49" s="165">
-        <v>0.89100951575892395</v>
-      </c>
-      <c r="I49" s="176">
-        <v>24</v>
-      </c>
-      <c r="J49" s="166">
-        <v>1.68814282715754</v>
-      </c>
-      <c r="K49" s="102">
-        <v>2.6370715572724599</v>
-      </c>
-      <c r="L49" s="102">
-        <v>0.92553063381835099</v>
-      </c>
-      <c r="M49" s="108">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D50" s="152"/>
-      <c r="E50" s="119" t="s">
-        <v>7</v>
-      </c>
-      <c r="F50" s="104">
-        <v>1.18240441860918</v>
-      </c>
-      <c r="G50" s="166">
-        <v>1.54027935246862</v>
-      </c>
-      <c r="H50" s="166">
-        <v>0.95365281351530395</v>
-      </c>
-      <c r="I50" s="176">
-        <v>-20</v>
-      </c>
-      <c r="J50" s="165">
-        <v>2.3955166648425901</v>
-      </c>
-      <c r="K50" s="106">
-        <v>3.9394499960077098</v>
-      </c>
-      <c r="L50" s="106">
-        <v>0.81399577288686298</v>
-      </c>
-      <c r="M50" s="108">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D51" s="152"/>
-      <c r="E51" s="119" t="s">
-        <v>8</v>
-      </c>
-      <c r="F51" s="104">
-        <v>3.38073406616734</v>
-      </c>
-      <c r="G51" s="165">
-        <v>6.5032005417382903</v>
-      </c>
-      <c r="H51" s="166">
-        <v>0.95746143633606295</v>
-      </c>
-      <c r="I51" s="175">
-        <v>15</v>
-      </c>
-      <c r="J51" s="165">
-        <v>3.49637808647475</v>
-      </c>
-      <c r="K51" s="102">
-        <v>5.5705857717349998</v>
-      </c>
-      <c r="L51" s="106">
-        <v>0.95114531328013696</v>
-      </c>
-      <c r="M51" s="103">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" spans="4:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D52" s="153"/>
-      <c r="E52" s="120" t="s">
+      <c r="F54" s="148">
+        <f>AVERAGE(F50:F53)</f>
+        <v>2.6747907946635596</v>
+      </c>
+      <c r="G54" s="110">
+        <f>AVERAGE(G50:G53)</f>
+        <v>4.5146709038271773</v>
+      </c>
+      <c r="H54" s="110">
+        <f>AVERAGE(H50:H53)</f>
+        <v>0.90015955976199424</v>
+      </c>
+      <c r="I54" s="151" cm="1">
+        <f t="array" ref="I54">AVERAGE(ABS(I50:I53))</f>
+        <v>18</v>
+      </c>
+      <c r="J54" s="109">
+        <f>AVERAGE(J50:J53)</f>
+        <v>2.8800314565458871</v>
+      </c>
+      <c r="K54" s="109">
+        <f>AVERAGE(K50:K53)</f>
+        <v>4.8634692793712908</v>
+      </c>
+      <c r="L54" s="109">
+        <f>AVERAGE(L50:L53)</f>
+        <v>0.88564340583097789</v>
+      </c>
+      <c r="M54" s="146" cm="1">
+        <f t="array" ref="M54">AVERAGE(ABS(M50:M53))</f>
+        <v>15.25</v>
+      </c>
+    </row>
+    <row r="55" spans="4:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D55" s="181" t="s">
         <v>9</v>
       </c>
-      <c r="F52" s="183">
-        <f>AVERAGE(F48:F51)</f>
-        <v>2.1359690878002953</v>
-      </c>
-      <c r="G52" s="110">
-        <f>AVERAGE(G48:G51)</f>
-        <v>3.5075720913937998</v>
-      </c>
-      <c r="H52" s="110">
-        <f>AVERAGE(H48:H51)</f>
-        <v>0.93914243065490455</v>
-      </c>
-      <c r="I52" s="188" cm="1">
-        <f t="array" ref="I52">AVERAGE(ABS(I48:I51))</f>
-        <v>15</v>
-      </c>
-      <c r="J52" s="109">
-        <f>AVERAGE(J48:J51)</f>
-        <v>2.3123602633336597</v>
-      </c>
-      <c r="K52" s="109">
-        <f>AVERAGE(K48:K51)</f>
-        <v>3.7525604819459746</v>
-      </c>
-      <c r="L52" s="109">
-        <f>AVERAGE(L48:L51)</f>
-        <v>0.90173616111266897</v>
-      </c>
-      <c r="M52" s="181" cm="1">
-        <f t="array" ref="M52">AVERAGE(ABS(M48:M51))</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D53" s="151">
-        <v>21</v>
-      </c>
-      <c r="E53" s="118" t="s">
-        <v>0</v>
-      </c>
-      <c r="F53" s="113">
-        <v>2.1129973554038899</v>
-      </c>
-      <c r="G53" s="114">
-        <v>3.2221003644184001</v>
-      </c>
-      <c r="H53" s="114">
-        <v>0.92579779817735197</v>
-      </c>
-      <c r="I53" s="178">
-        <v>6</v>
-      </c>
-      <c r="J53" s="168">
-        <v>2.14389271031561</v>
-      </c>
-      <c r="K53" s="168">
-        <v>3.8133579830603002</v>
-      </c>
-      <c r="L53" s="168">
-        <v>0.86590238254708896</v>
-      </c>
-      <c r="M53" s="115">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="54" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D54" s="152"/>
-      <c r="E54" s="119" t="s">
-        <v>6</v>
-      </c>
-      <c r="F54" s="107">
-        <v>2.7022792382965002</v>
-      </c>
-      <c r="G54" s="165">
-        <v>4.3644126052041301</v>
-      </c>
-      <c r="H54" s="165">
-        <v>0.84116428262109</v>
-      </c>
-      <c r="I54" s="176">
-        <v>31</v>
-      </c>
-      <c r="J54" s="166">
-        <v>2.3045171885303999</v>
-      </c>
-      <c r="K54" s="102">
-        <v>3.4848589581447</v>
-      </c>
-      <c r="L54" s="102">
-        <v>0.88070730043297996</v>
-      </c>
-      <c r="M54" s="108">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="55" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D55" s="152"/>
-      <c r="E55" s="119" t="s">
-        <v>7</v>
-      </c>
-      <c r="F55" s="104">
-        <v>1.5929165836094401</v>
-      </c>
-      <c r="G55" s="166">
-        <v>1.9831003708369099</v>
-      </c>
-      <c r="H55" s="166">
-        <v>0.92825204303803599</v>
-      </c>
-      <c r="I55" s="175">
-        <v>-13</v>
-      </c>
-      <c r="J55" s="165">
-        <v>1.77413054896351</v>
-      </c>
-      <c r="K55" s="106">
-        <v>2.6534778524276499</v>
-      </c>
-      <c r="L55" s="106">
-        <v>0.86806701328723801</v>
-      </c>
-      <c r="M55" s="103">
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="56" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D56" s="152"/>
-      <c r="E56" s="119" t="s">
-        <v>8</v>
-      </c>
-      <c r="F56" s="104">
-        <v>4.2909700013444096</v>
-      </c>
-      <c r="G56" s="166">
-        <v>8.4890702748492703</v>
-      </c>
-      <c r="H56" s="165">
-        <v>0.90542411521149901</v>
-      </c>
-      <c r="I56" s="176">
-        <v>22</v>
-      </c>
-      <c r="J56" s="165">
-        <v>5.2975853783740297</v>
-      </c>
-      <c r="K56" s="106">
-        <v>9.5021823238525105</v>
-      </c>
-      <c r="L56" s="102">
-        <v>0.92789692705660498</v>
-      </c>
-      <c r="M56" s="108">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57" spans="4:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D57" s="153"/>
-      <c r="E57" s="120" t="s">
-        <v>9</v>
-      </c>
-      <c r="F57" s="183">
-        <f>AVERAGE(F53:F56)</f>
-        <v>2.6747907946635596</v>
-      </c>
-      <c r="G57" s="110">
-        <f>AVERAGE(G53:G56)</f>
-        <v>4.5146709038271773</v>
-      </c>
-      <c r="H57" s="110">
-        <f>AVERAGE(H53:H56)</f>
-        <v>0.90015955976199424</v>
-      </c>
-      <c r="I57" s="188" cm="1">
-        <f t="array" ref="I57">AVERAGE(ABS(I53:I56))</f>
-        <v>18</v>
-      </c>
-      <c r="J57" s="109">
-        <f>AVERAGE(J53:J56)</f>
-        <v>2.8800314565458871</v>
-      </c>
-      <c r="K57" s="109">
-        <f>AVERAGE(K53:K56)</f>
-        <v>4.8634692793712908</v>
-      </c>
-      <c r="L57" s="109">
-        <f>AVERAGE(L53:L56)</f>
-        <v>0.88564340583097789</v>
-      </c>
-      <c r="M57" s="181" cm="1">
-        <f t="array" ref="M57">AVERAGE(ABS(M53:M56))</f>
-        <v>15.25</v>
-      </c>
-    </row>
-    <row r="58" spans="4:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D58" s="162" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="163"/>
-      <c r="F58" s="184">
-        <f>AVERAGE(F47,F52,F57)</f>
+      <c r="E55" s="182"/>
+      <c r="F55" s="149">
+        <f t="shared" ref="F55:M55" si="7">AVERAGE(F44,F49,F54)</f>
         <v>2.1519019847241818</v>
       </c>
-      <c r="G58" s="171">
-        <f>AVERAGE(G47,G52,G57)</f>
+      <c r="G55" s="136">
+        <f t="shared" si="7"/>
         <v>3.5639650679250701</v>
       </c>
-      <c r="H58" s="171">
-        <f>AVERAGE(H47,H52,H57)</f>
+      <c r="H55" s="136">
+        <f t="shared" si="7"/>
         <v>0.93524402885015689</v>
       </c>
-      <c r="I58" s="179">
-        <f>AVERAGE(I47,I52,I57)</f>
+      <c r="I55" s="144">
+        <f t="shared" si="7"/>
         <v>15.833333333333334</v>
       </c>
-      <c r="J58" s="170">
-        <f>AVERAGE(J47,J52,J57)</f>
+      <c r="J55" s="135">
+        <f t="shared" si="7"/>
         <v>2.2776308536949266</v>
       </c>
-      <c r="K58" s="170">
-        <f>AVERAGE(K47,K52,K57)</f>
+      <c r="K55" s="135">
+        <f t="shared" si="7"/>
         <v>3.7603605058238752</v>
       </c>
-      <c r="L58" s="170">
-        <f>AVERAGE(L47,L52,L57)</f>
+      <c r="L55" s="135">
+        <f t="shared" si="7"/>
         <v>0.91488429714260311</v>
       </c>
-      <c r="M58" s="182">
-        <f>AVERAGE(M47,M52,M57)</f>
+      <c r="M55" s="147">
+        <f t="shared" si="7"/>
         <v>10.583333333333334</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="D53:D57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="J41:M41"/>
-    <mergeCell ref="D43:D47"/>
-    <mergeCell ref="D48:D52"/>
+  <mergeCells count="20">
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D31:D35"/>
+    <mergeCell ref="F6:J6"/>
+    <mergeCell ref="K6:O6"/>
+    <mergeCell ref="D21:D25"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="N19:Q19"/>
+    <mergeCell ref="P6:T6"/>
+    <mergeCell ref="U6:U7"/>
     <mergeCell ref="D12:D15"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="J19:M19"/>
-    <mergeCell ref="D21:D25"/>
-    <mergeCell ref="D26:D30"/>
-    <mergeCell ref="D31:D35"/>
-    <mergeCell ref="F6:J6"/>
-    <mergeCell ref="K6:O6"/>
-    <mergeCell ref="P6:T6"/>
-    <mergeCell ref="U6:U7"/>
-    <mergeCell ref="C8:C13"/>
-    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D50:D54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="D40:D44"/>
+    <mergeCell ref="D45:D49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
modelling with synthetic dataset
</commit_message>
<xml_diff>
--- a/Logging/Tools/Results_Summary.xlsx
+++ b/Logging/Tools/Results_Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/github/Forecasting/Logging/Tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2BAB60-33F0-9D44-9210-6589301FAC88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAF5F60-6BFA-2249-BF66-367BD3317654}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" activeTab="1" xr2:uid="{D6C4A1CF-C8B6-1A42-B202-9397802E1C24}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" activeTab="1" xr2:uid="{D6C4A1CF-C8B6-1A42-B202-9397802E1C24}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="239">
   <si>
     <t>2014/15</t>
   </si>
@@ -778,6 +778,12 @@
   </si>
   <si>
     <t>Linear Model with Confidence Intervals and Squared Inputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRU			</t>
+  </si>
+  <si>
+    <t>GRU + Model Uncertainty</t>
   </si>
 </sst>
 </file>
@@ -1197,7 +1203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="188">
+  <cellXfs count="196">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1475,19 +1481,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1499,16 +1502,46 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1520,37 +1553,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1565,14 +1589,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6926,8 +6954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F65057-F8D9-5340-9C4E-E5CBE3EA5B75}">
   <dimension ref="B1:BW103"/>
   <sheetViews>
-    <sheetView topLeftCell="R3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X56" sqref="X56:AA59"/>
+    <sheetView topLeftCell="D49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE38" sqref="AE38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6954,28 +6982,28 @@
     </row>
     <row r="2" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="13"/>
-      <c r="E2" s="171" t="s">
+      <c r="E2" s="156" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="172"/>
-      <c r="G2" s="172"/>
-      <c r="H2" s="172"/>
-      <c r="I2" s="173"/>
-      <c r="J2" s="171" t="s">
+      <c r="F2" s="157"/>
+      <c r="G2" s="157"/>
+      <c r="H2" s="157"/>
+      <c r="I2" s="158"/>
+      <c r="J2" s="156" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="172"/>
-      <c r="L2" s="172"/>
-      <c r="M2" s="172"/>
-      <c r="N2" s="173"/>
-      <c r="O2" s="171" t="s">
+      <c r="K2" s="157"/>
+      <c r="L2" s="157"/>
+      <c r="M2" s="157"/>
+      <c r="N2" s="158"/>
+      <c r="O2" s="156" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="172"/>
-      <c r="Q2" s="172"/>
-      <c r="R2" s="172"/>
-      <c r="S2" s="173"/>
-      <c r="T2" s="174" t="s">
+      <c r="P2" s="157"/>
+      <c r="Q2" s="157"/>
+      <c r="R2" s="157"/>
+      <c r="S2" s="158"/>
+      <c r="T2" s="169" t="s">
         <v>9</v>
       </c>
     </row>
@@ -7026,13 +7054,13 @@
       <c r="S3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="T3" s="174"/>
+      <c r="T3" s="169"/>
     </row>
     <row r="4" spans="2:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="170" t="s">
+      <c r="B4" s="168" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="175" t="s">
+      <c r="C4" s="170" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="8" t="s">
@@ -7092,8 +7120,8 @@
       </c>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B5" s="170"/>
-      <c r="C5" s="165"/>
+      <c r="B5" s="168"/>
+      <c r="C5" s="166"/>
       <c r="D5" s="9" t="s">
         <v>2</v>
       </c>
@@ -7151,8 +7179,8 @@
       </c>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B6" s="170"/>
-      <c r="C6" s="176"/>
+      <c r="B6" s="168"/>
+      <c r="C6" s="171"/>
       <c r="D6" s="11" t="s">
         <v>3</v>
       </c>
@@ -7210,8 +7238,8 @@
       </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B7" s="170"/>
-      <c r="C7" s="165" t="s">
+      <c r="B7" s="168"/>
+      <c r="C7" s="166" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="9" t="s">
@@ -7271,8 +7299,8 @@
       </c>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B8" s="170"/>
-      <c r="C8" s="165"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="166"/>
       <c r="D8" s="9" t="s">
         <v>2</v>
       </c>
@@ -7330,8 +7358,8 @@
       </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B9" s="170"/>
-      <c r="C9" s="176"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="171"/>
       <c r="D9" s="11" t="s">
         <v>3</v>
       </c>
@@ -7389,8 +7417,8 @@
       </c>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B10" s="170"/>
-      <c r="C10" s="165" t="s">
+      <c r="B10" s="168"/>
+      <c r="C10" s="166" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="9" t="s">
@@ -7450,8 +7478,8 @@
       </c>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B11" s="170"/>
-      <c r="C11" s="165"/>
+      <c r="B11" s="168"/>
+      <c r="C11" s="166"/>
       <c r="D11" s="9" t="s">
         <v>2</v>
       </c>
@@ -7509,8 +7537,8 @@
       </c>
     </row>
     <row r="12" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="170"/>
-      <c r="C12" s="166"/>
+      <c r="B12" s="168"/>
+      <c r="C12" s="167"/>
       <c r="D12" s="10" t="s">
         <v>3</v>
       </c>
@@ -7568,8 +7596,8 @@
       </c>
     </row>
     <row r="13" spans="2:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="170"/>
-      <c r="C13" s="165" t="s">
+      <c r="B13" s="168"/>
+      <c r="C13" s="166" t="s">
         <v>208</v>
       </c>
       <c r="D13" s="9" t="s">
@@ -7629,8 +7657,8 @@
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B14" s="170"/>
-      <c r="C14" s="165"/>
+      <c r="B14" s="168"/>
+      <c r="C14" s="166"/>
       <c r="D14" s="9" t="s">
         <v>2</v>
       </c>
@@ -7692,8 +7720,8 @@
       </c>
     </row>
     <row r="15" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="170"/>
-      <c r="C15" s="166"/>
+      <c r="B15" s="168"/>
+      <c r="C15" s="167"/>
       <c r="D15" s="10" t="s">
         <v>3</v>
       </c>
@@ -7751,7 +7779,7 @@
       </c>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="C16" s="165" t="s">
+      <c r="C16" s="166" t="s">
         <v>207</v>
       </c>
       <c r="D16" s="9" t="s">
@@ -7811,7 +7839,7 @@
       </c>
     </row>
     <row r="17" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="C17" s="165"/>
+      <c r="C17" s="166"/>
       <c r="D17" s="9" t="s">
         <v>2</v>
       </c>
@@ -7869,7 +7897,7 @@
       </c>
     </row>
     <row r="18" spans="2:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="166"/>
+      <c r="C18" s="167"/>
       <c r="D18" s="10" t="s">
         <v>3</v>
       </c>
@@ -7927,7 +7955,7 @@
       </c>
     </row>
     <row r="19" spans="2:39" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C19" s="165" t="s">
+      <c r="C19" s="166" t="s">
         <v>182</v>
       </c>
       <c r="D19" s="9" t="s">
@@ -7962,7 +7990,7 @@
       <c r="T19" s="48"/>
     </row>
     <row r="20" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="C20" s="165"/>
+      <c r="C20" s="166"/>
       <c r="D20" s="9" t="s">
         <v>2</v>
       </c>
@@ -7995,7 +8023,7 @@
       <c r="T20" s="48"/>
     </row>
     <row r="21" spans="2:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="166"/>
+      <c r="C21" s="167"/>
       <c r="D21" s="10" t="s">
         <v>3</v>
       </c>
@@ -8028,7 +8056,7 @@
       <c r="T21" s="52"/>
     </row>
     <row r="22" spans="2:39" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="165" t="s">
+      <c r="C22" s="166" t="s">
         <v>183</v>
       </c>
       <c r="D22" s="9" t="s">
@@ -8063,7 +8091,7 @@
       <c r="T22" s="25"/>
     </row>
     <row r="23" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="C23" s="165"/>
+      <c r="C23" s="166"/>
       <c r="D23" s="9" t="s">
         <v>2</v>
       </c>
@@ -8096,7 +8124,7 @@
       <c r="T23" s="32"/>
     </row>
     <row r="24" spans="2:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="166"/>
+      <c r="C24" s="167"/>
       <c r="D24" s="10" t="s">
         <v>3</v>
       </c>
@@ -8130,48 +8158,48 @@
     </row>
     <row r="25" spans="2:39" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E26" s="171" t="s">
+      <c r="E26" s="156" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="172"/>
-      <c r="G26" s="172"/>
-      <c r="H26" s="172"/>
-      <c r="I26" s="173"/>
-      <c r="J26" s="171" t="s">
+      <c r="F26" s="157"/>
+      <c r="G26" s="157"/>
+      <c r="H26" s="157"/>
+      <c r="I26" s="158"/>
+      <c r="J26" s="156" t="s">
         <v>11</v>
       </c>
-      <c r="K26" s="172"/>
-      <c r="L26" s="172"/>
-      <c r="M26" s="172"/>
-      <c r="N26" s="173"/>
-      <c r="O26" s="171" t="s">
+      <c r="K26" s="157"/>
+      <c r="L26" s="157"/>
+      <c r="M26" s="157"/>
+      <c r="N26" s="158"/>
+      <c r="O26" s="156" t="s">
         <v>12</v>
       </c>
-      <c r="P26" s="172"/>
-      <c r="Q26" s="172"/>
-      <c r="R26" s="172"/>
-      <c r="S26" s="173"/>
+      <c r="P26" s="157"/>
+      <c r="Q26" s="157"/>
+      <c r="R26" s="157"/>
+      <c r="S26" s="158"/>
       <c r="T26" s="68"/>
-      <c r="X26" s="180" t="s">
+      <c r="X26" s="155" t="s">
         <v>209</v>
       </c>
-      <c r="Y26" s="180"/>
-      <c r="Z26" s="180"/>
-      <c r="AA26" s="180"/>
-      <c r="AB26" s="180"/>
-      <c r="AC26" s="180"/>
-      <c r="AD26" s="180"/>
-      <c r="AE26" s="180"/>
-      <c r="AF26" s="180" t="s">
+      <c r="Y26" s="155"/>
+      <c r="Z26" s="155"/>
+      <c r="AA26" s="155"/>
+      <c r="AB26" s="155"/>
+      <c r="AC26" s="155"/>
+      <c r="AD26" s="155"/>
+      <c r="AE26" s="155"/>
+      <c r="AF26" s="155" t="s">
         <v>206</v>
       </c>
-      <c r="AG26" s="180"/>
-      <c r="AH26" s="180"/>
-      <c r="AI26" s="180"/>
-      <c r="AJ26" s="180"/>
-      <c r="AK26" s="180"/>
-      <c r="AL26" s="180"/>
-      <c r="AM26" s="180"/>
+      <c r="AG26" s="155"/>
+      <c r="AH26" s="155"/>
+      <c r="AI26" s="155"/>
+      <c r="AJ26" s="155"/>
+      <c r="AK26" s="155"/>
+      <c r="AL26" s="155"/>
+      <c r="AM26" s="155"/>
     </row>
     <row r="27" spans="2:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E27" s="69" t="s">
@@ -8222,36 +8250,36 @@
       <c r="T27" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="X27" s="180" t="s">
+      <c r="X27" s="155" t="s">
         <v>210</v>
       </c>
-      <c r="Y27" s="180"/>
-      <c r="Z27" s="180"/>
-      <c r="AA27" s="180"/>
-      <c r="AB27" s="180" t="s">
+      <c r="Y27" s="155"/>
+      <c r="Z27" s="155"/>
+      <c r="AA27" s="155"/>
+      <c r="AB27" s="155" t="s">
         <v>5</v>
       </c>
-      <c r="AC27" s="180"/>
-      <c r="AD27" s="180"/>
-      <c r="AE27" s="180"/>
-      <c r="AF27" s="180" t="s">
+      <c r="AC27" s="155"/>
+      <c r="AD27" s="155"/>
+      <c r="AE27" s="155"/>
+      <c r="AF27" s="155" t="s">
         <v>210</v>
       </c>
-      <c r="AG27" s="180"/>
-      <c r="AH27" s="180"/>
-      <c r="AI27" s="180"/>
-      <c r="AJ27" s="180" t="s">
+      <c r="AG27" s="155"/>
+      <c r="AH27" s="155"/>
+      <c r="AI27" s="155"/>
+      <c r="AJ27" s="155" t="s">
         <v>5</v>
       </c>
-      <c r="AK27" s="180"/>
-      <c r="AL27" s="180"/>
-      <c r="AM27" s="180"/>
+      <c r="AK27" s="155"/>
+      <c r="AL27" s="155"/>
+      <c r="AM27" s="155"/>
     </row>
     <row r="28" spans="2:39" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="177" t="s">
+      <c r="B28" s="162" t="s">
         <v>209</v>
       </c>
-      <c r="C28" s="160" t="s">
+      <c r="C28" s="159" t="s">
         <v>210</v>
       </c>
       <c r="D28" s="53" t="s">
@@ -8366,7 +8394,7 @@
     </row>
     <row r="29" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B29" s="163"/>
-      <c r="C29" s="161"/>
+      <c r="C29" s="160"/>
       <c r="D29" s="2" t="s">
         <v>2</v>
       </c>
@@ -8422,7 +8450,7 @@
         <f t="shared" ref="T29:T39" si="12">AVERAGE(I29,N29,S29)</f>
         <v>3.5639650679250701</v>
       </c>
-      <c r="V29" s="152">
+      <c r="V29" s="179">
         <v>7</v>
       </c>
       <c r="W29" s="101" t="s">
@@ -8479,7 +8507,7 @@
     </row>
     <row r="30" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B30" s="163"/>
-      <c r="C30" s="161"/>
+      <c r="C30" s="160"/>
       <c r="D30" s="2" t="s">
         <v>3</v>
       </c>
@@ -8535,7 +8563,7 @@
         <f t="shared" si="12"/>
         <v>0.93524402885015689</v>
       </c>
-      <c r="V30" s="153"/>
+      <c r="V30" s="180"/>
       <c r="W30" s="105" t="s">
         <v>6</v>
       </c>
@@ -8590,7 +8618,7 @@
     </row>
     <row r="31" spans="2:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="163"/>
-      <c r="C31" s="162"/>
+      <c r="C31" s="161"/>
       <c r="D31" s="54" t="s">
         <v>211</v>
       </c>
@@ -8646,7 +8674,7 @@
         <f t="shared" si="12"/>
         <v>15.833333333333334</v>
       </c>
-      <c r="V31" s="153"/>
+      <c r="V31" s="180"/>
       <c r="W31" s="105" t="s">
         <v>7</v>
       </c>
@@ -8701,7 +8729,7 @@
     </row>
     <row r="32" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B32" s="163"/>
-      <c r="C32" s="160" t="s">
+      <c r="C32" s="159" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="53" t="s">
@@ -8759,7 +8787,7 @@
         <f t="shared" si="12"/>
         <v>2.2776308536949266</v>
       </c>
-      <c r="V32" s="153"/>
+      <c r="V32" s="180"/>
       <c r="W32" s="105" t="s">
         <v>8</v>
       </c>
@@ -8814,7 +8842,7 @@
     </row>
     <row r="33" spans="2:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="163"/>
-      <c r="C33" s="161"/>
+      <c r="C33" s="160"/>
       <c r="D33" s="2" t="s">
         <v>2</v>
       </c>
@@ -8870,7 +8898,7 @@
         <f t="shared" si="12"/>
         <v>3.7603605058238752</v>
       </c>
-      <c r="V33" s="154"/>
+      <c r="V33" s="181"/>
       <c r="W33" s="72" t="s">
         <v>9</v>
       </c>
@@ -8941,7 +8969,7 @@
     </row>
     <row r="34" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B34" s="163"/>
-      <c r="C34" s="161"/>
+      <c r="C34" s="160"/>
       <c r="D34" s="2" t="s">
         <v>3</v>
       </c>
@@ -8997,7 +9025,7 @@
         <f t="shared" si="12"/>
         <v>0.91488429714260311</v>
       </c>
-      <c r="V34" s="152">
+      <c r="V34" s="179">
         <v>14</v>
       </c>
       <c r="W34" s="101" t="s">
@@ -9054,7 +9082,7 @@
     </row>
     <row r="35" spans="2:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="163"/>
-      <c r="C35" s="162"/>
+      <c r="C35" s="161"/>
       <c r="D35" s="95" t="s">
         <v>211</v>
       </c>
@@ -9110,7 +9138,7 @@
         <f t="shared" si="12"/>
         <v>10.583333333333334</v>
       </c>
-      <c r="V35" s="153"/>
+      <c r="V35" s="180"/>
       <c r="W35" s="105" t="s">
         <v>6</v>
       </c>
@@ -9165,7 +9193,7 @@
     </row>
     <row r="36" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B36" s="163"/>
-      <c r="C36" s="161" t="s">
+      <c r="C36" s="160" t="s">
         <v>4</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -9223,7 +9251,7 @@
         <f t="shared" si="12"/>
         <v>3.0008085841689058</v>
       </c>
-      <c r="V36" s="153"/>
+      <c r="V36" s="180"/>
       <c r="W36" s="105" t="s">
         <v>7</v>
       </c>
@@ -9278,7 +9306,7 @@
     </row>
     <row r="37" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B37" s="163"/>
-      <c r="C37" s="161"/>
+      <c r="C37" s="160"/>
       <c r="D37" s="2" t="s">
         <v>2</v>
       </c>
@@ -9334,7 +9362,7 @@
         <f t="shared" si="12"/>
         <v>5.158547971052232</v>
       </c>
-      <c r="V37" s="153"/>
+      <c r="V37" s="180"/>
       <c r="W37" s="105" t="s">
         <v>8</v>
       </c>
@@ -9389,7 +9417,7 @@
     </row>
     <row r="38" spans="2:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="163"/>
-      <c r="C38" s="161"/>
+      <c r="C38" s="160"/>
       <c r="D38" s="2" t="s">
         <v>3</v>
       </c>
@@ -9445,7 +9473,7 @@
         <f t="shared" si="12"/>
         <v>0.87064370203199515</v>
       </c>
-      <c r="V38" s="154"/>
+      <c r="V38" s="181"/>
       <c r="W38" s="72" t="s">
         <v>9</v>
       </c>
@@ -9515,8 +9543,8 @@
       </c>
     </row>
     <row r="39" spans="2:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="178"/>
-      <c r="C39" s="179"/>
+      <c r="B39" s="164"/>
+      <c r="C39" s="165"/>
       <c r="D39" s="92" t="s">
         <v>212</v>
       </c>
@@ -9572,7 +9600,7 @@
         <f t="shared" si="12"/>
         <v>23.25</v>
       </c>
-      <c r="V39" s="152">
+      <c r="V39" s="179">
         <v>21</v>
       </c>
       <c r="W39" s="101" t="s">
@@ -9631,7 +9659,7 @@
       <c r="B40" s="163" t="s">
         <v>206</v>
       </c>
-      <c r="C40" s="161" t="s">
+      <c r="C40" s="160" t="s">
         <v>210</v>
       </c>
       <c r="D40" s="13" t="s">
@@ -9689,7 +9717,7 @@
         <f>AVERAGE(I40,N40,S40)</f>
         <v>0.48197307962486019</v>
       </c>
-      <c r="V40" s="153"/>
+      <c r="V40" s="180"/>
       <c r="W40" s="105" t="s">
         <v>6</v>
       </c>
@@ -9744,7 +9772,7 @@
     </row>
     <row r="41" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B41" s="163"/>
-      <c r="C41" s="161"/>
+      <c r="C41" s="160"/>
       <c r="D41" s="13" t="s">
         <v>2</v>
       </c>
@@ -9800,7 +9828,7 @@
         <f>AVERAGE(I41,N41,S41)</f>
         <v>0.71483607643238045</v>
       </c>
-      <c r="V41" s="153"/>
+      <c r="V41" s="180"/>
       <c r="W41" s="105" t="s">
         <v>7</v>
       </c>
@@ -9855,7 +9883,7 @@
     </row>
     <row r="42" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B42" s="163"/>
-      <c r="C42" s="161"/>
+      <c r="C42" s="160"/>
       <c r="D42" s="13" t="s">
         <v>3</v>
       </c>
@@ -9911,7 +9939,7 @@
         <f>AVERAGE(I42,N42,S42)</f>
         <v>0.89514895097951153</v>
       </c>
-      <c r="V42" s="153"/>
+      <c r="V42" s="180"/>
       <c r="W42" s="105" t="s">
         <v>8</v>
       </c>
@@ -9966,7 +9994,7 @@
     </row>
     <row r="43" spans="2:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B43" s="163"/>
-      <c r="C43" s="162"/>
+      <c r="C43" s="161"/>
       <c r="D43" s="54" t="s">
         <v>211</v>
       </c>
@@ -10022,7 +10050,7 @@
         <f>AVERAGE(I43,N43,S43)</f>
         <v>12.666666666666666</v>
       </c>
-      <c r="V43" s="154"/>
+      <c r="V43" s="181"/>
       <c r="W43" s="72" t="s">
         <v>9</v>
       </c>
@@ -10093,7 +10121,7 @@
     </row>
     <row r="44" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B44" s="163"/>
-      <c r="C44" s="160" t="s">
+      <c r="C44" s="159" t="s">
         <v>5</v>
       </c>
       <c r="D44" s="13" t="s">
@@ -10151,10 +10179,10 @@
         <f t="shared" ref="T44:T51" si="21">AVERAGE(I44,N44,S44)</f>
         <v>0.38309457795371937</v>
       </c>
-      <c r="V44" s="155" t="s">
+      <c r="V44" s="182" t="s">
         <v>9</v>
       </c>
-      <c r="W44" s="156"/>
+      <c r="W44" s="183"/>
       <c r="X44" s="113">
         <f t="shared" ref="X44:AM44" si="22">AVERAGE(X33,X38,X43)</f>
         <v>2.1519019847241818</v>
@@ -10222,7 +10250,7 @@
     </row>
     <row r="45" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B45" s="163"/>
-      <c r="C45" s="161"/>
+      <c r="C45" s="160"/>
       <c r="D45" s="13" t="s">
         <v>2</v>
       </c>
@@ -10281,7 +10309,7 @@
     </row>
     <row r="46" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B46" s="163"/>
-      <c r="C46" s="161"/>
+      <c r="C46" s="160"/>
       <c r="D46" s="13" t="s">
         <v>3</v>
       </c>
@@ -10340,7 +10368,7 @@
     </row>
     <row r="47" spans="2:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B47" s="163"/>
-      <c r="C47" s="162"/>
+      <c r="C47" s="161"/>
       <c r="D47" s="54" t="s">
         <v>212</v>
       </c>
@@ -10399,7 +10427,7 @@
     </row>
     <row r="48" spans="2:40" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="163"/>
-      <c r="C48" s="160" t="s">
+      <c r="C48" s="159" t="s">
         <v>4</v>
       </c>
       <c r="D48" s="13" t="s">
@@ -10484,7 +10512,7 @@
     </row>
     <row r="49" spans="2:75" x14ac:dyDescent="0.2">
       <c r="B49" s="163"/>
-      <c r="C49" s="161"/>
+      <c r="C49" s="160"/>
       <c r="D49" s="13" t="s">
         <v>2</v>
       </c>
@@ -10567,7 +10595,7 @@
     </row>
     <row r="50" spans="2:75" x14ac:dyDescent="0.2">
       <c r="B50" s="163"/>
-      <c r="C50" s="161"/>
+      <c r="C50" s="160"/>
       <c r="D50" s="13" t="s">
         <v>3</v>
       </c>
@@ -10661,8 +10689,8 @@
       </c>
     </row>
     <row r="51" spans="2:75" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="164"/>
-      <c r="C51" s="162"/>
+      <c r="B51" s="175"/>
+      <c r="C51" s="161"/>
       <c r="D51" s="54" t="s">
         <v>212</v>
       </c>
@@ -10915,10 +10943,10 @@
       <c r="BW55" s="13"/>
     </row>
     <row r="56" spans="2:75" x14ac:dyDescent="0.2">
-      <c r="B56" s="167">
+      <c r="B56" s="176">
         <v>0</v>
       </c>
-      <c r="C56" s="157">
+      <c r="C56" s="172">
         <v>0</v>
       </c>
       <c r="D56" s="53" t="s">
@@ -11006,8 +11034,8 @@
       <c r="BW56" s="55"/>
     </row>
     <row r="57" spans="2:75" x14ac:dyDescent="0.2">
-      <c r="B57" s="168"/>
-      <c r="C57" s="158"/>
+      <c r="B57" s="177"/>
+      <c r="C57" s="173"/>
       <c r="D57" s="2" t="s">
         <v>2</v>
       </c>
@@ -11097,8 +11125,8 @@
       <c r="BW57" s="55"/>
     </row>
     <row r="58" spans="2:75" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="169"/>
-      <c r="C58" s="159"/>
+      <c r="B58" s="178"/>
+      <c r="C58" s="174"/>
       <c r="D58" s="54" t="s">
         <v>3</v>
       </c>
@@ -11180,10 +11208,10 @@
       <c r="BW58" s="55"/>
     </row>
     <row r="59" spans="2:75" x14ac:dyDescent="0.2">
-      <c r="B59" s="167">
+      <c r="B59" s="176">
         <v>0</v>
       </c>
-      <c r="C59" s="157">
+      <c r="C59" s="172">
         <v>1E-3</v>
       </c>
       <c r="D59" s="53" t="s">
@@ -11241,8 +11269,8 @@
       </c>
     </row>
     <row r="60" spans="2:75" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="168"/>
-      <c r="C60" s="158"/>
+      <c r="B60" s="177"/>
+      <c r="C60" s="173"/>
       <c r="D60" s="2" t="s">
         <v>2</v>
       </c>
@@ -11300,8 +11328,8 @@
       </c>
     </row>
     <row r="61" spans="2:75" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="169"/>
-      <c r="C61" s="159"/>
+      <c r="B61" s="178"/>
+      <c r="C61" s="174"/>
       <c r="D61" s="54" t="s">
         <v>3</v>
       </c>
@@ -11339,10 +11367,10 @@
       </c>
     </row>
     <row r="62" spans="2:75" x14ac:dyDescent="0.2">
-      <c r="B62" s="157">
+      <c r="B62" s="172">
         <v>0</v>
       </c>
-      <c r="C62" s="157">
+      <c r="C62" s="172">
         <v>0.01</v>
       </c>
       <c r="D62" s="53" t="s">
@@ -11382,8 +11410,8 @@
       </c>
     </row>
     <row r="63" spans="2:75" x14ac:dyDescent="0.2">
-      <c r="B63" s="158"/>
-      <c r="C63" s="158"/>
+      <c r="B63" s="173"/>
+      <c r="C63" s="173"/>
       <c r="D63" s="2" t="s">
         <v>2</v>
       </c>
@@ -11416,8 +11444,8 @@
       <c r="AF63" s="14"/>
     </row>
     <row r="64" spans="2:75" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="159"/>
-      <c r="C64" s="159"/>
+      <c r="B64" s="174"/>
+      <c r="C64" s="174"/>
       <c r="D64" s="54" t="s">
         <v>3</v>
       </c>
@@ -11447,10 +11475,10 @@
       <c r="AF64" s="14"/>
     </row>
     <row r="65" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B65" s="157">
+      <c r="B65" s="172">
         <v>0</v>
       </c>
-      <c r="C65" s="157">
+      <c r="C65" s="172">
         <v>0.1</v>
       </c>
       <c r="D65" s="53" t="s">
@@ -11478,8 +11506,8 @@
       <c r="N65"/>
     </row>
     <row r="66" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B66" s="158"/>
-      <c r="C66" s="158"/>
+      <c r="B66" s="173"/>
+      <c r="C66" s="173"/>
       <c r="D66" s="2" t="s">
         <v>2</v>
       </c>
@@ -11505,8 +11533,8 @@
       <c r="N66"/>
     </row>
     <row r="67" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="159"/>
-      <c r="C67" s="159"/>
+      <c r="B67" s="174"/>
+      <c r="C67" s="174"/>
       <c r="D67" s="54" t="s">
         <v>3</v>
       </c>
@@ -11535,10 +11563,10 @@
       <c r="N67"/>
     </row>
     <row r="68" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B68" s="157">
+      <c r="B68" s="172">
         <v>1E-3</v>
       </c>
-      <c r="C68" s="157">
+      <c r="C68" s="172">
         <v>0</v>
       </c>
       <c r="D68" s="53" t="s">
@@ -11566,8 +11594,8 @@
       <c r="N68"/>
     </row>
     <row r="69" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B69" s="158"/>
-      <c r="C69" s="158"/>
+      <c r="B69" s="173"/>
+      <c r="C69" s="173"/>
       <c r="D69" s="2" t="s">
         <v>2</v>
       </c>
@@ -11593,8 +11621,8 @@
       <c r="N69"/>
     </row>
     <row r="70" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="159"/>
-      <c r="C70" s="159"/>
+      <c r="B70" s="174"/>
+      <c r="C70" s="174"/>
       <c r="D70" s="54" t="s">
         <v>3</v>
       </c>
@@ -11621,10 +11649,10 @@
       <c r="O70" s="1"/>
     </row>
     <row r="71" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B71" s="157">
+      <c r="B71" s="172">
         <v>1E-3</v>
       </c>
-      <c r="C71" s="157">
+      <c r="C71" s="172">
         <v>1E-3</v>
       </c>
       <c r="D71" s="53" t="s">
@@ -11656,8 +11684,8 @@
       <c r="O71" s="1"/>
     </row>
     <row r="72" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B72" s="158"/>
-      <c r="C72" s="158"/>
+      <c r="B72" s="173"/>
+      <c r="C72" s="173"/>
       <c r="D72" s="2" t="s">
         <v>2</v>
       </c>
@@ -11684,8 +11712,8 @@
       <c r="O72" s="1"/>
     </row>
     <row r="73" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="159"/>
-      <c r="C73" s="159"/>
+      <c r="B73" s="174"/>
+      <c r="C73" s="174"/>
       <c r="D73" s="54" t="s">
         <v>3</v>
       </c>
@@ -11713,10 +11741,10 @@
       <c r="S73" s="1"/>
     </row>
     <row r="74" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B74" s="157">
+      <c r="B74" s="172">
         <v>1E-3</v>
       </c>
-      <c r="C74" s="157">
+      <c r="C74" s="172">
         <v>0.01</v>
       </c>
       <c r="D74" s="53" t="s">
@@ -11745,8 +11773,8 @@
       <c r="O74" s="1"/>
     </row>
     <row r="75" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B75" s="158"/>
-      <c r="C75" s="158"/>
+      <c r="B75" s="173"/>
+      <c r="C75" s="173"/>
       <c r="D75" s="2" t="s">
         <v>2</v>
       </c>
@@ -11769,8 +11797,8 @@
       <c r="N75"/>
     </row>
     <row r="76" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="159"/>
-      <c r="C76" s="159"/>
+      <c r="B76" s="174"/>
+      <c r="C76" s="174"/>
       <c r="D76" s="54" t="s">
         <v>3</v>
       </c>
@@ -11793,10 +11821,10 @@
       <c r="N76"/>
     </row>
     <row r="77" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B77" s="157">
+      <c r="B77" s="172">
         <v>1E-3</v>
       </c>
-      <c r="C77" s="157">
+      <c r="C77" s="172">
         <v>0.1</v>
       </c>
       <c r="D77" s="53" t="s">
@@ -11821,8 +11849,8 @@
       <c r="N77"/>
     </row>
     <row r="78" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B78" s="158"/>
-      <c r="C78" s="158"/>
+      <c r="B78" s="173"/>
+      <c r="C78" s="173"/>
       <c r="D78" s="2" t="s">
         <v>2</v>
       </c>
@@ -11845,8 +11873,8 @@
       <c r="N78"/>
     </row>
     <row r="79" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="159"/>
-      <c r="C79" s="159"/>
+      <c r="B79" s="174"/>
+      <c r="C79" s="174"/>
       <c r="D79" s="54" t="s">
         <v>3</v>
       </c>
@@ -11869,10 +11897,10 @@
       <c r="N79"/>
     </row>
     <row r="80" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B80" s="157">
+      <c r="B80" s="172">
         <v>0.01</v>
       </c>
-      <c r="C80" s="157">
+      <c r="C80" s="172">
         <v>0</v>
       </c>
       <c r="D80" s="53" t="s">
@@ -11897,8 +11925,8 @@
       <c r="N80"/>
     </row>
     <row r="81" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B81" s="158"/>
-      <c r="C81" s="158"/>
+      <c r="B81" s="173"/>
+      <c r="C81" s="173"/>
       <c r="D81" s="2" t="s">
         <v>2</v>
       </c>
@@ -11921,8 +11949,8 @@
       <c r="N81"/>
     </row>
     <row r="82" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="159"/>
-      <c r="C82" s="159"/>
+      <c r="B82" s="174"/>
+      <c r="C82" s="174"/>
       <c r="D82" s="54" t="s">
         <v>3</v>
       </c>
@@ -11945,10 +11973,10 @@
       <c r="N82"/>
     </row>
     <row r="83" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B83" s="157">
+      <c r="B83" s="172">
         <v>0.01</v>
       </c>
-      <c r="C83" s="157">
+      <c r="C83" s="172">
         <v>1E-3</v>
       </c>
       <c r="D83" s="53" t="s">
@@ -11973,8 +12001,8 @@
       <c r="N83"/>
     </row>
     <row r="84" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B84" s="158"/>
-      <c r="C84" s="158"/>
+      <c r="B84" s="173"/>
+      <c r="C84" s="173"/>
       <c r="D84" s="2" t="s">
         <v>2</v>
       </c>
@@ -11997,8 +12025,8 @@
       <c r="N84"/>
     </row>
     <row r="85" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="159"/>
-      <c r="C85" s="159"/>
+      <c r="B85" s="174"/>
+      <c r="C85" s="174"/>
       <c r="D85" s="54" t="s">
         <v>3</v>
       </c>
@@ -12021,10 +12049,10 @@
       <c r="N85"/>
     </row>
     <row r="86" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B86" s="157">
+      <c r="B86" s="172">
         <v>0.01</v>
       </c>
-      <c r="C86" s="157">
+      <c r="C86" s="172">
         <v>0.01</v>
       </c>
       <c r="D86" s="53" t="s">
@@ -12049,8 +12077,8 @@
       <c r="N86"/>
     </row>
     <row r="87" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B87" s="158"/>
-      <c r="C87" s="158"/>
+      <c r="B87" s="173"/>
+      <c r="C87" s="173"/>
       <c r="D87" s="2" t="s">
         <v>2</v>
       </c>
@@ -12073,8 +12101,8 @@
       <c r="N87"/>
     </row>
     <row r="88" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="159"/>
-      <c r="C88" s="159"/>
+      <c r="B88" s="174"/>
+      <c r="C88" s="174"/>
       <c r="D88" s="54" t="s">
         <v>3</v>
       </c>
@@ -12097,10 +12125,10 @@
       <c r="N88"/>
     </row>
     <row r="89" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B89" s="157">
+      <c r="B89" s="172">
         <v>0.01</v>
       </c>
-      <c r="C89" s="157">
+      <c r="C89" s="172">
         <v>0.1</v>
       </c>
       <c r="D89" s="53" t="s">
@@ -12125,8 +12153,8 @@
       <c r="N89"/>
     </row>
     <row r="90" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B90" s="158"/>
-      <c r="C90" s="158"/>
+      <c r="B90" s="173"/>
+      <c r="C90" s="173"/>
       <c r="D90" s="2" t="s">
         <v>2</v>
       </c>
@@ -12149,8 +12177,8 @@
       <c r="N90"/>
     </row>
     <row r="91" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="159"/>
-      <c r="C91" s="159"/>
+      <c r="B91" s="174"/>
+      <c r="C91" s="174"/>
       <c r="D91" s="54" t="s">
         <v>3</v>
       </c>
@@ -12173,10 +12201,10 @@
       <c r="N91"/>
     </row>
     <row r="92" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B92" s="157">
+      <c r="B92" s="172">
         <v>0.1</v>
       </c>
-      <c r="C92" s="157">
+      <c r="C92" s="172">
         <v>0</v>
       </c>
       <c r="D92" s="53" t="s">
@@ -12201,8 +12229,8 @@
       <c r="N92"/>
     </row>
     <row r="93" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B93" s="158"/>
-      <c r="C93" s="158"/>
+      <c r="B93" s="173"/>
+      <c r="C93" s="173"/>
       <c r="D93" s="2" t="s">
         <v>2</v>
       </c>
@@ -12224,8 +12252,8 @@
       </c>
     </row>
     <row r="94" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="159"/>
-      <c r="C94" s="159"/>
+      <c r="B94" s="174"/>
+      <c r="C94" s="174"/>
       <c r="D94" s="54" t="s">
         <v>3</v>
       </c>
@@ -12247,10 +12275,10 @@
       </c>
     </row>
     <row r="95" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B95" s="157">
+      <c r="B95" s="172">
         <v>0.1</v>
       </c>
-      <c r="C95" s="157">
+      <c r="C95" s="172">
         <v>1E-3</v>
       </c>
       <c r="D95" s="53" t="s">
@@ -12274,8 +12302,8 @@
       </c>
     </row>
     <row r="96" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B96" s="158"/>
-      <c r="C96" s="158"/>
+      <c r="B96" s="173"/>
+      <c r="C96" s="173"/>
       <c r="D96" s="2" t="s">
         <v>2</v>
       </c>
@@ -12297,8 +12325,8 @@
       </c>
     </row>
     <row r="97" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="159"/>
-      <c r="C97" s="159"/>
+      <c r="B97" s="174"/>
+      <c r="C97" s="174"/>
       <c r="D97" s="54" t="s">
         <v>3</v>
       </c>
@@ -12320,10 +12348,10 @@
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B98" s="157">
+      <c r="B98" s="172">
         <v>0.1</v>
       </c>
-      <c r="C98" s="157">
+      <c r="C98" s="172">
         <v>0.01</v>
       </c>
       <c r="D98" s="53" t="s">
@@ -12347,8 +12375,8 @@
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B99" s="158"/>
-      <c r="C99" s="158"/>
+      <c r="B99" s="173"/>
+      <c r="C99" s="173"/>
       <c r="D99" s="2" t="s">
         <v>2</v>
       </c>
@@ -12370,8 +12398,8 @@
       </c>
     </row>
     <row r="100" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="159"/>
-      <c r="C100" s="159"/>
+      <c r="B100" s="174"/>
+      <c r="C100" s="174"/>
       <c r="D100" s="54" t="s">
         <v>3</v>
       </c>
@@ -12393,10 +12421,10 @@
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B101" s="157">
+      <c r="B101" s="172">
         <v>0.1</v>
       </c>
-      <c r="C101" s="157">
+      <c r="C101" s="172">
         <v>0.1</v>
       </c>
       <c r="D101" s="53" t="s">
@@ -12420,8 +12448,8 @@
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B102" s="158"/>
-      <c r="C102" s="158"/>
+      <c r="B102" s="173"/>
+      <c r="C102" s="173"/>
       <c r="D102" s="2" t="s">
         <v>2</v>
       </c>
@@ -12443,8 +12471,8 @@
       </c>
     </row>
     <row r="103" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="159"/>
-      <c r="C103" s="159"/>
+      <c r="B103" s="174"/>
+      <c r="C103" s="174"/>
       <c r="D103" s="54" t="s">
         <v>3</v>
       </c>
@@ -12467,37 +12495,24 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="AF26:AM26"/>
-    <mergeCell ref="X27:AA27"/>
-    <mergeCell ref="AB27:AE27"/>
-    <mergeCell ref="AF27:AI27"/>
-    <mergeCell ref="AJ27:AM27"/>
-    <mergeCell ref="X26:AE26"/>
-    <mergeCell ref="J26:N26"/>
-    <mergeCell ref="O26:S26"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="B28:B39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="B4:B15"/>
-    <mergeCell ref="O2:S2"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:N2"/>
-    <mergeCell ref="C89:C91"/>
-    <mergeCell ref="C92:C94"/>
-    <mergeCell ref="C95:C97"/>
-    <mergeCell ref="C98:C100"/>
-    <mergeCell ref="C71:C73"/>
-    <mergeCell ref="C74:C76"/>
-    <mergeCell ref="C77:C79"/>
-    <mergeCell ref="C80:C82"/>
-    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="V29:V33"/>
+    <mergeCell ref="V34:V38"/>
+    <mergeCell ref="V39:V43"/>
+    <mergeCell ref="V44:W44"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="C68:C70"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="B40:B51"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="C56:C58"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="C62:C64"/>
     <mergeCell ref="C101:C103"/>
     <mergeCell ref="B62:B64"/>
     <mergeCell ref="B65:B67"/>
@@ -12514,24 +12529,37 @@
     <mergeCell ref="B98:B100"/>
     <mergeCell ref="B101:B103"/>
     <mergeCell ref="C86:C88"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="B40:B51"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="C62:C64"/>
-    <mergeCell ref="V29:V33"/>
-    <mergeCell ref="V34:V38"/>
-    <mergeCell ref="V39:V43"/>
-    <mergeCell ref="V44:W44"/>
-    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="C89:C91"/>
+    <mergeCell ref="C92:C94"/>
+    <mergeCell ref="C95:C97"/>
+    <mergeCell ref="C98:C100"/>
+    <mergeCell ref="C71:C73"/>
+    <mergeCell ref="C74:C76"/>
+    <mergeCell ref="C77:C79"/>
+    <mergeCell ref="C80:C82"/>
+    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="B4:B15"/>
+    <mergeCell ref="O2:S2"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="J26:N26"/>
+    <mergeCell ref="O26:S26"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="B28:B39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="AF26:AM26"/>
+    <mergeCell ref="X27:AA27"/>
+    <mergeCell ref="AB27:AE27"/>
+    <mergeCell ref="AF27:AI27"/>
+    <mergeCell ref="AJ27:AM27"/>
+    <mergeCell ref="X26:AE26"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12541,10 +12569,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AFB687B-AE8A-9E4C-93B1-A2032A687EEF}">
-  <dimension ref="C4:Y55"/>
+  <dimension ref="C4:Y74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58:M64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12565,28 +12593,28 @@
     </row>
     <row r="6" spans="3:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C6" s="13"/>
-      <c r="F6" s="171" t="s">
+      <c r="F6" s="156" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="172"/>
-      <c r="H6" s="172"/>
-      <c r="I6" s="172"/>
-      <c r="J6" s="173"/>
-      <c r="K6" s="171" t="s">
+      <c r="G6" s="157"/>
+      <c r="H6" s="157"/>
+      <c r="I6" s="157"/>
+      <c r="J6" s="158"/>
+      <c r="K6" s="156" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="172"/>
-      <c r="M6" s="172"/>
-      <c r="N6" s="172"/>
-      <c r="O6" s="173"/>
-      <c r="P6" s="171" t="s">
+      <c r="L6" s="157"/>
+      <c r="M6" s="157"/>
+      <c r="N6" s="157"/>
+      <c r="O6" s="158"/>
+      <c r="P6" s="156" t="s">
         <v>12</v>
       </c>
-      <c r="Q6" s="172"/>
-      <c r="R6" s="172"/>
-      <c r="S6" s="172"/>
-      <c r="T6" s="173"/>
-      <c r="U6" s="174" t="s">
+      <c r="Q6" s="157"/>
+      <c r="R6" s="157"/>
+      <c r="S6" s="157"/>
+      <c r="T6" s="158"/>
+      <c r="U6" s="169" t="s">
         <v>9</v>
       </c>
       <c r="X6" s="121" t="s">
@@ -12643,7 +12671,7 @@
       <c r="T7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="U7" s="174"/>
+      <c r="U7" s="169"/>
       <c r="X7" s="122" t="s">
         <v>212</v>
       </c>
@@ -12652,10 +12680,10 @@
       </c>
     </row>
     <row r="8" spans="3:25" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="170" t="s">
+      <c r="C8" s="168" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="160" t="s">
+      <c r="D8" s="159" t="s">
         <v>210</v>
       </c>
       <c r="E8" s="53" t="s">
@@ -12721,8 +12749,8 @@
       </c>
     </row>
     <row r="9" spans="3:25" x14ac:dyDescent="0.2">
-      <c r="C9" s="170"/>
-      <c r="D9" s="161"/>
+      <c r="C9" s="168"/>
+      <c r="D9" s="160"/>
       <c r="E9" s="2" t="s">
         <v>2</v>
       </c>
@@ -12786,8 +12814,8 @@
       </c>
     </row>
     <row r="10" spans="3:25" x14ac:dyDescent="0.2">
-      <c r="C10" s="170"/>
-      <c r="D10" s="161"/>
+      <c r="C10" s="168"/>
+      <c r="D10" s="160"/>
       <c r="E10" s="2" t="s">
         <v>3</v>
       </c>
@@ -12851,8 +12879,8 @@
       </c>
     </row>
     <row r="11" spans="3:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="170"/>
-      <c r="D11" s="162"/>
+      <c r="C11" s="168"/>
+      <c r="D11" s="161"/>
       <c r="E11" s="54" t="s">
         <v>211</v>
       </c>
@@ -12916,8 +12944,8 @@
       </c>
     </row>
     <row r="12" spans="3:25" x14ac:dyDescent="0.2">
-      <c r="C12" s="170"/>
-      <c r="D12" s="160" t="s">
+      <c r="C12" s="168"/>
+      <c r="D12" s="159" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="53" t="s">
@@ -12983,8 +13011,8 @@
       </c>
     </row>
     <row r="13" spans="3:25" x14ac:dyDescent="0.2">
-      <c r="C13" s="170"/>
-      <c r="D13" s="161"/>
+      <c r="C13" s="168"/>
+      <c r="D13" s="160"/>
       <c r="E13" s="2" t="s">
         <v>2</v>
       </c>
@@ -13048,7 +13076,7 @@
       </c>
     </row>
     <row r="14" spans="3:25" x14ac:dyDescent="0.2">
-      <c r="D14" s="161"/>
+      <c r="D14" s="160"/>
       <c r="E14" s="2" t="s">
         <v>3</v>
       </c>
@@ -13112,7 +13140,7 @@
       </c>
     </row>
     <row r="15" spans="3:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="162"/>
+      <c r="D15" s="161"/>
       <c r="E15" s="50" t="s">
         <v>211</v>
       </c>
@@ -13187,24 +13215,24 @@
     <row r="19" spans="4:22" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D19" s="129"/>
       <c r="E19" s="129"/>
-      <c r="F19" s="160" t="s">
+      <c r="F19" s="159" t="s">
         <v>218</v>
       </c>
-      <c r="G19" s="185"/>
-      <c r="H19" s="185"/>
-      <c r="I19" s="186"/>
-      <c r="J19" s="185" t="s">
+      <c r="G19" s="184"/>
+      <c r="H19" s="184"/>
+      <c r="I19" s="185"/>
+      <c r="J19" s="184" t="s">
         <v>217</v>
       </c>
-      <c r="K19" s="185"/>
-      <c r="L19" s="185"/>
-      <c r="M19" s="187"/>
-      <c r="N19" s="160" t="s">
+      <c r="K19" s="184"/>
+      <c r="L19" s="184"/>
+      <c r="M19" s="186"/>
+      <c r="N19" s="159" t="s">
         <v>236</v>
       </c>
-      <c r="O19" s="185"/>
-      <c r="P19" s="185"/>
-      <c r="Q19" s="186"/>
+      <c r="O19" s="184"/>
+      <c r="P19" s="184"/>
+      <c r="Q19" s="185"/>
       <c r="R19" s="14"/>
       <c r="S19" s="14"/>
       <c r="T19" s="14"/>
@@ -13259,7 +13287,7 @@
       <c r="U20" s="14"/>
     </row>
     <row r="21" spans="4:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D21" s="152">
+      <c r="D21" s="179">
         <v>7</v>
       </c>
       <c r="E21" s="130" t="s">
@@ -13307,7 +13335,7 @@
       <c r="U21" s="14"/>
     </row>
     <row r="22" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D22" s="153"/>
+      <c r="D22" s="180"/>
       <c r="E22" s="6" t="s">
         <v>6</v>
       </c>
@@ -13354,7 +13382,7 @@
       <c r="V22" s="14"/>
     </row>
     <row r="23" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D23" s="153"/>
+      <c r="D23" s="180"/>
       <c r="E23" s="6" t="s">
         <v>7</v>
       </c>
@@ -13401,7 +13429,7 @@
       <c r="V23" s="14"/>
     </row>
     <row r="24" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D24" s="153"/>
+      <c r="D24" s="180"/>
       <c r="E24" s="6" t="s">
         <v>8</v>
       </c>
@@ -13448,7 +13476,7 @@
       <c r="V24" s="14"/>
     </row>
     <row r="25" spans="4:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D25" s="154"/>
+      <c r="D25" s="181"/>
       <c r="E25" s="127" t="s">
         <v>9</v>
       </c>
@@ -13507,7 +13535,7 @@
       <c r="V25" s="14"/>
     </row>
     <row r="26" spans="4:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D26" s="152">
+      <c r="D26" s="179">
         <v>14</v>
       </c>
       <c r="E26" s="130" t="s">
@@ -13550,21 +13578,13 @@
         <v>-1</v>
       </c>
       <c r="R26" s="14"/>
-      <c r="S26" s="14">
-        <v>2.9577961416509502</v>
-      </c>
-      <c r="T26" s="14">
-        <v>3.6086103265852998</v>
-      </c>
-      <c r="U26" s="14">
-        <v>2.29420340487271</v>
-      </c>
-      <c r="V26" s="14">
-        <v>5.0369887593202503</v>
-      </c>
+      <c r="S26" s="14"/>
+      <c r="T26" s="14"/>
+      <c r="U26" s="14"/>
+      <c r="V26" s="14"/>
     </row>
     <row r="27" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D27" s="153"/>
+      <c r="D27" s="180"/>
       <c r="E27" s="6" t="s">
         <v>6</v>
       </c>
@@ -13605,21 +13625,13 @@
         <v>24</v>
       </c>
       <c r="R27" s="14"/>
-      <c r="S27" s="14">
-        <v>4.3657949130589202</v>
-      </c>
-      <c r="T27" s="14">
-        <v>5.4770218720708899</v>
-      </c>
-      <c r="U27" s="14">
-        <v>2.8968259156070699</v>
-      </c>
-      <c r="V27" s="14">
-        <v>9.1738224310701302</v>
-      </c>
+      <c r="S27" s="14"/>
+      <c r="T27" s="14"/>
+      <c r="U27" s="14"/>
+      <c r="V27" s="14"/>
     </row>
     <row r="28" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D28" s="153"/>
+      <c r="D28" s="180"/>
       <c r="E28" s="6" t="s">
         <v>7</v>
       </c>
@@ -13660,21 +13672,13 @@
         <v>-12</v>
       </c>
       <c r="R28" s="14"/>
-      <c r="S28" s="14">
-        <v>0.71245087138951502</v>
-      </c>
-      <c r="T28" s="14">
-        <v>0.62210520724011198</v>
-      </c>
-      <c r="U28" s="14">
-        <v>0.86830984627044105</v>
-      </c>
-      <c r="V28" s="14">
-        <v>0.81204631699589402</v>
-      </c>
+      <c r="S28" s="14"/>
+      <c r="T28" s="14"/>
+      <c r="U28" s="14"/>
+      <c r="V28" s="14"/>
     </row>
     <row r="29" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D29" s="153"/>
+      <c r="D29" s="180"/>
       <c r="E29" s="6" t="s">
         <v>8</v>
       </c>
@@ -13715,21 +13719,13 @@
         <v>15</v>
       </c>
       <c r="R29" s="14"/>
-      <c r="S29" s="14">
-        <v>-57</v>
-      </c>
-      <c r="T29" s="14">
-        <v>-128</v>
-      </c>
-      <c r="U29" s="14">
-        <v>-6</v>
-      </c>
-      <c r="V29" s="14">
-        <v>23</v>
-      </c>
+      <c r="S29" s="14"/>
+      <c r="T29" s="14"/>
+      <c r="U29" s="14"/>
+      <c r="V29" s="14"/>
     </row>
     <row r="30" spans="4:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="154"/>
+      <c r="D30" s="181"/>
       <c r="E30" s="128" t="s">
         <v>9</v>
       </c>
@@ -13784,7 +13780,7 @@
       <c r="R30" s="14"/>
     </row>
     <row r="31" spans="4:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D31" s="152">
+      <c r="D31" s="179">
         <v>21</v>
       </c>
       <c r="E31" s="130" t="s">
@@ -13829,7 +13825,7 @@
       <c r="R31" s="14"/>
     </row>
     <row r="32" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D32" s="153"/>
+      <c r="D32" s="180"/>
       <c r="E32" s="6" t="s">
         <v>6</v>
       </c>
@@ -13872,7 +13868,7 @@
       <c r="R32" s="14"/>
     </row>
     <row r="33" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D33" s="153"/>
+      <c r="D33" s="180"/>
       <c r="E33" s="6" t="s">
         <v>7</v>
       </c>
@@ -13915,7 +13911,7 @@
       <c r="R33" s="14"/>
     </row>
     <row r="34" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D34" s="153"/>
+      <c r="D34" s="180"/>
       <c r="E34" s="6" t="s">
         <v>8</v>
       </c>
@@ -13958,7 +13954,7 @@
       <c r="R34" s="14"/>
     </row>
     <row r="35" spans="4:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D35" s="154"/>
+      <c r="D35" s="181"/>
       <c r="E35" s="6" t="s">
         <v>9</v>
       </c>
@@ -14011,24 +14007,16 @@
         <v>53.5</v>
       </c>
       <c r="R35" s="14"/>
-      <c r="S35" s="14">
-        <v>2.9512770024242001</v>
-      </c>
-      <c r="T35" s="14">
-        <v>2.6259942309225002</v>
-      </c>
-      <c r="U35" s="14">
-        <v>1.50589329905638</v>
-      </c>
-      <c r="V35" s="14">
-        <v>3.5480996358027301</v>
-      </c>
+      <c r="S35" s="14"/>
+      <c r="T35" s="14"/>
+      <c r="U35" s="14"/>
+      <c r="V35" s="14"/>
     </row>
     <row r="36" spans="4:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D36" s="181" t="s">
+      <c r="D36" s="187" t="s">
         <v>9</v>
       </c>
-      <c r="E36" s="182"/>
+      <c r="E36" s="188"/>
       <c r="F36" s="134">
         <f t="shared" ref="F36:M36" si="5">AVERAGE(F25,F30,F35)</f>
         <v>2.6236353004055935</v>
@@ -14078,61 +14066,37 @@
         <v>26.5</v>
       </c>
       <c r="R36" s="14"/>
-      <c r="S36" s="14">
-        <v>4.3127364592540296</v>
-      </c>
-      <c r="T36" s="14">
-        <v>4.0622906378416799</v>
-      </c>
-      <c r="U36" s="14">
-        <v>2.0698032495027499</v>
-      </c>
-      <c r="V36" s="14">
-        <v>5.8785085877251104</v>
-      </c>
+      <c r="S36" s="14"/>
+      <c r="T36" s="14"/>
+      <c r="U36" s="14"/>
+      <c r="V36" s="14"/>
     </row>
     <row r="37" spans="4:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="P37" s="14"/>
       <c r="Q37" s="14"/>
       <c r="R37" s="14"/>
-      <c r="S37" s="14">
-        <v>0.86352584150675904</v>
-      </c>
-      <c r="T37" s="14">
-        <v>0.91021773196631095</v>
-      </c>
-      <c r="U37" s="14">
-        <v>0.96135869199740298</v>
-      </c>
-      <c r="V37" s="14">
-        <v>0.973848575563387</v>
-      </c>
+      <c r="S37" s="14"/>
+      <c r="T37" s="14"/>
+      <c r="U37" s="14"/>
+      <c r="V37" s="14"/>
     </row>
     <row r="38" spans="4:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F38" s="180" t="s">
+      <c r="F38" s="155" t="s">
         <v>210</v>
       </c>
-      <c r="G38" s="180"/>
-      <c r="H38" s="180"/>
-      <c r="I38" s="183"/>
-      <c r="J38" s="184" t="s">
+      <c r="G38" s="155"/>
+      <c r="H38" s="155"/>
+      <c r="I38" s="189"/>
+      <c r="J38" s="190" t="s">
         <v>5</v>
       </c>
-      <c r="K38" s="180"/>
-      <c r="L38" s="180"/>
-      <c r="M38" s="180"/>
-      <c r="S38" s="14">
-        <v>-8</v>
-      </c>
-      <c r="T38" s="14">
-        <v>17</v>
-      </c>
-      <c r="U38" s="14">
-        <v>-17</v>
-      </c>
-      <c r="V38" s="14">
-        <v>10</v>
-      </c>
+      <c r="K38" s="155"/>
+      <c r="L38" s="155"/>
+      <c r="M38" s="155"/>
+      <c r="S38" s="14"/>
+      <c r="T38" s="14"/>
+      <c r="U38" s="14"/>
+      <c r="V38" s="14"/>
     </row>
     <row r="39" spans="4:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D39" s="97" t="s">
@@ -14167,7 +14131,7 @@
       </c>
     </row>
     <row r="40" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D40" s="152">
+      <c r="D40" s="179">
         <v>7</v>
       </c>
       <c r="E40" s="118" t="s">
@@ -14197,9 +14161,16 @@
       <c r="M40" s="108">
         <v>2</v>
       </c>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
+      <c r="S40" s="14"/>
+      <c r="T40" s="14"/>
     </row>
     <row r="41" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D41" s="153"/>
+      <c r="D41" s="180"/>
       <c r="E41" s="119" t="s">
         <v>6</v>
       </c>
@@ -14227,9 +14198,16 @@
       <c r="M41" s="108">
         <v>2</v>
       </c>
+      <c r="N41" s="14"/>
+      <c r="O41" s="14"/>
+      <c r="P41" s="14"/>
+      <c r="Q41" s="14"/>
+      <c r="R41" s="14"/>
+      <c r="S41" s="14"/>
+      <c r="T41" s="14"/>
     </row>
     <row r="42" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D42" s="153"/>
+      <c r="D42" s="180"/>
       <c r="E42" s="119" t="s">
         <v>7</v>
       </c>
@@ -14257,9 +14235,16 @@
       <c r="M42" s="108">
         <v>-22</v>
       </c>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14"/>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
+      <c r="T42" s="14"/>
     </row>
     <row r="43" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D43" s="153"/>
+      <c r="D43" s="180"/>
       <c r="E43" s="119" t="s">
         <v>8</v>
       </c>
@@ -14287,9 +14272,16 @@
       <c r="M43" s="103">
         <v>8</v>
       </c>
+      <c r="N43" s="14"/>
+      <c r="O43" s="14"/>
+      <c r="P43" s="14"/>
+      <c r="Q43" s="14"/>
+      <c r="R43" s="14"/>
+      <c r="S43" s="14"/>
+      <c r="T43" s="14"/>
     </row>
     <row r="44" spans="4:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D44" s="154"/>
+      <c r="D44" s="181"/>
       <c r="E44" s="120" t="s">
         <v>9</v>
       </c>
@@ -14325,9 +14317,16 @@
         <f t="array" ref="M44">AVERAGE(ABS(M40:M43))</f>
         <v>8.5</v>
       </c>
+      <c r="N44" s="14"/>
+      <c r="O44" s="14"/>
+      <c r="P44" s="14"/>
+      <c r="Q44" s="14"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="14"/>
+      <c r="T44" s="14"/>
     </row>
     <row r="45" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D45" s="152">
+      <c r="D45" s="179">
         <v>14</v>
       </c>
       <c r="E45" s="118" t="s">
@@ -14357,9 +14356,18 @@
       <c r="M45" s="115">
         <v>6</v>
       </c>
+      <c r="N45" s="14"/>
+      <c r="O45" s="14"/>
+      <c r="P45" s="14"/>
+      <c r="Q45" s="14"/>
+      <c r="R45" s="14"/>
+      <c r="S45" s="14"/>
+      <c r="T45" s="14"/>
+      <c r="U45" s="14"/>
+      <c r="V45" s="14"/>
     </row>
     <row r="46" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D46" s="153"/>
+      <c r="D46" s="180"/>
       <c r="E46" s="119" t="s">
         <v>6</v>
       </c>
@@ -14387,9 +14395,18 @@
       <c r="M46" s="108">
         <v>10</v>
       </c>
+      <c r="N46" s="14"/>
+      <c r="O46" s="14"/>
+      <c r="P46" s="14"/>
+      <c r="Q46" s="14"/>
+      <c r="R46" s="14"/>
+      <c r="S46" s="14"/>
+      <c r="T46" s="14"/>
+      <c r="U46" s="14"/>
+      <c r="V46" s="14"/>
     </row>
     <row r="47" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D47" s="153"/>
+      <c r="D47" s="180"/>
       <c r="E47" s="119" t="s">
         <v>7</v>
       </c>
@@ -14417,9 +14434,18 @@
       <c r="M47" s="108">
         <v>4</v>
       </c>
+      <c r="N47" s="14"/>
+      <c r="O47" s="14"/>
+      <c r="P47" s="14"/>
+      <c r="Q47" s="14"/>
+      <c r="R47" s="14"/>
+      <c r="S47" s="14"/>
+      <c r="T47" s="14"/>
+      <c r="U47" s="14"/>
+      <c r="V47" s="14"/>
     </row>
     <row r="48" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D48" s="153"/>
+      <c r="D48" s="180"/>
       <c r="E48" s="119" t="s">
         <v>8</v>
       </c>
@@ -14447,9 +14473,18 @@
       <c r="M48" s="103">
         <v>12</v>
       </c>
-    </row>
-    <row r="49" spans="4:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D49" s="154"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="14"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="14"/>
+      <c r="R48" s="14"/>
+      <c r="S48" s="14"/>
+      <c r="T48" s="14"/>
+      <c r="U48" s="14"/>
+      <c r="V48" s="14"/>
+    </row>
+    <row r="49" spans="4:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D49" s="181"/>
       <c r="E49" s="120" t="s">
         <v>9</v>
       </c>
@@ -14485,9 +14520,16 @@
         <f t="array" ref="M49">AVERAGE(ABS(M45:M48))</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="50" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D50" s="152">
+      <c r="N49" s="14"/>
+      <c r="O49" s="14"/>
+      <c r="P49" s="14"/>
+      <c r="Q49" s="14"/>
+      <c r="R49" s="14"/>
+      <c r="S49" s="14"/>
+      <c r="T49" s="14"/>
+    </row>
+    <row r="50" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D50" s="179">
         <v>21</v>
       </c>
       <c r="E50" s="118" t="s">
@@ -14517,9 +14559,16 @@
       <c r="M50" s="115">
         <v>14</v>
       </c>
-    </row>
-    <row r="51" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D51" s="153"/>
+      <c r="N50" s="14"/>
+      <c r="O50" s="14"/>
+      <c r="P50" s="14"/>
+      <c r="Q50" s="14"/>
+      <c r="R50" s="14"/>
+      <c r="S50" s="14"/>
+      <c r="T50" s="14"/>
+    </row>
+    <row r="51" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D51" s="180"/>
       <c r="E51" s="119" t="s">
         <v>6</v>
       </c>
@@ -14547,9 +14596,16 @@
       <c r="M51" s="108">
         <v>16</v>
       </c>
-    </row>
-    <row r="52" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D52" s="153"/>
+      <c r="N51" s="14"/>
+      <c r="O51" s="14"/>
+      <c r="P51" s="14"/>
+      <c r="Q51" s="14"/>
+      <c r="R51" s="14"/>
+      <c r="S51" s="14"/>
+      <c r="T51" s="14"/>
+    </row>
+    <row r="52" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D52" s="180"/>
       <c r="E52" s="119" t="s">
         <v>7</v>
       </c>
@@ -14577,9 +14633,17 @@
       <c r="M52" s="103">
         <v>-19</v>
       </c>
-    </row>
-    <row r="53" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D53" s="153"/>
+      <c r="O52" s="14"/>
+      <c r="P52" s="14"/>
+      <c r="Q52" s="14"/>
+      <c r="R52" s="14"/>
+      <c r="T52" s="14"/>
+      <c r="U52" s="14"/>
+      <c r="V52" s="14"/>
+      <c r="W52" s="14"/>
+    </row>
+    <row r="53" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D53" s="180"/>
       <c r="E53" s="119" t="s">
         <v>8</v>
       </c>
@@ -14607,9 +14671,17 @@
       <c r="M53" s="108">
         <v>12</v>
       </c>
-    </row>
-    <row r="54" spans="4:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D54" s="154"/>
+      <c r="O53" s="14"/>
+      <c r="P53" s="14"/>
+      <c r="Q53" s="14"/>
+      <c r="R53" s="14"/>
+      <c r="T53" s="14"/>
+      <c r="U53" s="14"/>
+      <c r="V53" s="14"/>
+      <c r="W53" s="14"/>
+    </row>
+    <row r="54" spans="4:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D54" s="181"/>
       <c r="E54" s="120" t="s">
         <v>9</v>
       </c>
@@ -14645,12 +14717,21 @@
         <f t="array" ref="M54">AVERAGE(ABS(M50:M53))</f>
         <v>15.25</v>
       </c>
-    </row>
-    <row r="55" spans="4:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D55" s="181" t="s">
+      <c r="O54" s="191"/>
+      <c r="P54" s="191"/>
+      <c r="Q54" s="191"/>
+      <c r="R54" s="191"/>
+      <c r="S54" s="129"/>
+      <c r="T54" s="191"/>
+      <c r="U54" s="14"/>
+      <c r="V54" s="14"/>
+      <c r="W54" s="14"/>
+    </row>
+    <row r="55" spans="4:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D55" s="187" t="s">
         <v>9</v>
       </c>
-      <c r="E55" s="182"/>
+      <c r="E55" s="188"/>
       <c r="F55" s="149">
         <f t="shared" ref="F55:M55" si="7">AVERAGE(F44,F49,F54)</f>
         <v>2.1519019847241818</v>
@@ -14683,9 +14764,354 @@
         <f t="shared" si="7"/>
         <v>10.583333333333334</v>
       </c>
+      <c r="O55" s="191"/>
+      <c r="P55" s="191"/>
+      <c r="Q55" s="191"/>
+      <c r="R55" s="191"/>
+      <c r="S55" s="129"/>
+      <c r="T55" s="191"/>
+      <c r="U55" s="14"/>
+      <c r="V55" s="14"/>
+      <c r="W55" s="14"/>
+    </row>
+    <row r="56" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="O56" s="131"/>
+      <c r="P56" s="131"/>
+      <c r="Q56" s="131"/>
+      <c r="R56" s="195"/>
+      <c r="S56" s="129"/>
+      <c r="T56" s="129"/>
+    </row>
+    <row r="57" spans="4:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N57" s="129"/>
+      <c r="O57" s="129"/>
+      <c r="P57" s="129"/>
+      <c r="Q57" s="129"/>
+      <c r="R57" s="129"/>
+      <c r="S57" s="129"/>
+    </row>
+    <row r="58" spans="4:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F58" s="155" t="s">
+        <v>237</v>
+      </c>
+      <c r="G58" s="155"/>
+      <c r="H58" s="155"/>
+      <c r="I58" s="155"/>
+      <c r="J58" s="190" t="s">
+        <v>238</v>
+      </c>
+      <c r="K58" s="155"/>
+      <c r="L58" s="155"/>
+      <c r="M58" s="155"/>
+    </row>
+    <row r="59" spans="4:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D59" s="97" t="s">
+        <v>215</v>
+      </c>
+      <c r="E59" s="98" t="s">
+        <v>216</v>
+      </c>
+      <c r="F59" s="97" t="s">
+        <v>1</v>
+      </c>
+      <c r="G59" s="98" t="s">
+        <v>2</v>
+      </c>
+      <c r="H59" s="98" t="s">
+        <v>3</v>
+      </c>
+      <c r="I59" s="100" t="s">
+        <v>211</v>
+      </c>
+      <c r="J59" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="K59" s="98" t="s">
+        <v>2</v>
+      </c>
+      <c r="L59" s="98" t="s">
+        <v>3</v>
+      </c>
+      <c r="M59" s="100" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="60" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D60" s="179">
+        <v>14</v>
+      </c>
+      <c r="E60" s="152" t="s">
+        <v>0</v>
+      </c>
+      <c r="F60" s="114">
+        <v>1.6694034748597599</v>
+      </c>
+      <c r="G60" s="114">
+        <v>2.8631346027687301</v>
+      </c>
+      <c r="H60" s="133">
+        <v>0.91627292446532504</v>
+      </c>
+      <c r="I60" s="115">
+        <v>6</v>
+      </c>
+      <c r="J60" s="192">
+        <v>1.8716683459222501</v>
+      </c>
+      <c r="K60" s="133">
+        <v>2.8920662596319802</v>
+      </c>
+      <c r="L60" s="114">
+        <v>0.90109769670162998</v>
+      </c>
+      <c r="M60" s="130">
+        <v>-1</v>
+      </c>
+      <c r="R60" s="191"/>
+      <c r="S60" s="191"/>
+      <c r="T60" s="191"/>
+      <c r="U60" s="191"/>
+      <c r="V60" s="129"/>
+      <c r="W60" s="129"/>
+    </row>
+    <row r="61" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D61" s="180"/>
+      <c r="E61" s="153" t="s">
+        <v>6</v>
+      </c>
+      <c r="F61" s="132">
+        <v>1.68814282715754</v>
+      </c>
+      <c r="G61" s="102">
+        <v>2.6370715572724599</v>
+      </c>
+      <c r="H61" s="106">
+        <v>0.92553063381835099</v>
+      </c>
+      <c r="I61" s="103">
+        <v>10</v>
+      </c>
+      <c r="J61" s="107">
+        <v>2.0266915069861202</v>
+      </c>
+      <c r="K61" s="131">
+        <v>3.3041747487395901</v>
+      </c>
+      <c r="L61" s="132">
+        <v>0.93052967471808901</v>
+      </c>
+      <c r="M61" s="6">
+        <v>9</v>
+      </c>
+      <c r="R61" s="191"/>
+      <c r="S61" s="191"/>
+      <c r="T61" s="191"/>
+      <c r="U61" s="191"/>
+      <c r="V61" s="129"/>
+      <c r="W61" s="129"/>
+    </row>
+    <row r="62" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D62" s="180"/>
+      <c r="E62" s="153" t="s">
+        <v>7</v>
+      </c>
+      <c r="F62" s="131">
+        <v>2.3955166648425901</v>
+      </c>
+      <c r="G62" s="106">
+        <v>3.9394499960077098</v>
+      </c>
+      <c r="H62" s="106">
+        <v>0.81399577288686298</v>
+      </c>
+      <c r="I62" s="108">
+        <v>4</v>
+      </c>
+      <c r="J62" s="104">
+        <v>1.40851515885283</v>
+      </c>
+      <c r="K62" s="132">
+        <v>1.82884617928689</v>
+      </c>
+      <c r="L62" s="132">
+        <v>0.93458900397100697</v>
+      </c>
+      <c r="M62" s="193">
+        <v>-26</v>
+      </c>
+      <c r="R62" s="191"/>
+      <c r="S62" s="191"/>
+      <c r="T62" s="191"/>
+      <c r="U62" s="191"/>
+      <c r="V62" s="129"/>
+      <c r="W62" s="129"/>
+    </row>
+    <row r="63" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D63" s="180"/>
+      <c r="E63" s="153" t="s">
+        <v>8</v>
+      </c>
+      <c r="F63" s="132">
+        <v>3.49637808647475</v>
+      </c>
+      <c r="G63" s="102">
+        <v>5.5705857717349998</v>
+      </c>
+      <c r="H63" s="102">
+        <v>0.95114531328013696</v>
+      </c>
+      <c r="I63" s="103">
+        <v>12</v>
+      </c>
+      <c r="J63" s="107">
+        <v>3.9502869519813402</v>
+      </c>
+      <c r="K63" s="131">
+        <v>7.7375523253014098</v>
+      </c>
+      <c r="L63" s="131">
+        <v>0.94440656659134303</v>
+      </c>
+      <c r="M63" s="6">
+        <v>10</v>
+      </c>
+      <c r="R63" s="191"/>
+      <c r="S63" s="191"/>
+      <c r="T63" s="191"/>
+      <c r="U63" s="191"/>
+      <c r="V63" s="129"/>
+      <c r="W63" s="129"/>
+    </row>
+    <row r="64" spans="4:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D64" s="181"/>
+      <c r="E64" s="154" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" s="110">
+        <f>AVERAGE(F60:F63)</f>
+        <v>2.3123602633336597</v>
+      </c>
+      <c r="G64" s="110">
+        <f>AVERAGE(G60:G63)</f>
+        <v>3.7525604819459746</v>
+      </c>
+      <c r="H64" s="109">
+        <f>AVERAGE(H60:H63)</f>
+        <v>0.90173616111266897</v>
+      </c>
+      <c r="I64" s="146" cm="1">
+        <f t="array" ref="I64">AVERAGE(ABS(I60:I63))</f>
+        <v>8</v>
+      </c>
+      <c r="J64" s="112">
+        <f>AVERAGE(J60:J63)</f>
+        <v>2.314290490935635</v>
+      </c>
+      <c r="K64" s="109">
+        <f>AVERAGE(K60:K63)</f>
+        <v>3.9406598782399676</v>
+      </c>
+      <c r="L64" s="110">
+        <f>AVERAGE(L60:L63)</f>
+        <v>0.92765573549551728</v>
+      </c>
+      <c r="M64" s="111" cm="1">
+        <f t="array" ref="M64">AVERAGE(ABS(M60:M63))</f>
+        <v>11.5</v>
+      </c>
+      <c r="R64" s="131"/>
+      <c r="S64" s="131"/>
+      <c r="T64" s="132"/>
+      <c r="U64" s="194"/>
+      <c r="V64" s="129"/>
+      <c r="W64" s="129"/>
+    </row>
+    <row r="65" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="R65" s="129"/>
+      <c r="S65" s="129"/>
+      <c r="T65" s="129"/>
+      <c r="U65" s="129"/>
+      <c r="V65" s="129"/>
+      <c r="W65" s="129"/>
+    </row>
+    <row r="66" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="J66" s="14"/>
+      <c r="K66" s="14"/>
+      <c r="L66" s="14"/>
+      <c r="M66" s="14"/>
+      <c r="R66" s="129"/>
+      <c r="S66" s="129"/>
+      <c r="T66" s="129"/>
+      <c r="U66" s="129"/>
+      <c r="V66" s="129"/>
+      <c r="W66" s="129"/>
+    </row>
+    <row r="67" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="R67" s="129"/>
+      <c r="S67" s="129"/>
+      <c r="T67" s="129"/>
+      <c r="U67" s="129"/>
+      <c r="V67" s="129"/>
+      <c r="W67" s="129"/>
+    </row>
+    <row r="68" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="R68" s="129"/>
+      <c r="S68" s="129"/>
+      <c r="T68" s="129"/>
+      <c r="U68" s="129"/>
+      <c r="V68" s="129"/>
+      <c r="W68" s="129"/>
+    </row>
+    <row r="71" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="N71" s="14"/>
+      <c r="O71" s="14"/>
+      <c r="Q71" s="14"/>
+      <c r="R71" s="14"/>
+      <c r="S71" s="14"/>
+      <c r="T71" s="14"/>
+    </row>
+    <row r="72" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="N72" s="14"/>
+      <c r="O72" s="14"/>
+      <c r="Q72" s="14"/>
+      <c r="R72" s="14"/>
+      <c r="S72" s="14"/>
+      <c r="T72" s="14"/>
+    </row>
+    <row r="73" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="N73" s="14"/>
+      <c r="O73" s="14"/>
+      <c r="Q73" s="14"/>
+      <c r="R73" s="14"/>
+      <c r="S73" s="14"/>
+      <c r="T73" s="14"/>
+    </row>
+    <row r="74" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="L74" s="14"/>
+      <c r="M74" s="14"/>
+      <c r="N74" s="14"/>
+      <c r="O74" s="14"/>
+      <c r="Q74" s="14"/>
+      <c r="R74" s="14"/>
+      <c r="S74" s="14"/>
+      <c r="T74" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="23">
+    <mergeCell ref="D60:D64"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="J58:M58"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="D40:D44"/>
+    <mergeCell ref="D45:D49"/>
+    <mergeCell ref="U6:U7"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="J19:M19"/>
+    <mergeCell ref="D50:D54"/>
     <mergeCell ref="C8:C13"/>
     <mergeCell ref="D8:D11"/>
     <mergeCell ref="D31:D35"/>
@@ -14695,17 +15121,6 @@
     <mergeCell ref="D26:D30"/>
     <mergeCell ref="N19:Q19"/>
     <mergeCell ref="P6:T6"/>
-    <mergeCell ref="U6:U7"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="J19:M19"/>
-    <mergeCell ref="D50:D54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="D40:D44"/>
-    <mergeCell ref="D45:D49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>